<commit_message>
fixed some bugs, updated replacement level, recalculated slopes of regression lines.
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:140008_{60430132-97E6-42F1-B325-ABC7F6561C2F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D9D91CE6-20DE-4295-84A2-2DD965E3D856}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="draftpicks" sheetId="1" r:id="rId1"/>
@@ -230,9 +230,6 @@
     <t>Nomar Mazara</t>
   </si>
   <si>
-    <t>Michael Foltynewicz</t>
-  </si>
-  <si>
     <t>Robbie Ray</t>
   </si>
   <si>
@@ -524,12 +521,6 @@
     <t>Raisel Iglesias</t>
   </si>
   <si>
-    <t>Vladimir Guerrero, Jr.</t>
-  </si>
-  <si>
-    <t>Fernando Tatis, Jr.</t>
-  </si>
-  <si>
     <t>J.T. Realmuto</t>
   </si>
   <si>
@@ -650,9 +641,6 @@
     <t>Johan Camargo</t>
   </si>
   <si>
-    <t>Ronald Acuna</t>
-  </si>
-  <si>
     <t>Brian Anderson</t>
   </si>
   <si>
@@ -705,12 +693,24 @@
   </si>
   <si>
     <t>Willie Calhoun</t>
+  </si>
+  <si>
+    <t>Ronald Acuna Jr.</t>
+  </si>
+  <si>
+    <t>Mike Foltynewicz</t>
+  </si>
+  <si>
+    <t>Vladimir Guerrero Jr.</t>
+  </si>
+  <si>
+    <t>Fernando Tatis Jr.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
@@ -1549,11 +1549,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="H195" sqref="H195"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2229,7 +2229,7 @@
         <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>69</v>
+        <v>225</v>
       </c>
       <c r="C40" s="2">
         <v>5</v>
@@ -2246,7 +2246,7 @@
         <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C41" s="2">
         <v>13</v>
@@ -2263,7 +2263,7 @@
         <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C42" s="2">
         <v>8</v>
@@ -2280,7 +2280,7 @@
         <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" s="2">
         <v>8</v>
@@ -2297,7 +2297,7 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C44" s="2">
         <v>0</v>
@@ -2311,10 +2311,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C45" s="2">
         <v>10</v>
@@ -2328,10 +2328,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C46" s="2">
         <v>5</v>
@@ -2345,10 +2345,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C47" s="2">
         <v>18</v>
@@ -2362,16 +2362,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C48" s="2">
         <v>7</v>
       </c>
       <c r="D48" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="E48" s="1">
         <v>43465</v>
@@ -2379,16 +2379,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C49" s="2">
         <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E49" s="1">
         <v>43465</v>
@@ -2396,10 +2396,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C50" s="2">
         <v>8</v>
@@ -2413,10 +2413,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C51" s="2">
         <v>8</v>
@@ -2430,10 +2430,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C52" s="2">
         <v>13</v>
@@ -2447,10 +2447,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C53" s="2">
         <v>8</v>
@@ -2464,10 +2464,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C54" s="2">
         <v>0</v>
@@ -2481,10 +2481,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C55" s="2">
         <v>0</v>
@@ -2501,7 +2501,7 @@
         <v>24</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C56" s="2">
         <v>20</v>
@@ -2518,13 +2518,13 @@
         <v>24</v>
       </c>
       <c r="B57" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C57" s="2">
         <v>15</v>
       </c>
       <c r="D57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E57" s="1">
         <v>43465</v>
@@ -2535,7 +2535,7 @@
         <v>24</v>
       </c>
       <c r="B58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C58" s="2">
         <v>5</v>
@@ -2552,7 +2552,7 @@
         <v>24</v>
       </c>
       <c r="B59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C59" s="2">
         <v>9</v>
@@ -2569,7 +2569,7 @@
         <v>24</v>
       </c>
       <c r="B60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C60" s="2">
         <v>37</v>
@@ -2586,7 +2586,7 @@
         <v>24</v>
       </c>
       <c r="B61" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C61" s="2">
         <v>23</v>
@@ -2603,7 +2603,7 @@
         <v>24</v>
       </c>
       <c r="B62" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C62" s="2">
         <v>23</v>
@@ -2620,7 +2620,7 @@
         <v>24</v>
       </c>
       <c r="B63" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C63" s="2">
         <v>19</v>
@@ -2637,7 +2637,7 @@
         <v>24</v>
       </c>
       <c r="B64" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C64" s="2">
         <v>23</v>
@@ -2654,7 +2654,7 @@
         <v>24</v>
       </c>
       <c r="B65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C65" s="2">
         <v>0</v>
@@ -2671,13 +2671,13 @@
         <v>41</v>
       </c>
       <c r="B66" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C66" s="2">
         <v>13</v>
       </c>
       <c r="D66" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E66" s="1">
         <v>43465</v>
@@ -2688,7 +2688,7 @@
         <v>41</v>
       </c>
       <c r="B67" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C67" s="2">
         <v>5</v>
@@ -2705,7 +2705,7 @@
         <v>41</v>
       </c>
       <c r="B68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C68" s="2">
         <v>8</v>
@@ -2722,7 +2722,7 @@
         <v>41</v>
       </c>
       <c r="B69" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C69" s="2">
         <v>19</v>
@@ -2739,7 +2739,7 @@
         <v>41</v>
       </c>
       <c r="B70" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C70" s="2">
         <v>7</v>
@@ -2756,7 +2756,7 @@
         <v>41</v>
       </c>
       <c r="B71" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C71" s="2">
         <v>26</v>
@@ -2773,7 +2773,7 @@
         <v>41</v>
       </c>
       <c r="B72" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C72" s="2">
         <v>8</v>
@@ -2790,7 +2790,7 @@
         <v>41</v>
       </c>
       <c r="B73" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C73" s="2">
         <v>10</v>
@@ -2807,7 +2807,7 @@
         <v>41</v>
       </c>
       <c r="B74" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C74" s="2">
         <v>5</v>
@@ -2824,7 +2824,7 @@
         <v>41</v>
       </c>
       <c r="B75" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C75" s="2">
         <v>10</v>
@@ -2841,7 +2841,7 @@
         <v>26</v>
       </c>
       <c r="B76" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C76" s="2">
         <v>7</v>
@@ -2858,7 +2858,7 @@
         <v>26</v>
       </c>
       <c r="B77" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C77" s="2">
         <v>6</v>
@@ -2875,7 +2875,7 @@
         <v>26</v>
       </c>
       <c r="B78" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C78" s="2">
         <v>8</v>
@@ -2892,7 +2892,7 @@
         <v>26</v>
       </c>
       <c r="B79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C79" s="2">
         <v>23</v>
@@ -2909,7 +2909,7 @@
         <v>26</v>
       </c>
       <c r="B80" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C80" s="2">
         <v>22</v>
@@ -2926,7 +2926,7 @@
         <v>26</v>
       </c>
       <c r="B81" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C81" s="2">
         <v>43</v>
@@ -2943,7 +2943,7 @@
         <v>26</v>
       </c>
       <c r="B82" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C82" s="2">
         <v>16</v>
@@ -2960,7 +2960,7 @@
         <v>26</v>
       </c>
       <c r="B83" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C83" s="2">
         <v>5</v>
@@ -2977,7 +2977,7 @@
         <v>26</v>
       </c>
       <c r="B84" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C84" s="2">
         <v>7</v>
@@ -2994,7 +2994,7 @@
         <v>26</v>
       </c>
       <c r="B85" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C85" s="2">
         <v>0</v>
@@ -3011,7 +3011,7 @@
         <v>19</v>
       </c>
       <c r="B86" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C86" s="2">
         <v>15</v>
@@ -3028,7 +3028,7 @@
         <v>19</v>
       </c>
       <c r="B87" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C87" s="2">
         <v>11</v>
@@ -3045,7 +3045,7 @@
         <v>19</v>
       </c>
       <c r="B88" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C88" s="2">
         <v>10</v>
@@ -3062,7 +3062,7 @@
         <v>19</v>
       </c>
       <c r="B89" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C89" s="2">
         <v>7</v>
@@ -3079,7 +3079,7 @@
         <v>19</v>
       </c>
       <c r="B90" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C90" s="2">
         <v>24</v>
@@ -3096,7 +3096,7 @@
         <v>19</v>
       </c>
       <c r="B91" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C91" s="2">
         <v>6</v>
@@ -3113,7 +3113,7 @@
         <v>19</v>
       </c>
       <c r="B92" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C92" s="2">
         <v>5</v>
@@ -3130,7 +3130,7 @@
         <v>19</v>
       </c>
       <c r="B93" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C93" s="2">
         <v>5</v>
@@ -3147,7 +3147,7 @@
         <v>15</v>
       </c>
       <c r="B94" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C94" s="2">
         <v>15</v>
@@ -3164,7 +3164,7 @@
         <v>15</v>
       </c>
       <c r="B95" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C95" s="2">
         <v>22</v>
@@ -3181,13 +3181,13 @@
         <v>15</v>
       </c>
       <c r="B96" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C96" s="2">
         <v>10</v>
       </c>
       <c r="D96" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E96" s="1">
         <v>43465</v>
@@ -3198,7 +3198,7 @@
         <v>15</v>
       </c>
       <c r="B97" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C97" s="2">
         <v>29</v>
@@ -3215,7 +3215,7 @@
         <v>15</v>
       </c>
       <c r="B98" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C98" s="2">
         <v>5</v>
@@ -3232,7 +3232,7 @@
         <v>15</v>
       </c>
       <c r="B99" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C99" s="2">
         <v>8</v>
@@ -3249,7 +3249,7 @@
         <v>15</v>
       </c>
       <c r="B100" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C100" s="2">
         <v>13</v>
@@ -3266,7 +3266,7 @@
         <v>15</v>
       </c>
       <c r="B101" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C101" s="2">
         <v>11</v>
@@ -3283,7 +3283,7 @@
         <v>15</v>
       </c>
       <c r="B102" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C102" s="2">
         <v>7</v>
@@ -3300,7 +3300,7 @@
         <v>17</v>
       </c>
       <c r="B103" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C103" s="2">
         <v>8</v>
@@ -3317,7 +3317,7 @@
         <v>17</v>
       </c>
       <c r="B104" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C104" s="2">
         <v>13</v>
@@ -3334,7 +3334,7 @@
         <v>17</v>
       </c>
       <c r="B105" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C105" s="2">
         <v>8</v>
@@ -3351,7 +3351,7 @@
         <v>17</v>
       </c>
       <c r="B106" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C106" s="2">
         <v>12</v>
@@ -3368,7 +3368,7 @@
         <v>17</v>
       </c>
       <c r="B107" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C107" s="2">
         <v>12</v>
@@ -3385,7 +3385,7 @@
         <v>17</v>
       </c>
       <c r="B108" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C108" s="2">
         <v>23</v>
@@ -3402,7 +3402,7 @@
         <v>17</v>
       </c>
       <c r="B109" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C109" s="2">
         <v>5</v>
@@ -3419,7 +3419,7 @@
         <v>17</v>
       </c>
       <c r="B110" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C110" s="2">
         <v>12</v>
@@ -3436,7 +3436,7 @@
         <v>17</v>
       </c>
       <c r="B111" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C111" s="2">
         <v>10</v>
@@ -3453,7 +3453,7 @@
         <v>17</v>
       </c>
       <c r="B112" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C112" s="2">
         <v>5</v>
@@ -3470,7 +3470,7 @@
         <v>22</v>
       </c>
       <c r="B113" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C113" s="2">
         <v>16</v>
@@ -3487,7 +3487,7 @@
         <v>22</v>
       </c>
       <c r="B114" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C114" s="2">
         <v>5</v>
@@ -3504,7 +3504,7 @@
         <v>22</v>
       </c>
       <c r="B115" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C115" s="2">
         <v>14</v>
@@ -3521,7 +3521,7 @@
         <v>22</v>
       </c>
       <c r="B116" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C116" s="2">
         <v>13</v>
@@ -3538,7 +3538,7 @@
         <v>22</v>
       </c>
       <c r="B117" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C117" s="2">
         <v>7</v>
@@ -3555,7 +3555,7 @@
         <v>22</v>
       </c>
       <c r="B118" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C118" s="2">
         <v>13</v>
@@ -3572,7 +3572,7 @@
         <v>22</v>
       </c>
       <c r="B119" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C119" s="2">
         <v>8</v>
@@ -3589,7 +3589,7 @@
         <v>22</v>
       </c>
       <c r="B120" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C120" s="2">
         <v>6</v>
@@ -3606,7 +3606,7 @@
         <v>22</v>
       </c>
       <c r="B121" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C121" s="2">
         <v>8</v>
@@ -3623,7 +3623,7 @@
         <v>22</v>
       </c>
       <c r="B122" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C122" s="2">
         <v>9</v>
@@ -3640,7 +3640,7 @@
         <v>22</v>
       </c>
       <c r="B123" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C123" s="2">
         <v>0</v>
@@ -3657,7 +3657,7 @@
         <v>22</v>
       </c>
       <c r="B124" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C124" s="2">
         <v>0</v>
@@ -3674,7 +3674,7 @@
         <v>12</v>
       </c>
       <c r="B125" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C125" s="2">
         <v>8</v>
@@ -3691,7 +3691,7 @@
         <v>12</v>
       </c>
       <c r="B126" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C126" s="2">
         <v>13</v>
@@ -3708,7 +3708,7 @@
         <v>12</v>
       </c>
       <c r="B127" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C127" s="2">
         <v>18</v>
@@ -3725,7 +3725,7 @@
         <v>12</v>
       </c>
       <c r="B128" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C128" s="2">
         <v>7</v>
@@ -3742,7 +3742,7 @@
         <v>12</v>
       </c>
       <c r="B129" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C129" s="2">
         <v>29</v>
@@ -3759,7 +3759,7 @@
         <v>12</v>
       </c>
       <c r="B130" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C130" s="2">
         <v>8</v>
@@ -3776,7 +3776,7 @@
         <v>12</v>
       </c>
       <c r="B131" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C131" s="2">
         <v>6</v>
@@ -3793,7 +3793,7 @@
         <v>12</v>
       </c>
       <c r="B132" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C132" s="2">
         <v>8</v>
@@ -3810,7 +3810,7 @@
         <v>12</v>
       </c>
       <c r="B133" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C133" s="2">
         <v>5</v>
@@ -3827,7 +3827,7 @@
         <v>12</v>
       </c>
       <c r="B134" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C134" s="2">
         <v>14</v>
@@ -3844,7 +3844,7 @@
         <v>12</v>
       </c>
       <c r="B135" t="s">
-        <v>167</v>
+        <v>226</v>
       </c>
       <c r="C135" s="2">
         <v>0</v>
@@ -3861,7 +3861,7 @@
         <v>12</v>
       </c>
       <c r="B136" t="s">
-        <v>168</v>
+        <v>227</v>
       </c>
       <c r="C136" s="2">
         <v>3</v>
@@ -3878,13 +3878,13 @@
         <v>39</v>
       </c>
       <c r="B137" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C137" s="2">
         <v>20</v>
       </c>
       <c r="D137" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E137" s="1">
         <v>43465</v>
@@ -3895,7 +3895,7 @@
         <v>39</v>
       </c>
       <c r="B138" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C138" s="2">
         <v>8</v>
@@ -3912,7 +3912,7 @@
         <v>39</v>
       </c>
       <c r="B139" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C139" s="2">
         <v>35</v>
@@ -3929,7 +3929,7 @@
         <v>39</v>
       </c>
       <c r="B140" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C140" s="2">
         <v>18</v>
@@ -3946,7 +3946,7 @@
         <v>39</v>
       </c>
       <c r="B141" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C141" s="2">
         <v>13</v>
@@ -3963,7 +3963,7 @@
         <v>39</v>
       </c>
       <c r="B142" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C142" s="2">
         <v>28</v>
@@ -3980,7 +3980,7 @@
         <v>39</v>
       </c>
       <c r="B143" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C143" s="2">
         <v>18</v>
@@ -3997,7 +3997,7 @@
         <v>39</v>
       </c>
       <c r="B144" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C144" s="2">
         <v>23</v>
@@ -4014,7 +4014,7 @@
         <v>39</v>
       </c>
       <c r="B145" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C145" s="2">
         <v>8</v>
@@ -4031,7 +4031,7 @@
         <v>39</v>
       </c>
       <c r="B146" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C146" s="2">
         <v>5</v>
@@ -4048,7 +4048,7 @@
         <v>39</v>
       </c>
       <c r="B147" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C147" s="2">
         <v>0</v>
@@ -4065,7 +4065,7 @@
         <v>39</v>
       </c>
       <c r="B148" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C148" s="2">
         <v>0</v>
@@ -4082,13 +4082,13 @@
         <v>9</v>
       </c>
       <c r="B149" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C149" s="2">
         <v>17</v>
       </c>
       <c r="D149" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E149" s="1">
         <v>43465</v>
@@ -4099,7 +4099,7 @@
         <v>9</v>
       </c>
       <c r="B150" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C150" s="2">
         <v>14</v>
@@ -4116,7 +4116,7 @@
         <v>9</v>
       </c>
       <c r="B151" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C151" s="2">
         <v>8</v>
@@ -4133,7 +4133,7 @@
         <v>9</v>
       </c>
       <c r="B152" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C152" s="2">
         <v>8</v>
@@ -4150,7 +4150,7 @@
         <v>9</v>
       </c>
       <c r="B153" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C153" s="2">
         <v>23</v>
@@ -4167,7 +4167,7 @@
         <v>9</v>
       </c>
       <c r="B154" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C154" s="2">
         <v>9</v>
@@ -4184,7 +4184,7 @@
         <v>9</v>
       </c>
       <c r="B155" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C155" s="2">
         <v>11</v>
@@ -4201,7 +4201,7 @@
         <v>9</v>
       </c>
       <c r="B156" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C156" s="2">
         <v>6</v>
@@ -4218,7 +4218,7 @@
         <v>9</v>
       </c>
       <c r="B157" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C157" s="2">
         <v>20</v>
@@ -4235,7 +4235,7 @@
         <v>9</v>
       </c>
       <c r="B158" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C158" s="2">
         <v>7</v>
@@ -4252,7 +4252,7 @@
         <v>9</v>
       </c>
       <c r="B159" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C159" s="2">
         <v>0</v>
@@ -4269,13 +4269,13 @@
         <v>37</v>
       </c>
       <c r="B160" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C160" s="2">
         <v>13</v>
       </c>
       <c r="D160" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E160" s="1">
         <v>43465</v>
@@ -4286,7 +4286,7 @@
         <v>37</v>
       </c>
       <c r="B161" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C161" s="2">
         <v>5</v>
@@ -4303,7 +4303,7 @@
         <v>37</v>
       </c>
       <c r="B162" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C162" s="2">
         <v>5</v>
@@ -4320,7 +4320,7 @@
         <v>37</v>
       </c>
       <c r="B163" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C163" s="2">
         <v>28</v>
@@ -4337,7 +4337,7 @@
         <v>37</v>
       </c>
       <c r="B164" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C164" s="2">
         <v>18</v>
@@ -4354,7 +4354,7 @@
         <v>37</v>
       </c>
       <c r="B165" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C165" s="2">
         <v>23</v>
@@ -4371,7 +4371,7 @@
         <v>37</v>
       </c>
       <c r="B166" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C166" s="2">
         <v>25</v>
@@ -4388,7 +4388,7 @@
         <v>37</v>
       </c>
       <c r="B167" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C167" s="2">
         <v>18</v>
@@ -4405,7 +4405,7 @@
         <v>37</v>
       </c>
       <c r="B168" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C168" s="2">
         <v>9</v>
@@ -4422,7 +4422,7 @@
         <v>37</v>
       </c>
       <c r="B169" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C169" s="2">
         <v>14</v>
@@ -4439,7 +4439,7 @@
         <v>37</v>
       </c>
       <c r="B170" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C170" s="2">
         <v>0</v>
@@ -4456,7 +4456,7 @@
         <v>37</v>
       </c>
       <c r="B171" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C171" s="2">
         <v>0</v>
@@ -4473,7 +4473,7 @@
         <v>35</v>
       </c>
       <c r="B172" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C172" s="2">
         <v>10</v>
@@ -4490,7 +4490,7 @@
         <v>35</v>
       </c>
       <c r="B173" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C173" s="2">
         <v>8</v>
@@ -4507,7 +4507,7 @@
         <v>35</v>
       </c>
       <c r="B174" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C174" s="2">
         <v>13</v>
@@ -4524,7 +4524,7 @@
         <v>35</v>
       </c>
       <c r="B175" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C175" s="2">
         <v>33</v>
@@ -4541,13 +4541,13 @@
         <v>35</v>
       </c>
       <c r="B176" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C176" s="2">
         <v>5</v>
       </c>
       <c r="D176" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E176" s="1">
         <v>43465</v>
@@ -4558,7 +4558,7 @@
         <v>35</v>
       </c>
       <c r="B177" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="C177" s="2">
         <v>5</v>
@@ -4575,7 +4575,7 @@
         <v>35</v>
       </c>
       <c r="B178" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C178" s="2">
         <v>5</v>
@@ -4592,7 +4592,7 @@
         <v>35</v>
       </c>
       <c r="B179" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C179" s="2">
         <v>33</v>
@@ -4609,7 +4609,7 @@
         <v>35</v>
       </c>
       <c r="B180" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C180" s="2">
         <v>8</v>
@@ -4626,7 +4626,7 @@
         <v>35</v>
       </c>
       <c r="B181" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C181" s="2">
         <v>48</v>
@@ -4643,7 +4643,7 @@
         <v>35</v>
       </c>
       <c r="B182" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C182" s="2">
         <v>2</v>
@@ -4660,7 +4660,7 @@
         <v>35</v>
       </c>
       <c r="B183" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C183" s="2">
         <v>3</v>
@@ -4677,7 +4677,7 @@
         <v>5</v>
       </c>
       <c r="B184" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C184" s="2">
         <v>13</v>
@@ -4694,7 +4694,7 @@
         <v>5</v>
       </c>
       <c r="B185" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C185" s="2">
         <v>13</v>
@@ -4711,7 +4711,7 @@
         <v>5</v>
       </c>
       <c r="B186" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C186" s="2">
         <v>12</v>
@@ -4728,7 +4728,7 @@
         <v>5</v>
       </c>
       <c r="B187" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C187" s="2">
         <v>22</v>
@@ -4745,7 +4745,7 @@
         <v>5</v>
       </c>
       <c r="B188" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C188" s="2">
         <v>22</v>
@@ -4762,7 +4762,7 @@
         <v>5</v>
       </c>
       <c r="B189" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C189" s="2">
         <v>5</v>
@@ -4779,7 +4779,7 @@
         <v>5</v>
       </c>
       <c r="B190" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C190" s="2">
         <v>5</v>
@@ -4796,7 +4796,7 @@
         <v>5</v>
       </c>
       <c r="B191" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C191" s="2">
         <v>5</v>
@@ -4813,7 +4813,7 @@
         <v>5</v>
       </c>
       <c r="B192" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C192" s="2">
         <v>29</v>
@@ -4830,7 +4830,7 @@
         <v>5</v>
       </c>
       <c r="B193" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C193" s="2">
         <v>6</v>
@@ -4847,7 +4847,7 @@
         <v>5</v>
       </c>
       <c r="B194" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C194" s="2">
         <v>3</v>
@@ -4864,7 +4864,7 @@
         <v>5</v>
       </c>
       <c r="B195" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C195" s="2">
         <v>4</v>
@@ -4883,7 +4883,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
fixed replacement pitching, reorganized things a bit
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D9D91CE6-20DE-4295-84A2-2DD965E3D856}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{02028A75-CB38-4465-BA5C-54EC645167C4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="232">
   <si>
     <t>team</t>
   </si>
@@ -705,6 +705,18 @@
   </si>
   <si>
     <t>Fernando Tatis Jr.</t>
+  </si>
+  <si>
+    <t>Willy Adames</t>
+  </si>
+  <si>
+    <t>DH</t>
+  </si>
+  <si>
+    <t>Kyle Hendricks</t>
+  </si>
+  <si>
+    <t>Jean Segura</t>
   </si>
 </sst>
 </file>
@@ -1550,10 +1562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E195"/>
+  <dimension ref="A1:E198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="B136" sqref="B136"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="E198" sqref="E198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4873,6 +4885,57 @@
         <v>48</v>
       </c>
       <c r="E195" s="1">
+        <v>43465</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>15</v>
+      </c>
+      <c r="B196" t="s">
+        <v>228</v>
+      </c>
+      <c r="C196" s="2">
+        <v>5</v>
+      </c>
+      <c r="D196" t="s">
+        <v>229</v>
+      </c>
+      <c r="E196" s="1">
+        <v>43465</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>24</v>
+      </c>
+      <c r="B197" t="s">
+        <v>230</v>
+      </c>
+      <c r="C197" s="2">
+        <v>18</v>
+      </c>
+      <c r="D197" t="s">
+        <v>21</v>
+      </c>
+      <c r="E197" s="1">
+        <v>43465</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>26</v>
+      </c>
+      <c r="B198" t="s">
+        <v>231</v>
+      </c>
+      <c r="C198" s="2">
+        <v>22</v>
+      </c>
+      <c r="D198" t="s">
+        <v>8</v>
+      </c>
+      <c r="E198" s="1">
         <v>43465</v>
       </c>
     </row>

</xml_diff>

<commit_message>
end of dispersal draft, start of auction. added some new features to the draft guide.
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{02028A75-CB38-4465-BA5C-54EC645167C4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0BA82F97-A659-410A-B3AF-24FBBEE1381F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="238">
   <si>
     <t>team</t>
   </si>
@@ -717,6 +717,24 @@
   </si>
   <si>
     <t>Jean Segura</t>
+  </si>
+  <si>
+    <t>Ross Stripling</t>
+  </si>
+  <si>
+    <t>Jorge Polanco</t>
+  </si>
+  <si>
+    <t>Michael Kopech</t>
+  </si>
+  <si>
+    <t>Niko Goodrum</t>
+  </si>
+  <si>
+    <t>Jose Alvarado</t>
+  </si>
+  <si>
+    <t>Lourdes Gurriel Jr.</t>
   </si>
 </sst>
 </file>
@@ -1562,10 +1580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E198"/>
+  <dimension ref="A1:E204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="E198" sqref="E198"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="B199" sqref="B199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2162,7 +2180,7 @@
         <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E35" s="1">
         <v>43465</v>
@@ -2179,7 +2197,7 @@
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E36" s="1">
         <v>43465</v>
@@ -3692,7 +3710,7 @@
         <v>8</v>
       </c>
       <c r="D125" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="E125" s="1">
         <v>43465</v>
@@ -4321,7 +4339,7 @@
         <v>5</v>
       </c>
       <c r="D162" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E162" s="1">
         <v>43465</v>
@@ -4937,6 +4955,108 @@
       </c>
       <c r="E198" s="1">
         <v>43465</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>19</v>
+      </c>
+      <c r="B199" t="s">
+        <v>237</v>
+      </c>
+      <c r="C199" s="2">
+        <v>7</v>
+      </c>
+      <c r="D199" t="s">
+        <v>29</v>
+      </c>
+      <c r="E199" s="1">
+        <v>43465</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>6</v>
+      </c>
+      <c r="B200" t="s">
+        <v>232</v>
+      </c>
+      <c r="C200" s="2">
+        <v>5</v>
+      </c>
+      <c r="D200" t="s">
+        <v>21</v>
+      </c>
+      <c r="E200" s="1">
+        <v>43103</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>84</v>
+      </c>
+      <c r="B201" t="s">
+        <v>233</v>
+      </c>
+      <c r="C201" s="2">
+        <v>13</v>
+      </c>
+      <c r="D201" t="s">
+        <v>8</v>
+      </c>
+      <c r="E201" s="1">
+        <v>43103</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>24</v>
+      </c>
+      <c r="B202" t="s">
+        <v>234</v>
+      </c>
+      <c r="C202" s="2">
+        <v>0</v>
+      </c>
+      <c r="D202" t="s">
+        <v>48</v>
+      </c>
+      <c r="E202" s="1">
+        <v>43103</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>19</v>
+      </c>
+      <c r="B203" t="s">
+        <v>235</v>
+      </c>
+      <c r="C203" s="2">
+        <v>5</v>
+      </c>
+      <c r="D203" t="s">
+        <v>29</v>
+      </c>
+      <c r="E203" s="1">
+        <v>43103</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>6</v>
+      </c>
+      <c r="B204" t="s">
+        <v>236</v>
+      </c>
+      <c r="C204" s="2">
+        <v>5</v>
+      </c>
+      <c r="D204" t="s">
+        <v>21</v>
+      </c>
+      <c r="E204" s="1">
+        <v>43103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first day of draft picks
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0BA82F97-A659-410A-B3AF-24FBBEE1381F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D878B45D-6CDE-4556-9932-DA97DFF81C66}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="246">
   <si>
     <t>team</t>
   </si>
@@ -735,6 +735,30 @@
   </si>
   <si>
     <t>Lourdes Gurriel Jr.</t>
+  </si>
+  <si>
+    <t>Max Scherzer</t>
+  </si>
+  <si>
+    <t>Giancarlo Stanton</t>
+  </si>
+  <si>
+    <t>Paul Goldschmidt</t>
+  </si>
+  <si>
+    <t>Aroldis Chapman</t>
+  </si>
+  <si>
+    <t>Buster Posey</t>
+  </si>
+  <si>
+    <t>Kenley Jansen</t>
+  </si>
+  <si>
+    <t>Shin-Soo Choo</t>
+  </si>
+  <si>
+    <t>Willians Astudillo</t>
   </si>
 </sst>
 </file>
@@ -1580,14 +1604,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E204"/>
+  <dimension ref="A1:E212"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="B199" sqref="B199"/>
+      <selection activeCell="E206" sqref="E206:E212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1598,7 +1624,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -1615,7 +1641,7 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>8</v>
       </c>
       <c r="D2" t="s">
@@ -1632,7 +1658,7 @@
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>18</v>
       </c>
       <c r="D3" t="s">
@@ -1649,7 +1675,7 @@
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>8</v>
       </c>
       <c r="D4" t="s">
@@ -1666,7 +1692,7 @@
       <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>17</v>
       </c>
       <c r="D5" t="s">
@@ -1683,7 +1709,7 @@
       <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>18</v>
       </c>
       <c r="D6" t="s">
@@ -1700,7 +1726,7 @@
       <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>18</v>
       </c>
       <c r="D7" t="s">
@@ -1717,7 +1743,7 @@
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>7</v>
       </c>
       <c r="D8" t="s">
@@ -1734,7 +1760,7 @@
       <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>19</v>
       </c>
       <c r="D9" t="s">
@@ -1751,7 +1777,7 @@
       <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>13</v>
       </c>
       <c r="D10" t="s">
@@ -1768,7 +1794,7 @@
       <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>8</v>
       </c>
       <c r="D11" t="s">
@@ -1785,7 +1811,7 @@
       <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>8</v>
       </c>
       <c r="D12" t="s">
@@ -1802,7 +1828,7 @@
       <c r="B13" t="s">
         <v>34</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>11</v>
       </c>
       <c r="D13" t="s">
@@ -1819,7 +1845,7 @@
       <c r="B14" t="s">
         <v>36</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>19</v>
       </c>
       <c r="D14" t="s">
@@ -1836,7 +1862,7 @@
       <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>7</v>
       </c>
       <c r="D15" t="s">
@@ -1853,7 +1879,7 @@
       <c r="B16" t="s">
         <v>40</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>14</v>
       </c>
       <c r="D16" t="s">
@@ -1870,7 +1896,7 @@
       <c r="B17" t="s">
         <v>42</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>12</v>
       </c>
       <c r="D17" t="s">
@@ -1887,7 +1913,7 @@
       <c r="B18" t="s">
         <v>44</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>8</v>
       </c>
       <c r="D18" t="s">
@@ -1904,7 +1930,7 @@
       <c r="B19" t="s">
         <v>46</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>7</v>
       </c>
       <c r="D19" t="s">
@@ -1921,7 +1947,7 @@
       <c r="B20" t="s">
         <v>47</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>2</v>
       </c>
       <c r="D20" t="s">
@@ -1938,7 +1964,7 @@
       <c r="B21" t="s">
         <v>49</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>6</v>
       </c>
       <c r="D21" t="s">
@@ -5057,6 +5083,142 @@
       </c>
       <c r="E204" s="1">
         <v>43103</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>5</v>
+      </c>
+      <c r="B205" t="s">
+        <v>238</v>
+      </c>
+      <c r="C205" s="2">
+        <v>48</v>
+      </c>
+      <c r="D205" t="s">
+        <v>21</v>
+      </c>
+      <c r="E205" s="1">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>26</v>
+      </c>
+      <c r="B206" t="s">
+        <v>239</v>
+      </c>
+      <c r="C206" s="2">
+        <v>43</v>
+      </c>
+      <c r="D206" t="s">
+        <v>14</v>
+      </c>
+      <c r="E206" s="1">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>43</v>
+      </c>
+      <c r="B207" t="s">
+        <v>240</v>
+      </c>
+      <c r="C207" s="2">
+        <v>15</v>
+      </c>
+      <c r="D207" t="s">
+        <v>33</v>
+      </c>
+      <c r="E207" s="1">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>17</v>
+      </c>
+      <c r="B208" t="s">
+        <v>241</v>
+      </c>
+      <c r="C208" s="2">
+        <v>37</v>
+      </c>
+      <c r="D208" t="s">
+        <v>21</v>
+      </c>
+      <c r="E208" s="1">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>5</v>
+      </c>
+      <c r="B209" t="s">
+        <v>242</v>
+      </c>
+      <c r="C209" s="2">
+        <v>25</v>
+      </c>
+      <c r="D209" t="s">
+        <v>106</v>
+      </c>
+      <c r="E209" s="1">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>9</v>
+      </c>
+      <c r="B210" t="s">
+        <v>243</v>
+      </c>
+      <c r="C210" s="2">
+        <v>20</v>
+      </c>
+      <c r="D210" t="s">
+        <v>21</v>
+      </c>
+      <c r="E210" s="1">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>9</v>
+      </c>
+      <c r="B211" t="s">
+        <v>244</v>
+      </c>
+      <c r="C211" s="2">
+        <v>20</v>
+      </c>
+      <c r="D211" t="s">
+        <v>14</v>
+      </c>
+      <c r="E211" s="1">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>37</v>
+      </c>
+      <c r="B212" t="s">
+        <v>245</v>
+      </c>
+      <c r="C212" s="2">
+        <v>9</v>
+      </c>
+      <c r="D212" t="s">
+        <v>106</v>
+      </c>
+      <c r="E212" s="1">
+        <v>43108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying to fix replacement level
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BB803CB6-FC17-4583-B117-4DE21BBA9067}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C059CB16-3E48-4591-ABAB-E7FDCA74E4F5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="278">
   <si>
     <t>team</t>
   </si>
@@ -831,6 +831,30 @@
   </si>
   <si>
     <t>Starling Marte</t>
+  </si>
+  <si>
+    <t>Eric Hosmer</t>
+  </si>
+  <si>
+    <t>Robinson Cano</t>
+  </si>
+  <si>
+    <t>Albert Pujols</t>
+  </si>
+  <si>
+    <t>Dallas Keuchel</t>
+  </si>
+  <si>
+    <t>Joshua James</t>
+  </si>
+  <si>
+    <t>Jonathan Schoop</t>
+  </si>
+  <si>
+    <t>Edwin Encarnacion</t>
+  </si>
+  <si>
+    <t>Asdrubal Cabrera</t>
   </si>
 </sst>
 </file>
@@ -840,7 +864,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -974,6 +998,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF55595C"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1317,10 +1347,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1676,10 +1707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E236"/>
+  <dimension ref="A1:E244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
-      <selection activeCell="L233" sqref="L233"/>
+    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
+      <selection activeCell="D243" sqref="D243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5700,6 +5731,142 @@
       </c>
       <c r="E236" s="1">
         <v>43111</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>84</v>
+      </c>
+      <c r="B237" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C237" s="2">
+        <v>14</v>
+      </c>
+      <c r="D237" t="s">
+        <v>33</v>
+      </c>
+      <c r="E237" s="1">
+        <v>43114</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>17</v>
+      </c>
+      <c r="B238" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C238" s="2">
+        <v>17</v>
+      </c>
+      <c r="D238" t="s">
+        <v>29</v>
+      </c>
+      <c r="E238" s="1">
+        <v>43114</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>27</v>
+      </c>
+      <c r="B239" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C239" s="2">
+        <v>10</v>
+      </c>
+      <c r="D239" t="s">
+        <v>61</v>
+      </c>
+      <c r="E239" s="1">
+        <v>43114</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>41</v>
+      </c>
+      <c r="B240" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C240" s="2">
+        <v>16</v>
+      </c>
+      <c r="D240" t="s">
+        <v>21</v>
+      </c>
+      <c r="E240" s="1">
+        <v>43114</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>9</v>
+      </c>
+      <c r="B241" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C241" s="2">
+        <v>16</v>
+      </c>
+      <c r="D241" t="s">
+        <v>21</v>
+      </c>
+      <c r="E241" s="1">
+        <v>43114</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>27</v>
+      </c>
+      <c r="B242" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C242" s="2">
+        <v>10</v>
+      </c>
+      <c r="D242" t="s">
+        <v>95</v>
+      </c>
+      <c r="E242" s="1">
+        <v>43114</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>19</v>
+      </c>
+      <c r="B243" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C243" s="2">
+        <v>23</v>
+      </c>
+      <c r="D243" t="s">
+        <v>61</v>
+      </c>
+      <c r="E243" s="1">
+        <v>43114</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>27</v>
+      </c>
+      <c r="B244" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C244" s="2">
+        <v>5</v>
+      </c>
+      <c r="D244" t="s">
+        <v>8</v>
+      </c>
+      <c r="E244" s="1">
+        <v>43114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More draft picks, corrected data entry errors
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D0CBEE02-A9B3-492B-89E5-0F4E40AA13AE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74B0925-397B-45FC-B6CF-3024FB753F9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,19 @@
     <sheet name="draftpicks" sheetId="1" r:id="rId1"/>
     <sheet name="teams" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="318">
   <si>
     <t>team</t>
   </si>
@@ -903,6 +910,78 @@
   </si>
   <si>
     <t>Cedric Mullins II</t>
+  </si>
+  <si>
+    <t>Jon Gray</t>
+  </si>
+  <si>
+    <t>Starlin Castro</t>
+  </si>
+  <si>
+    <t>Daniel Murphy</t>
+  </si>
+  <si>
+    <t>Max Kepler</t>
+  </si>
+  <si>
+    <t>Dylan Bundy</t>
+  </si>
+  <si>
+    <t>Salvador Perez</t>
+  </si>
+  <si>
+    <t>Joc Pederson</t>
+  </si>
+  <si>
+    <t>Yu Darvish</t>
+  </si>
+  <si>
+    <t>Justus Sheffield</t>
+  </si>
+  <si>
+    <t>Seranthony Dominguez</t>
+  </si>
+  <si>
+    <t>Kevin Gausman</t>
+  </si>
+  <si>
+    <t>Kyle Schwarber</t>
+  </si>
+  <si>
+    <t>Marcus Semien</t>
+  </si>
+  <si>
+    <t>Shane Bieber</t>
+  </si>
+  <si>
+    <t>DJ LeMahieu</t>
+  </si>
+  <si>
+    <t>Archie Bradley</t>
+  </si>
+  <si>
+    <t>Justin Upton</t>
+  </si>
+  <si>
+    <t>Ender Inciarte</t>
+  </si>
+  <si>
+    <t>Yoan Moncada</t>
+  </si>
+  <si>
+    <t>Adam Eaton</t>
+  </si>
+  <si>
+    <t>Carlos Santana</t>
+  </si>
+  <si>
+    <t>Byron Buxton</t>
+  </si>
+  <si>
+    <t>David Robertson</t>
+  </si>
+  <si>
+    <t>Rich Hill</t>
   </si>
 </sst>
 </file>
@@ -1748,10 +1827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E260"/>
+  <dimension ref="A1:E284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A251" workbookViewId="0">
+      <selection activeCell="E284" sqref="A276:E284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3201,7 +3280,7 @@
         <v>0</v>
       </c>
       <c r="D85" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="E85" s="1">
         <v>43465</v>
@@ -5272,7 +5351,7 @@
         <v>239</v>
       </c>
       <c r="C207" s="2">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D207" t="s">
         <v>33</v>
@@ -5289,7 +5368,7 @@
         <v>240</v>
       </c>
       <c r="C208" s="2">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D208" t="s">
         <v>21</v>
@@ -5306,7 +5385,7 @@
         <v>241</v>
       </c>
       <c r="C209" s="2">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D209" t="s">
         <v>105</v>
@@ -5340,7 +5419,7 @@
         <v>243</v>
       </c>
       <c r="C211" s="2">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D211" t="s">
         <v>14</v>
@@ -6182,7 +6261,418 @@
         <v>43116</v>
       </c>
     </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>24</v>
+      </c>
+      <c r="B261" t="s">
+        <v>294</v>
+      </c>
+      <c r="C261" s="2">
+        <v>12</v>
+      </c>
+      <c r="D261" t="s">
+        <v>21</v>
+      </c>
+      <c r="E261" s="1">
+        <v>43117</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>24</v>
+      </c>
+      <c r="B262" t="s">
+        <v>295</v>
+      </c>
+      <c r="C262" s="2">
+        <v>9</v>
+      </c>
+      <c r="D262" t="s">
+        <v>29</v>
+      </c>
+      <c r="E262" s="1">
+        <v>43117</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>22</v>
+      </c>
+      <c r="B263" t="s">
+        <v>297</v>
+      </c>
+      <c r="C263" s="2">
+        <v>14</v>
+      </c>
+      <c r="D263" t="s">
+        <v>14</v>
+      </c>
+      <c r="E263" s="1">
+        <v>43117</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>22</v>
+      </c>
+      <c r="B264" t="s">
+        <v>299</v>
+      </c>
+      <c r="C264" s="2">
+        <v>20</v>
+      </c>
+      <c r="D264" t="s">
+        <v>105</v>
+      </c>
+      <c r="E264" s="1">
+        <v>43117</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>17</v>
+      </c>
+      <c r="B265" t="s">
+        <v>298</v>
+      </c>
+      <c r="C265" s="2">
+        <v>6</v>
+      </c>
+      <c r="D265" t="s">
+        <v>21</v>
+      </c>
+      <c r="E265" s="1">
+        <v>43117</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>17</v>
+      </c>
+      <c r="B266" t="s">
+        <v>300</v>
+      </c>
+      <c r="C266" s="2">
+        <v>17</v>
+      </c>
+      <c r="D266" t="s">
+        <v>14</v>
+      </c>
+      <c r="E266" s="1">
+        <v>43117</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>39</v>
+      </c>
+      <c r="B267" t="s">
+        <v>301</v>
+      </c>
+      <c r="C267" s="2">
+        <v>15</v>
+      </c>
+      <c r="D267" t="s">
+        <v>21</v>
+      </c>
+      <c r="E267" s="1">
+        <v>43117</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>37</v>
+      </c>
+      <c r="B268" t="s">
+        <v>296</v>
+      </c>
+      <c r="C268" s="2">
+        <v>19</v>
+      </c>
+      <c r="D268" t="s">
+        <v>95</v>
+      </c>
+      <c r="E268" s="1">
+        <v>43117</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>6</v>
+      </c>
+      <c r="B269" t="s">
+        <v>302</v>
+      </c>
+      <c r="C269" s="2">
+        <v>4</v>
+      </c>
+      <c r="D269" t="s">
+        <v>21</v>
+      </c>
+      <c r="E269" s="1">
+        <v>43118</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>6</v>
+      </c>
+      <c r="B270" t="s">
+        <v>304</v>
+      </c>
+      <c r="C270" s="2">
+        <v>21</v>
+      </c>
+      <c r="D270" t="s">
+        <v>21</v>
+      </c>
+      <c r="E270" s="1">
+        <v>43118</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>84</v>
+      </c>
+      <c r="B271" t="s">
+        <v>307</v>
+      </c>
+      <c r="C271" s="2">
+        <v>13</v>
+      </c>
+      <c r="D271" t="s">
+        <v>21</v>
+      </c>
+      <c r="E271" s="1">
+        <v>43118</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>41</v>
+      </c>
+      <c r="B272" t="s">
+        <v>305</v>
+      </c>
+      <c r="C272" s="2">
+        <v>18</v>
+      </c>
+      <c r="D272" t="s">
+        <v>14</v>
+      </c>
+      <c r="E272" s="1">
+        <v>43118</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>41</v>
+      </c>
+      <c r="B273" t="s">
+        <v>306</v>
+      </c>
+      <c r="C273" s="2">
+        <v>9</v>
+      </c>
+      <c r="D273" t="s">
+        <v>8</v>
+      </c>
+      <c r="E273" s="1">
+        <v>43118</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>22</v>
+      </c>
+      <c r="B274" t="s">
+        <v>303</v>
+      </c>
+      <c r="C274" s="2">
+        <v>12</v>
+      </c>
+      <c r="D274" t="s">
+        <v>21</v>
+      </c>
+      <c r="E274" s="1">
+        <v>43118</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>22</v>
+      </c>
+      <c r="B275" t="s">
+        <v>309</v>
+      </c>
+      <c r="C275" s="2">
+        <v>12</v>
+      </c>
+      <c r="D275" t="s">
+        <v>21</v>
+      </c>
+      <c r="E275" s="1">
+        <v>43118</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>9</v>
+      </c>
+      <c r="B276" t="s">
+        <v>308</v>
+      </c>
+      <c r="C276" s="2">
+        <v>10</v>
+      </c>
+      <c r="D276" t="s">
+        <v>95</v>
+      </c>
+      <c r="E276" s="1">
+        <v>43118</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>22</v>
+      </c>
+      <c r="B277" t="s">
+        <v>310</v>
+      </c>
+      <c r="C277" s="2">
+        <v>26</v>
+      </c>
+      <c r="D277" t="s">
+        <v>14</v>
+      </c>
+      <c r="E277" s="1">
+        <v>43121</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>22</v>
+      </c>
+      <c r="B278" t="s">
+        <v>311</v>
+      </c>
+      <c r="C278" s="2">
+        <v>19</v>
+      </c>
+      <c r="D278" t="s">
+        <v>14</v>
+      </c>
+      <c r="E278" s="1">
+        <v>43121</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>6</v>
+      </c>
+      <c r="B279" t="s">
+        <v>312</v>
+      </c>
+      <c r="C279" s="2">
+        <v>15</v>
+      </c>
+      <c r="D279" t="s">
+        <v>29</v>
+      </c>
+      <c r="E279" s="1">
+        <v>43121</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>84</v>
+      </c>
+      <c r="B280" t="s">
+        <v>313</v>
+      </c>
+      <c r="C280" s="2">
+        <v>13</v>
+      </c>
+      <c r="D280" t="s">
+        <v>14</v>
+      </c>
+      <c r="E280" s="1">
+        <v>43121</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>15</v>
+      </c>
+      <c r="B281" t="s">
+        <v>314</v>
+      </c>
+      <c r="C281" s="2">
+        <v>15</v>
+      </c>
+      <c r="D281" t="s">
+        <v>33</v>
+      </c>
+      <c r="E281" s="1">
+        <v>43121</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>39</v>
+      </c>
+      <c r="B282" t="s">
+        <v>315</v>
+      </c>
+      <c r="C282" s="2">
+        <v>15</v>
+      </c>
+      <c r="D282" t="s">
+        <v>14</v>
+      </c>
+      <c r="E282" s="1">
+        <v>43121</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>43</v>
+      </c>
+      <c r="B283" t="s">
+        <v>316</v>
+      </c>
+      <c r="C283" s="2">
+        <v>8</v>
+      </c>
+      <c r="D283" t="s">
+        <v>21</v>
+      </c>
+      <c r="E283" s="1">
+        <v>43121</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>9</v>
+      </c>
+      <c r="B284" t="s">
+        <v>317</v>
+      </c>
+      <c r="C284" s="2">
+        <v>15</v>
+      </c>
+      <c r="D284" t="s">
+        <v>21</v>
+      </c>
+      <c r="E284" s="1">
+        <v>43121</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A261:E276">
+    <sortCondition ref="E261:E276"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
More draft picks, added fans and thebat and new depth charts
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFA116D-61BD-4F41-9653-E6230A689ED8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566B5C71-8569-45AA-A2FC-EF5940D2955B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="342">
   <si>
     <t>team</t>
   </si>
@@ -1030,6 +1030,30 @@
   </si>
   <si>
     <t>Jakob Junis</t>
+  </si>
+  <si>
+    <t>Rougned Odor</t>
+  </si>
+  <si>
+    <t>Andrew McCutchen</t>
+  </si>
+  <si>
+    <t>Alex Verdugo</t>
+  </si>
+  <si>
+    <t>Avisail Garcia</t>
+  </si>
+  <si>
+    <t>Hunter Renfroe</t>
+  </si>
+  <si>
+    <t>Tyler Flowers</t>
+  </si>
+  <si>
+    <t>Corey Knebel</t>
+  </si>
+  <si>
+    <t>Mike Zunino</t>
   </si>
 </sst>
 </file>
@@ -1885,10 +1909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E300"/>
+  <dimension ref="A1:E308"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A272" workbookViewId="0">
-      <selection activeCell="B300" sqref="B300"/>
+    <sheetView tabSelected="1" topLeftCell="A293" workbookViewId="0">
+      <selection activeCell="I295" sqref="I295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6997,6 +7021,142 @@
       </c>
       <c r="E300" s="1">
         <v>43123</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>22</v>
+      </c>
+      <c r="B301" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C301" s="2">
+        <v>19</v>
+      </c>
+      <c r="D301" t="s">
+        <v>95</v>
+      </c>
+      <c r="E301" s="1">
+        <v>43124</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>45</v>
+      </c>
+      <c r="B302" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C302" s="2">
+        <v>23</v>
+      </c>
+      <c r="D302" t="s">
+        <v>14</v>
+      </c>
+      <c r="E302" s="1">
+        <v>43124</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>9</v>
+      </c>
+      <c r="B303" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C303" s="2">
+        <v>8</v>
+      </c>
+      <c r="D303" t="s">
+        <v>14</v>
+      </c>
+      <c r="E303" s="1">
+        <v>43124</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>24</v>
+      </c>
+      <c r="B304" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C304" s="2">
+        <v>8</v>
+      </c>
+      <c r="D304" t="s">
+        <v>14</v>
+      </c>
+      <c r="E304" s="1">
+        <v>43124</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>12</v>
+      </c>
+      <c r="B305" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C305" s="2">
+        <v>14</v>
+      </c>
+      <c r="D305" t="s">
+        <v>14</v>
+      </c>
+      <c r="E305" s="1">
+        <v>43124</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>84</v>
+      </c>
+      <c r="B306" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C306" s="2">
+        <v>3</v>
+      </c>
+      <c r="D306" t="s">
+        <v>105</v>
+      </c>
+      <c r="E306" s="1">
+        <v>43124</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>24</v>
+      </c>
+      <c r="B307" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="C307" s="2">
+        <v>16</v>
+      </c>
+      <c r="D307" t="s">
+        <v>21</v>
+      </c>
+      <c r="E307" s="1">
+        <v>43124</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>12</v>
+      </c>
+      <c r="B308" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="C308" s="2">
+        <v>8</v>
+      </c>
+      <c r="D308" t="s">
+        <v>105</v>
+      </c>
+      <c r="E308" s="1">
+        <v>43124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added best picks of the draft to draft guide
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6AFF84-9B77-40BB-A478-3924B6047931}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3E98BB-8207-48B4-B263-74099F2C6554}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1925,8 +1925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E316"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A281" workbookViewId="0">
-      <selection activeCell="A293" sqref="A293:E316"/>
+    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
+      <selection activeCell="G204" sqref="G204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5334,7 +5334,7 @@
         <v>21</v>
       </c>
       <c r="E200" s="1">
-        <v>43103</v>
+        <v>43468</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5351,7 +5351,7 @@
         <v>8</v>
       </c>
       <c r="E201" s="1">
-        <v>43103</v>
+        <v>43468</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -5368,7 +5368,7 @@
         <v>48</v>
       </c>
       <c r="E202" s="1">
-        <v>43103</v>
+        <v>43468</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -5385,7 +5385,7 @@
         <v>29</v>
       </c>
       <c r="E203" s="1">
-        <v>43103</v>
+        <v>43468</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5402,7 +5402,7 @@
         <v>21</v>
       </c>
       <c r="E204" s="1">
-        <v>43103</v>
+        <v>43468</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -5419,7 +5419,7 @@
         <v>21</v>
       </c>
       <c r="E205" s="1">
-        <v>43108</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
@@ -5436,7 +5436,7 @@
         <v>14</v>
       </c>
       <c r="E206" s="1">
-        <v>43108</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -5453,7 +5453,7 @@
         <v>33</v>
       </c>
       <c r="E207" s="1">
-        <v>43108</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -5470,7 +5470,7 @@
         <v>21</v>
       </c>
       <c r="E208" s="1">
-        <v>43108</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -5487,7 +5487,7 @@
         <v>105</v>
       </c>
       <c r="E209" s="1">
-        <v>43108</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -5504,7 +5504,7 @@
         <v>21</v>
       </c>
       <c r="E210" s="1">
-        <v>43108</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -5521,7 +5521,7 @@
         <v>14</v>
       </c>
       <c r="E211" s="1">
-        <v>43108</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -5538,7 +5538,7 @@
         <v>105</v>
       </c>
       <c r="E212" s="1">
-        <v>43108</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -5555,7 +5555,7 @@
         <v>61</v>
       </c>
       <c r="E213" s="1">
-        <v>43109</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -5572,7 +5572,7 @@
         <v>21</v>
       </c>
       <c r="E214" s="1">
-        <v>43109</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -5589,7 +5589,7 @@
         <v>33</v>
       </c>
       <c r="E215" s="1">
-        <v>43109</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -5606,7 +5606,7 @@
         <v>95</v>
       </c>
       <c r="E216" s="1">
-        <v>43109</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -5623,7 +5623,7 @@
         <v>21</v>
       </c>
       <c r="E217" s="1">
-        <v>43109</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -5640,7 +5640,7 @@
         <v>61</v>
       </c>
       <c r="E218" s="1">
-        <v>43109</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -5657,7 +5657,7 @@
         <v>14</v>
       </c>
       <c r="E219" s="1">
-        <v>43109</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -5674,7 +5674,7 @@
         <v>228</v>
       </c>
       <c r="E220" s="1">
-        <v>43109</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
@@ -5691,7 +5691,7 @@
         <v>33</v>
       </c>
       <c r="E221" s="1">
-        <v>43110</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
@@ -5708,7 +5708,7 @@
         <v>21</v>
       </c>
       <c r="E222" s="1">
-        <v>43110</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -5725,7 +5725,7 @@
         <v>21</v>
       </c>
       <c r="E223" s="1">
-        <v>43110</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -5742,7 +5742,7 @@
         <v>14</v>
       </c>
       <c r="E224" s="1">
-        <v>43110</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -5759,7 +5759,7 @@
         <v>21</v>
       </c>
       <c r="E225" s="1">
-        <v>43110</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
@@ -5776,7 +5776,7 @@
         <v>11</v>
       </c>
       <c r="E226" s="1">
-        <v>43110</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -5793,7 +5793,7 @@
         <v>21</v>
       </c>
       <c r="E227" s="1">
-        <v>43110</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -5810,7 +5810,7 @@
         <v>21</v>
       </c>
       <c r="E228" s="1">
-        <v>43110</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -5827,7 +5827,7 @@
         <v>14</v>
       </c>
       <c r="E229" s="1">
-        <v>43111</v>
+        <v>43476</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
@@ -5844,7 +5844,7 @@
         <v>95</v>
       </c>
       <c r="E230" s="1">
-        <v>43111</v>
+        <v>43476</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -5861,7 +5861,7 @@
         <v>11</v>
       </c>
       <c r="E231" s="1">
-        <v>43111</v>
+        <v>43476</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
@@ -5878,7 +5878,7 @@
         <v>21</v>
       </c>
       <c r="E232" s="1">
-        <v>43111</v>
+        <v>43476</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
@@ -5895,7 +5895,7 @@
         <v>14</v>
       </c>
       <c r="E233" s="1">
-        <v>43111</v>
+        <v>43476</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
@@ -5912,7 +5912,7 @@
         <v>105</v>
       </c>
       <c r="E234" s="1">
-        <v>43111</v>
+        <v>43476</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
@@ -5929,7 +5929,7 @@
         <v>228</v>
       </c>
       <c r="E235" s="1">
-        <v>43111</v>
+        <v>43476</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
@@ -5946,7 +5946,7 @@
         <v>21</v>
       </c>
       <c r="E236" s="1">
-        <v>43111</v>
+        <v>43476</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
@@ -5963,7 +5963,7 @@
         <v>33</v>
       </c>
       <c r="E237" s="1">
-        <v>43114</v>
+        <v>43479</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -5980,7 +5980,7 @@
         <v>29</v>
       </c>
       <c r="E238" s="1">
-        <v>43114</v>
+        <v>43479</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
@@ -5997,7 +5997,7 @@
         <v>61</v>
       </c>
       <c r="E239" s="1">
-        <v>43114</v>
+        <v>43479</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
@@ -6014,7 +6014,7 @@
         <v>21</v>
       </c>
       <c r="E240" s="1">
-        <v>43114</v>
+        <v>43479</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -6031,7 +6031,7 @@
         <v>21</v>
       </c>
       <c r="E241" s="1">
-        <v>43114</v>
+        <v>43479</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
@@ -6048,7 +6048,7 @@
         <v>95</v>
       </c>
       <c r="E242" s="1">
-        <v>43114</v>
+        <v>43479</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
@@ -6065,7 +6065,7 @@
         <v>61</v>
       </c>
       <c r="E243" s="1">
-        <v>43114</v>
+        <v>43479</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
@@ -6082,7 +6082,7 @@
         <v>8</v>
       </c>
       <c r="E244" s="1">
-        <v>43114</v>
+        <v>43479</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -6099,7 +6099,7 @@
         <v>21</v>
       </c>
       <c r="E245" s="1">
-        <v>43115</v>
+        <v>43480</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6116,7 +6116,7 @@
         <v>14</v>
       </c>
       <c r="E246" s="1">
-        <v>43115</v>
+        <v>43480</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6133,7 +6133,7 @@
         <v>14</v>
       </c>
       <c r="E247" s="1">
-        <v>43115</v>
+        <v>43480</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
@@ -6150,7 +6150,7 @@
         <v>61</v>
       </c>
       <c r="E248" s="1">
-        <v>43115</v>
+        <v>43480</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
@@ -6167,7 +6167,7 @@
         <v>14</v>
       </c>
       <c r="E249" s="1">
-        <v>43115</v>
+        <v>43480</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
@@ -6184,7 +6184,7 @@
         <v>21</v>
       </c>
       <c r="E250" s="1">
-        <v>43115</v>
+        <v>43480</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -6201,7 +6201,7 @@
         <v>21</v>
       </c>
       <c r="E251" s="1">
-        <v>43115</v>
+        <v>43480</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
@@ -6218,7 +6218,7 @@
         <v>21</v>
       </c>
       <c r="E252" s="1">
-        <v>43115</v>
+        <v>43480</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
@@ -6235,7 +6235,7 @@
         <v>14</v>
       </c>
       <c r="E253" s="1">
-        <v>43116</v>
+        <v>43481</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -6252,7 +6252,7 @@
         <v>21</v>
       </c>
       <c r="E254" s="1">
-        <v>43116</v>
+        <v>43481</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
@@ -6269,7 +6269,7 @@
         <v>14</v>
       </c>
       <c r="E255" s="1">
-        <v>43116</v>
+        <v>43481</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
@@ -6286,7 +6286,7 @@
         <v>33</v>
       </c>
       <c r="E256" s="1">
-        <v>43116</v>
+        <v>43481</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
@@ -6303,7 +6303,7 @@
         <v>61</v>
       </c>
       <c r="E257" s="1">
-        <v>43116</v>
+        <v>43481</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -6320,7 +6320,7 @@
         <v>29</v>
       </c>
       <c r="E258" s="1">
-        <v>43116</v>
+        <v>43481</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
@@ -6337,7 +6337,7 @@
         <v>21</v>
       </c>
       <c r="E259" s="1">
-        <v>43116</v>
+        <v>43481</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -6354,7 +6354,7 @@
         <v>14</v>
       </c>
       <c r="E260" s="1">
-        <v>43116</v>
+        <v>43481</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -6371,7 +6371,7 @@
         <v>21</v>
       </c>
       <c r="E261" s="1">
-        <v>43117</v>
+        <v>43482</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
@@ -6388,7 +6388,7 @@
         <v>29</v>
       </c>
       <c r="E262" s="1">
-        <v>43117</v>
+        <v>43482</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
@@ -6405,7 +6405,7 @@
         <v>14</v>
       </c>
       <c r="E263" s="1">
-        <v>43117</v>
+        <v>43482</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
@@ -6422,7 +6422,7 @@
         <v>105</v>
       </c>
       <c r="E264" s="1">
-        <v>43117</v>
+        <v>43482</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
@@ -6439,7 +6439,7 @@
         <v>21</v>
       </c>
       <c r="E265" s="1">
-        <v>43117</v>
+        <v>43482</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
@@ -6456,7 +6456,7 @@
         <v>14</v>
       </c>
       <c r="E266" s="1">
-        <v>43117</v>
+        <v>43482</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
@@ -6473,7 +6473,7 @@
         <v>21</v>
       </c>
       <c r="E267" s="1">
-        <v>43117</v>
+        <v>43482</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
@@ -6490,7 +6490,7 @@
         <v>95</v>
       </c>
       <c r="E268" s="1">
-        <v>43117</v>
+        <v>43482</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
@@ -6507,7 +6507,7 @@
         <v>21</v>
       </c>
       <c r="E269" s="1">
-        <v>43118</v>
+        <v>43483</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
@@ -6524,7 +6524,7 @@
         <v>21</v>
       </c>
       <c r="E270" s="1">
-        <v>43118</v>
+        <v>43483</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
@@ -6541,7 +6541,7 @@
         <v>21</v>
       </c>
       <c r="E271" s="1">
-        <v>43118</v>
+        <v>43483</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
@@ -6558,7 +6558,7 @@
         <v>14</v>
       </c>
       <c r="E272" s="1">
-        <v>43118</v>
+        <v>43483</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
@@ -6575,7 +6575,7 @@
         <v>8</v>
       </c>
       <c r="E273" s="1">
-        <v>43118</v>
+        <v>43483</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
@@ -6592,7 +6592,7 @@
         <v>21</v>
       </c>
       <c r="E274" s="1">
-        <v>43118</v>
+        <v>43483</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
@@ -6609,7 +6609,7 @@
         <v>21</v>
       </c>
       <c r="E275" s="1">
-        <v>43118</v>
+        <v>43483</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
@@ -6626,7 +6626,7 @@
         <v>95</v>
       </c>
       <c r="E276" s="1">
-        <v>43118</v>
+        <v>43483</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
@@ -6643,7 +6643,7 @@
         <v>14</v>
       </c>
       <c r="E277" s="1">
-        <v>43121</v>
+        <v>43486</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
@@ -6660,7 +6660,7 @@
         <v>14</v>
       </c>
       <c r="E278" s="1">
-        <v>43121</v>
+        <v>43486</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
@@ -6677,7 +6677,7 @@
         <v>29</v>
       </c>
       <c r="E279" s="1">
-        <v>43121</v>
+        <v>43486</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.25">
@@ -6694,7 +6694,7 @@
         <v>14</v>
       </c>
       <c r="E280" s="1">
-        <v>43121</v>
+        <v>43486</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
@@ -6711,7 +6711,7 @@
         <v>33</v>
       </c>
       <c r="E281" s="1">
-        <v>43121</v>
+        <v>43486</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
@@ -6728,7 +6728,7 @@
         <v>14</v>
       </c>
       <c r="E282" s="1">
-        <v>43121</v>
+        <v>43486</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
@@ -6745,7 +6745,7 @@
         <v>21</v>
       </c>
       <c r="E283" s="1">
-        <v>43121</v>
+        <v>43486</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
@@ -6762,7 +6762,7 @@
         <v>21</v>
       </c>
       <c r="E284" s="1">
-        <v>43121</v>
+        <v>43486</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
@@ -6779,7 +6779,7 @@
         <v>105</v>
       </c>
       <c r="E285" s="1">
-        <v>43122</v>
+        <v>43487</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
@@ -6796,7 +6796,7 @@
         <v>14</v>
       </c>
       <c r="E286" s="1">
-        <v>43122</v>
+        <v>43487</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
@@ -6813,7 +6813,7 @@
         <v>11</v>
       </c>
       <c r="E287" s="1">
-        <v>43122</v>
+        <v>43487</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
@@ -6830,7 +6830,7 @@
         <v>105</v>
       </c>
       <c r="E288" s="1">
-        <v>43122</v>
+        <v>43487</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
@@ -6847,7 +6847,7 @@
         <v>11</v>
       </c>
       <c r="E289" s="1">
-        <v>43122</v>
+        <v>43487</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -6864,7 +6864,7 @@
         <v>21</v>
       </c>
       <c r="E290" s="1">
-        <v>43122</v>
+        <v>43487</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
@@ -6881,7 +6881,7 @@
         <v>105</v>
       </c>
       <c r="E291" s="1">
-        <v>43122</v>
+        <v>43487</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -6898,7 +6898,7 @@
         <v>105</v>
       </c>
       <c r="E292" s="1">
-        <v>43122</v>
+        <v>43487</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
@@ -6915,7 +6915,7 @@
         <v>14</v>
       </c>
       <c r="E293" s="1">
-        <v>43123</v>
+        <v>43488</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
@@ -6932,7 +6932,7 @@
         <v>8</v>
       </c>
       <c r="E294" s="1">
-        <v>43123</v>
+        <v>43488</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
@@ -6949,7 +6949,7 @@
         <v>21</v>
       </c>
       <c r="E295" s="1">
-        <v>43123</v>
+        <v>43488</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
@@ -6966,7 +6966,7 @@
         <v>21</v>
       </c>
       <c r="E296" s="1">
-        <v>43123</v>
+        <v>43488</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
@@ -6983,7 +6983,7 @@
         <v>33</v>
       </c>
       <c r="E297" s="1">
-        <v>43123</v>
+        <v>43488</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
@@ -7000,7 +7000,7 @@
         <v>14</v>
       </c>
       <c r="E298" s="1">
-        <v>43123</v>
+        <v>43488</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
@@ -7017,7 +7017,7 @@
         <v>21</v>
       </c>
       <c r="E299" s="1">
-        <v>43123</v>
+        <v>43488</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
@@ -7034,7 +7034,7 @@
         <v>21</v>
       </c>
       <c r="E300" s="1">
-        <v>43123</v>
+        <v>43488</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
@@ -7051,7 +7051,7 @@
         <v>95</v>
       </c>
       <c r="E301" s="1">
-        <v>43124</v>
+        <v>43489</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
@@ -7068,7 +7068,7 @@
         <v>14</v>
       </c>
       <c r="E302" s="1">
-        <v>43124</v>
+        <v>43489</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -7085,7 +7085,7 @@
         <v>14</v>
       </c>
       <c r="E303" s="1">
-        <v>43124</v>
+        <v>43489</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
@@ -7102,7 +7102,7 @@
         <v>14</v>
       </c>
       <c r="E304" s="1">
-        <v>43124</v>
+        <v>43489</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
@@ -7119,7 +7119,7 @@
         <v>14</v>
       </c>
       <c r="E305" s="1">
-        <v>43124</v>
+        <v>43489</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
@@ -7136,7 +7136,7 @@
         <v>105</v>
       </c>
       <c r="E306" s="1">
-        <v>43124</v>
+        <v>43489</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
@@ -7153,7 +7153,7 @@
         <v>21</v>
       </c>
       <c r="E307" s="1">
-        <v>43124</v>
+        <v>43489</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
@@ -7170,7 +7170,7 @@
         <v>105</v>
       </c>
       <c r="E308" s="1">
-        <v>43124</v>
+        <v>43489</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
@@ -7187,7 +7187,7 @@
         <v>21</v>
       </c>
       <c r="E309" s="1">
-        <v>43125</v>
+        <v>43490</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
@@ -7204,7 +7204,7 @@
         <v>21</v>
       </c>
       <c r="E310" s="1">
-        <v>43125</v>
+        <v>43490</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
@@ -7221,7 +7221,7 @@
         <v>14</v>
       </c>
       <c r="E311" s="1">
-        <v>43125</v>
+        <v>43490</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">
@@ -7238,7 +7238,7 @@
         <v>21</v>
       </c>
       <c r="E312" s="1">
-        <v>43125</v>
+        <v>43490</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
@@ -7255,7 +7255,7 @@
         <v>105</v>
       </c>
       <c r="E313" s="1">
-        <v>43125</v>
+        <v>43490</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.25">
@@ -7272,7 +7272,7 @@
         <v>14</v>
       </c>
       <c r="E314" s="1">
-        <v>43125</v>
+        <v>43490</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
@@ -7289,7 +7289,7 @@
         <v>21</v>
       </c>
       <c r="E315" s="1">
-        <v>43125</v>
+        <v>43490</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
@@ -7306,7 +7306,7 @@
         <v>95</v>
       </c>
       <c r="E316" s="1">
-        <v>43125</v>
+        <v>43490</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected bug where bench dollars weren't being counted
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DC2BEF-3EBA-4D08-BABD-A2B1B08086AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE8D09F-3216-44EA-933B-6498BDAC448F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1963,8 +1963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A308" workbookViewId="0">
-      <selection activeCell="E318" sqref="E318:E324"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
close to end of auction
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA1E302-8380-4335-AA0F-68270A07BAC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BF2203-7830-41CB-86F9-A5A9F0B9EE53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="503">
   <si>
     <t>team</t>
   </si>
@@ -1483,6 +1483,60 @@
   </si>
   <si>
     <t>Chris Paddack</t>
+  </si>
+  <si>
+    <t>Eduardo Nunez</t>
+  </si>
+  <si>
+    <t>Scott Schebler</t>
+  </si>
+  <si>
+    <t>Mike Minor</t>
+  </si>
+  <si>
+    <t>Jace Fry</t>
+  </si>
+  <si>
+    <t>Jay Bruce</t>
+  </si>
+  <si>
+    <t>Matt Kemp</t>
+  </si>
+  <si>
+    <t>Nick Hundley</t>
+  </si>
+  <si>
+    <t>Mitch Keller</t>
+  </si>
+  <si>
+    <t>Raimel Tapia</t>
+  </si>
+  <si>
+    <t>Orlando Arcia</t>
+  </si>
+  <si>
+    <t>Jeff McNeil</t>
+  </si>
+  <si>
+    <t>Bradley Zimmer</t>
+  </si>
+  <si>
+    <t>Mike Fiers</t>
+  </si>
+  <si>
+    <t>Todd Frazier</t>
+  </si>
+  <si>
+    <t>Fernando Romero</t>
+  </si>
+  <si>
+    <t>Greg Allen</t>
+  </si>
+  <si>
+    <t>Matt Duffy</t>
+  </si>
+  <si>
+    <t>Elias Diaz</t>
   </si>
 </sst>
 </file>
@@ -2331,10 +2385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E452"/>
+  <dimension ref="A1:E470"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A422" workbookViewId="0">
-      <selection activeCell="B452" sqref="B452"/>
+    <sheetView tabSelected="1" topLeftCell="A446" workbookViewId="0">
+      <selection activeCell="D461" sqref="D461"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10026,6 +10080,312 @@
         <v>21</v>
       </c>
       <c r="E452" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="453" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
+        <v>37</v>
+      </c>
+      <c r="B453" t="s">
+        <v>485</v>
+      </c>
+      <c r="C453" s="2">
+        <v>1</v>
+      </c>
+      <c r="D453" t="s">
+        <v>33</v>
+      </c>
+      <c r="E453" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="454" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
+        <v>24</v>
+      </c>
+      <c r="B454" t="s">
+        <v>486</v>
+      </c>
+      <c r="C454" s="2">
+        <v>1</v>
+      </c>
+      <c r="D454" t="s">
+        <v>14</v>
+      </c>
+      <c r="E454" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="455" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>45</v>
+      </c>
+      <c r="B455" t="s">
+        <v>487</v>
+      </c>
+      <c r="C455" s="2">
+        <v>1</v>
+      </c>
+      <c r="D455" t="s">
+        <v>21</v>
+      </c>
+      <c r="E455" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="456" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>5</v>
+      </c>
+      <c r="B456" t="s">
+        <v>488</v>
+      </c>
+      <c r="C456" s="2">
+        <v>1</v>
+      </c>
+      <c r="D456" t="s">
+        <v>21</v>
+      </c>
+      <c r="E456" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="457" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>39</v>
+      </c>
+      <c r="B457" t="s">
+        <v>489</v>
+      </c>
+      <c r="C457" s="2">
+        <v>3</v>
+      </c>
+      <c r="D457" t="s">
+        <v>14</v>
+      </c>
+      <c r="E457" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="458" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>26</v>
+      </c>
+      <c r="B458" t="s">
+        <v>490</v>
+      </c>
+      <c r="C458" s="2">
+        <v>2</v>
+      </c>
+      <c r="D458" t="s">
+        <v>228</v>
+      </c>
+      <c r="E458" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="459" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>43</v>
+      </c>
+      <c r="B459" t="s">
+        <v>502</v>
+      </c>
+      <c r="C459" s="2">
+        <v>1</v>
+      </c>
+      <c r="D459" t="s">
+        <v>105</v>
+      </c>
+      <c r="E459" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="460" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>19</v>
+      </c>
+      <c r="B460" t="s">
+        <v>491</v>
+      </c>
+      <c r="C460" s="2">
+        <v>1</v>
+      </c>
+      <c r="D460" t="s">
+        <v>105</v>
+      </c>
+      <c r="E460" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="461" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>39</v>
+      </c>
+      <c r="B461" t="s">
+        <v>492</v>
+      </c>
+      <c r="C461" s="2">
+        <v>3</v>
+      </c>
+      <c r="D461" t="s">
+        <v>21</v>
+      </c>
+      <c r="E461" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="462" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>24</v>
+      </c>
+      <c r="B462" t="s">
+        <v>501</v>
+      </c>
+      <c r="C462" s="2">
+        <v>1</v>
+      </c>
+      <c r="D462" t="s">
+        <v>11</v>
+      </c>
+      <c r="E462" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="463" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>5</v>
+      </c>
+      <c r="B463" t="s">
+        <v>493</v>
+      </c>
+      <c r="C463" s="2">
+        <v>1</v>
+      </c>
+      <c r="D463" t="s">
+        <v>228</v>
+      </c>
+      <c r="E463" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="464" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>39</v>
+      </c>
+      <c r="B464" t="s">
+        <v>494</v>
+      </c>
+      <c r="C464" s="2">
+        <v>1</v>
+      </c>
+      <c r="D464" t="s">
+        <v>95</v>
+      </c>
+      <c r="E464" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="465" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>43</v>
+      </c>
+      <c r="B465" t="s">
+        <v>495</v>
+      </c>
+      <c r="C465" s="2">
+        <v>2</v>
+      </c>
+      <c r="D465" t="s">
+        <v>228</v>
+      </c>
+      <c r="E465" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="466" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>43</v>
+      </c>
+      <c r="B466" t="s">
+        <v>496</v>
+      </c>
+      <c r="C466" s="2">
+        <v>1</v>
+      </c>
+      <c r="D466" t="s">
+        <v>14</v>
+      </c>
+      <c r="E466" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="467" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>37</v>
+      </c>
+      <c r="B467" t="s">
+        <v>497</v>
+      </c>
+      <c r="C467" s="2">
+        <v>1</v>
+      </c>
+      <c r="D467" t="s">
+        <v>21</v>
+      </c>
+      <c r="E467" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="468" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>24</v>
+      </c>
+      <c r="B468" t="s">
+        <v>498</v>
+      </c>
+      <c r="C468" s="2">
+        <v>1</v>
+      </c>
+      <c r="D468" t="s">
+        <v>33</v>
+      </c>
+      <c r="E468" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="469" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>5</v>
+      </c>
+      <c r="B469" t="s">
+        <v>499</v>
+      </c>
+      <c r="C469" s="2">
+        <v>1</v>
+      </c>
+      <c r="D469" t="s">
+        <v>21</v>
+      </c>
+      <c r="E469" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="470" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>39</v>
+      </c>
+      <c r="B470" t="s">
+        <v>500</v>
+      </c>
+      <c r="C470" s="2">
+        <v>1</v>
+      </c>
+      <c r="D470" t="s">
+        <v>14</v>
+      </c>
+      <c r="E470" s="1">
         <v>43515</v>
       </c>
     </row>

</xml_diff>

<commit_message>
end of bench draft
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BF2203-7830-41CB-86F9-A5A9F0B9EE53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429AFEEC-CC83-4888-95DA-84BA5385D8C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="507">
   <si>
     <t>team</t>
   </si>
@@ -1537,6 +1537,18 @@
   </si>
   <si>
     <t>Elias Diaz</t>
+  </si>
+  <si>
+    <t>Casey Mize</t>
+  </si>
+  <si>
+    <t>Mark Melancon </t>
+  </si>
+  <si>
+    <t>Victor Mesa</t>
+  </si>
+  <si>
+    <t>Josh Harrison</t>
   </si>
 </sst>
 </file>
@@ -2385,10 +2397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E470"/>
+  <dimension ref="A1:E474"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A446" workbookViewId="0">
-      <selection activeCell="D461" sqref="D461"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="D199" sqref="D199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5776,7 +5788,7 @@
         <v>7</v>
       </c>
       <c r="D199" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E199" s="1">
         <v>43465</v>
@@ -9873,7 +9885,7 @@
         <v>2</v>
       </c>
       <c r="D440" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E440" s="1">
         <v>43514</v>
@@ -9890,7 +9902,7 @@
         <v>1</v>
       </c>
       <c r="D441" t="s">
-        <v>14</v>
+        <v>228</v>
       </c>
       <c r="E441" s="1">
         <v>43514</v>
@@ -10247,7 +10259,7 @@
         <v>1</v>
       </c>
       <c r="D462" t="s">
-        <v>11</v>
+        <v>228</v>
       </c>
       <c r="E462" s="1">
         <v>43515</v>
@@ -10349,7 +10361,7 @@
         <v>1</v>
       </c>
       <c r="D468" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E468" s="1">
         <v>43515</v>
@@ -10383,9 +10395,77 @@
         <v>1</v>
       </c>
       <c r="D470" t="s">
-        <v>14</v>
+        <v>228</v>
       </c>
       <c r="E470" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="471" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>26</v>
+      </c>
+      <c r="B471" t="s">
+        <v>506</v>
+      </c>
+      <c r="C471" s="2">
+        <v>1</v>
+      </c>
+      <c r="D471" t="s">
+        <v>29</v>
+      </c>
+      <c r="E471" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="472" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>43</v>
+      </c>
+      <c r="B472" t="s">
+        <v>505</v>
+      </c>
+      <c r="C472" s="2">
+        <v>1</v>
+      </c>
+      <c r="D472" t="s">
+        <v>14</v>
+      </c>
+      <c r="E472" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="473" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>39</v>
+      </c>
+      <c r="B473" t="s">
+        <v>503</v>
+      </c>
+      <c r="C473" s="2">
+        <v>1</v>
+      </c>
+      <c r="D473" t="s">
+        <v>21</v>
+      </c>
+      <c r="E473" s="1">
+        <v>43515</v>
+      </c>
+    </row>
+    <row r="474" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>43</v>
+      </c>
+      <c r="B474" t="s">
+        <v>504</v>
+      </c>
+      <c r="C474" s="2">
+        <v>1</v>
+      </c>
+      <c r="D474" t="s">
+        <v>21</v>
+      </c>
+      <c r="E474" s="1">
         <v>43515</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more draft picks and work on valuation code
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HRDUser\Desktop\fantasy2020\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="21721"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="13770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8980" windowHeight="13780"/>
   </bookViews>
   <sheets>
     <sheet name="draftpicks" sheetId="1" r:id="rId1"/>
     <sheet name="teams" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="130">
   <si>
     <t>team</t>
   </si>
@@ -255,6 +253,168 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>Nick Madrigal</t>
+  </si>
+  <si>
+    <t>Vladimir Guerrero Jr.</t>
+  </si>
+  <si>
+    <t>Alec Bohm</t>
+  </si>
+  <si>
+    <t>Whit Merrifield</t>
+  </si>
+  <si>
+    <t>Byron Buxton</t>
+  </si>
+  <si>
+    <t>Franmil Reyes</t>
+  </si>
+  <si>
+    <t>Adley Rutschman</t>
+  </si>
+  <si>
+    <t>Royce Lewis</t>
+  </si>
+  <si>
+    <t>Chris Paddack</t>
+  </si>
+  <si>
+    <t>Blake Snell</t>
+  </si>
+  <si>
+    <t>Noah Syndergaard</t>
+  </si>
+  <si>
+    <t>Keston Hiura</t>
+  </si>
+  <si>
+    <t>Miguel Sano</t>
+  </si>
+  <si>
+    <t>Francisco Lindor</t>
+  </si>
+  <si>
+    <t>Kyle Tucker</t>
+  </si>
+  <si>
+    <t>Jarred Kelenic</t>
+  </si>
+  <si>
+    <t>Jose Berrios</t>
+  </si>
+  <si>
+    <t>Shane Bieber</t>
+  </si>
+  <si>
+    <t>Brendan McKay</t>
+  </si>
+  <si>
+    <t>Mike Soroka</t>
+  </si>
+  <si>
+    <t>Hector Neris</t>
+  </si>
+  <si>
+    <t>Mike Moustakas</t>
+  </si>
+  <si>
+    <t>Marcus Semien</t>
+  </si>
+  <si>
+    <t>C.J. Cron</t>
+  </si>
+  <si>
+    <t>Ryan McMahon</t>
+  </si>
+  <si>
+    <t>Seth Beer</t>
+  </si>
+  <si>
+    <t>Jonathan India</t>
+  </si>
+  <si>
+    <t>Mitch Keller</t>
+  </si>
+  <si>
+    <t>Dallas Keuchel</t>
+  </si>
+  <si>
+    <t>Joey Lucchesi</t>
+  </si>
+  <si>
+    <t>Jesus Luzardo</t>
+  </si>
+  <si>
+    <t>MacKenzie Gore</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>Jonathan Villar</t>
+  </si>
+  <si>
+    <t>Joey Gallo</t>
+  </si>
+  <si>
+    <t>Ramon Laureano</t>
+  </si>
+  <si>
+    <t>Danny Santana</t>
+  </si>
+  <si>
+    <t>Luis Robert</t>
+  </si>
+  <si>
+    <t>Kristian Robinson</t>
+  </si>
+  <si>
+    <t>Lance Lynn</t>
+  </si>
+  <si>
+    <t>Eduardo Rodriguez</t>
+  </si>
+  <si>
+    <t>Brandon Woodruff</t>
+  </si>
+  <si>
+    <t>Josh Hader</t>
+  </si>
+  <si>
+    <t>Kirby Yates</t>
+  </si>
+  <si>
+    <t>Howie Kendrick</t>
+  </si>
+  <si>
+    <t>Didi Gregorius</t>
+  </si>
+  <si>
+    <t>Andrew Benintendi</t>
+  </si>
+  <si>
+    <t>Charlie Blackmon</t>
+  </si>
+  <si>
+    <t>Brett Gardner</t>
+  </si>
+  <si>
+    <t>Tommy Pham</t>
+  </si>
+  <si>
+    <t>Yordan Alvarez</t>
+  </si>
+  <si>
+    <t>Marcus Stroman</t>
+  </si>
+  <si>
+    <t>Roberto Osuna</t>
+  </si>
+  <si>
+    <t>Matt Manning</t>
   </si>
 </sst>
 </file>
@@ -262,9 +422,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,6 +564,22 @@
       <color theme="1"/>
       <name val="Material Icons"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -702,7 +878,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -745,17 +921,53 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="78">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -784,11 +996,47 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -855,7 +1103,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -907,7 +1155,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1101,7 +1349,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1109,18 +1357,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F569"/>
+  <dimension ref="A1:F622"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:E25"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
-    <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1550,10 +1798,10 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="C26" s="2">
         <v>5</v>
@@ -1567,16 +1815,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="C27" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="E27" s="1">
         <v>43830</v>
@@ -1584,16 +1832,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="C28" s="2">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E28" s="1">
         <v>43830</v>
@@ -1601,16 +1849,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="C29" s="2">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E29" s="1">
         <v>43830</v>
@@ -1618,16 +1866,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="C30" s="2">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D30" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E30" s="1">
         <v>43830</v>
@@ -1635,16 +1883,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="C31" s="2">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="E31" s="1">
         <v>43830</v>
@@ -1652,16 +1900,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="C32" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="E32" s="1">
         <v>43830</v>
@@ -1669,16 +1917,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="C33" s="2">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="E33" s="1">
         <v>43830</v>
@@ -1686,16 +1934,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="C34" s="2">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="E34" s="1">
         <v>43830</v>
@@ -1703,16 +1951,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C35" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E35" s="1">
         <v>43830</v>
@@ -1720,16 +1968,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="C36" s="2">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D36" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="E36" s="1">
         <v>43830</v>
@@ -1737,13 +1985,13 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C37" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D37" t="s">
         <v>37</v>
@@ -1754,16 +2002,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="C38" s="2">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E38" s="1">
         <v>43830</v>
@@ -1771,16 +2019,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="C39" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E39" s="1">
         <v>43830</v>
@@ -1788,33 +2036,939 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="2">
+        <v>22</v>
+      </c>
+      <c r="D40" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" s="2">
         <v>5</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="D41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>75</v>
+      </c>
+      <c r="E42" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="2">
+        <v>17</v>
+      </c>
+      <c r="D43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="2">
+        <v>17</v>
+      </c>
+      <c r="D44" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="2">
+        <v>9</v>
+      </c>
+      <c r="D45" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="2">
+        <v>10</v>
+      </c>
+      <c r="D46" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="2">
+        <v>5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="2">
+        <v>8</v>
+      </c>
+      <c r="D48" t="s">
+        <v>37</v>
+      </c>
+      <c r="E48" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="2">
+        <v>23</v>
+      </c>
+      <c r="D49" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="2">
+        <v>13</v>
+      </c>
+      <c r="D50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="2">
+        <v>9</v>
+      </c>
+      <c r="D51" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>30</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="2">
+        <v>8</v>
+      </c>
+      <c r="D52" t="s">
+        <v>108</v>
+      </c>
+      <c r="E52" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>30</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" s="2">
+        <v>5</v>
+      </c>
+      <c r="D53" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>30</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0</v>
+      </c>
+      <c r="D54" t="s">
+        <v>75</v>
+      </c>
+      <c r="E54" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>30</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" s="2">
+        <v>7</v>
+      </c>
+      <c r="D55" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>30</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C56" s="2">
+        <v>20</v>
+      </c>
+      <c r="D56" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>30</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C57" s="2">
+        <v>9</v>
+      </c>
+      <c r="D57" t="s">
+        <v>18</v>
+      </c>
+      <c r="E57" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>30</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C58" s="2">
+        <v>14</v>
+      </c>
+      <c r="D58" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C59" s="2">
+        <v>0</v>
+      </c>
+      <c r="D59" t="s">
+        <v>75</v>
+      </c>
+      <c r="E59" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60" s="2">
+        <v>11</v>
+      </c>
+      <c r="D60" t="s">
+        <v>23</v>
+      </c>
+      <c r="E60" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C61" s="2">
+        <v>17</v>
+      </c>
+      <c r="D61" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C62" s="2">
+        <v>17</v>
+      </c>
+      <c r="D62" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C63" s="2">
+        <v>12</v>
+      </c>
+      <c r="D63" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C64" s="2">
+        <v>6</v>
+      </c>
+      <c r="D64" t="s">
+        <v>13</v>
+      </c>
+      <c r="E64" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C65" s="2">
+        <v>0</v>
+      </c>
+      <c r="D65" t="s">
+        <v>75</v>
+      </c>
+      <c r="E65" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>60</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C66" s="2">
+        <v>0</v>
+      </c>
+      <c r="D66" t="s">
+        <v>75</v>
+      </c>
+      <c r="E66" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>60</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C67" s="2">
+        <v>5</v>
+      </c>
+      <c r="D67" t="s">
+        <v>18</v>
+      </c>
+      <c r="E67" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>60</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C68" s="2">
+        <v>12</v>
+      </c>
+      <c r="D68" t="s">
+        <v>18</v>
+      </c>
+      <c r="E68" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>60</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C69" s="2">
+        <v>10</v>
+      </c>
+      <c r="D69" t="s">
+        <v>18</v>
+      </c>
+      <c r="E69" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>60</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C70" s="2">
+        <v>13</v>
+      </c>
+      <c r="D70" t="s">
+        <v>18</v>
+      </c>
+      <c r="E70" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>60</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C71" s="2">
+        <v>9</v>
+      </c>
+      <c r="D71" t="s">
+        <v>18</v>
+      </c>
+      <c r="E71" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>21</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C72" s="2">
+        <v>11</v>
+      </c>
+      <c r="D72" t="s">
+        <v>33</v>
+      </c>
+      <c r="E72" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>21</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C73" s="2">
+        <v>7</v>
+      </c>
+      <c r="D73" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>21</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C74" s="2">
+        <v>16</v>
+      </c>
+      <c r="D74" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>21</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C75" s="2">
+        <v>12</v>
+      </c>
+      <c r="D75" t="s">
+        <v>13</v>
+      </c>
+      <c r="E75" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>21</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C76" s="2">
+        <v>27</v>
+      </c>
+      <c r="D76" t="s">
+        <v>13</v>
+      </c>
+      <c r="E76" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>21</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C77" s="2">
+        <v>6</v>
+      </c>
+      <c r="D77" t="s">
+        <v>13</v>
+      </c>
+      <c r="E77" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>21</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C78" s="2">
+        <v>26</v>
+      </c>
+      <c r="D78" t="s">
+        <v>13</v>
+      </c>
+      <c r="E78" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>21</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C79" s="2">
+        <v>5</v>
+      </c>
+      <c r="D79" t="s">
+        <v>44</v>
+      </c>
+      <c r="E79" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>21</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C80" s="2">
+        <v>6</v>
+      </c>
+      <c r="D80" t="s">
+        <v>18</v>
+      </c>
+      <c r="E80" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>21</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C81" s="2">
+        <v>23</v>
+      </c>
+      <c r="D81" t="s">
+        <v>18</v>
+      </c>
+      <c r="E81" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>21</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C82" s="2">
+        <v>0</v>
+      </c>
+      <c r="D82" t="s">
+        <v>75</v>
+      </c>
+      <c r="E82" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>20</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C83" s="2">
+        <v>5</v>
+      </c>
+      <c r="D83" t="s">
+        <v>23</v>
+      </c>
+      <c r="E83" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>61</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C84" s="2">
+        <v>5</v>
+      </c>
+      <c r="D84" t="s">
+        <v>37</v>
+      </c>
+      <c r="E84" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>16</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C85" s="2">
+        <v>5</v>
+      </c>
+      <c r="D85" t="s">
+        <v>33</v>
+      </c>
+      <c r="E85" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>14</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C86" s="2">
+        <v>17</v>
+      </c>
+      <c r="D86" t="s">
+        <v>10</v>
+      </c>
+      <c r="E86" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>11</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C87" s="2">
+        <v>12</v>
+      </c>
+      <c r="D87" t="s">
+        <v>33</v>
+      </c>
+      <c r="E87" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>29</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C88" s="2">
+        <v>24</v>
+      </c>
+      <c r="D88" t="s">
+        <v>37</v>
+      </c>
+      <c r="E88" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>62</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C89" s="2">
+        <v>5</v>
+      </c>
+      <c r="D89" t="s">
+        <v>33</v>
+      </c>
+      <c r="E89" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>9</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C90" s="2">
+        <v>6</v>
+      </c>
+      <c r="D90" t="s">
+        <v>37</v>
+      </c>
+      <c r="E90" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>28</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C91" s="2">
+        <v>12</v>
+      </c>
+      <c r="D91" t="s">
+        <v>10</v>
+      </c>
+      <c r="E91" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>27</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C92" s="2">
+        <v>13</v>
+      </c>
+      <c r="D92" t="s">
+        <v>33</v>
+      </c>
+      <c r="E92" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C93" s="2">
         <v>12</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D93" t="s">
         <v>23</v>
       </c>
-      <c r="E40" s="1">
-        <v>43830</v>
-      </c>
-    </row>
-    <row r="53" ht="16.5" customHeight="1"/>
-    <row r="95" ht="24" customHeight="1"/>
-    <row r="202" ht="15.75" customHeight="1"/>
-    <row r="569" spans="6:6">
-      <c r="F569" s="4"/>
+      <c r="E93" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="106" ht="16.5" customHeight="1"/>
+    <row r="148" ht="24" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="622" spans="6:6" ht="15">
+      <c r="F622" s="4"/>
     </row>
   </sheetData>
   <sortState ref="A261:E276">
     <sortCondition ref="E261:E276"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1826,7 +2980,7 @@
       <selection sqref="A1:A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -1920,5 +3074,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed some bugs, added keepers:
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="250">
   <si>
     <t>team</t>
   </si>
@@ -415,6 +415,366 @@
   </si>
   <si>
     <t>Matt Manning</t>
+  </si>
+  <si>
+    <t>Nolan Arenado</t>
+  </si>
+  <si>
+    <t>Xander Bogaerts</t>
+  </si>
+  <si>
+    <t>Corey Seager</t>
+  </si>
+  <si>
+    <t>David Fletcher</t>
+  </si>
+  <si>
+    <t>Mookie Betts</t>
+  </si>
+  <si>
+    <t>Avisail Garcia</t>
+  </si>
+  <si>
+    <t>Miguel Andujar</t>
+  </si>
+  <si>
+    <t>Frankie Montas</t>
+  </si>
+  <si>
+    <t>Luis Severino</t>
+  </si>
+  <si>
+    <t>Vidal Brujan</t>
+  </si>
+  <si>
+    <t>Triston Casas</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>Michael Chavis</t>
+  </si>
+  <si>
+    <t>Tommy Edman</t>
+  </si>
+  <si>
+    <t>Dansby Swanson</t>
+  </si>
+  <si>
+    <t>Javier Baez</t>
+  </si>
+  <si>
+    <t>Max Kepler</t>
+  </si>
+  <si>
+    <t>Nolan Gorman</t>
+  </si>
+  <si>
+    <t>Lucas Giolito</t>
+  </si>
+  <si>
+    <t>Julio Urias</t>
+  </si>
+  <si>
+    <t>Luke Weaver</t>
+  </si>
+  <si>
+    <t>Archie Bradley</t>
+  </si>
+  <si>
+    <t>Sixto Sanchez</t>
+  </si>
+  <si>
+    <t>Yuli Gurriel</t>
+  </si>
+  <si>
+    <t>Paul DeJong</t>
+  </si>
+  <si>
+    <t>Nick Ahmed</t>
+  </si>
+  <si>
+    <t>Mark Canha</t>
+  </si>
+  <si>
+    <t>Yoenis Cespedes</t>
+  </si>
+  <si>
+    <t>Lourdes Gurriel Jr.</t>
+  </si>
+  <si>
+    <t>Daulton Varsho</t>
+  </si>
+  <si>
+    <t>Sonny Gray</t>
+  </si>
+  <si>
+    <t>Stephen Strasburg</t>
+  </si>
+  <si>
+    <t>Justin Verlander</t>
+  </si>
+  <si>
+    <t>Trea Turner</t>
+  </si>
+  <si>
+    <t>Cavan Biggio</t>
+  </si>
+  <si>
+    <t>Hunter Dozier</t>
+  </si>
+  <si>
+    <t>Christian Yelich</t>
+  </si>
+  <si>
+    <t>Luis Castillo</t>
+  </si>
+  <si>
+    <t>Mike Clevinger</t>
+  </si>
+  <si>
+    <t>Charlie Morton</t>
+  </si>
+  <si>
+    <t>Sean Doolittle</t>
+  </si>
+  <si>
+    <t>Emilio Pagan</t>
+  </si>
+  <si>
+    <t>Luis Patino</t>
+  </si>
+  <si>
+    <t>Jose Ramirez</t>
+  </si>
+  <si>
+    <t>Elvis Andrus</t>
+  </si>
+  <si>
+    <t>Fernando Tatis Jr.</t>
+  </si>
+  <si>
+    <t>Austin Meadows</t>
+  </si>
+  <si>
+    <t>George Springer</t>
+  </si>
+  <si>
+    <t>Marco Luciano</t>
+  </si>
+  <si>
+    <t>Monte Harrison</t>
+  </si>
+  <si>
+    <t>Gerrit Cole</t>
+  </si>
+  <si>
+    <t>Patrick Corbin</t>
+  </si>
+  <si>
+    <t>German Marquez</t>
+  </si>
+  <si>
+    <t>Alex Colome</t>
+  </si>
+  <si>
+    <t>Matt Olson</t>
+  </si>
+  <si>
+    <t>Yandy Diaz</t>
+  </si>
+  <si>
+    <t>Carlos Correa</t>
+  </si>
+  <si>
+    <t>J.D. Davis</t>
+  </si>
+  <si>
+    <t>J.D. Martinez</t>
+  </si>
+  <si>
+    <t>Victor Robles</t>
+  </si>
+  <si>
+    <t>Griffin Canning</t>
+  </si>
+  <si>
+    <t>Carlos Carrasco</t>
+  </si>
+  <si>
+    <t>Taylor Rogers</t>
+  </si>
+  <si>
+    <t>Michael Kopech</t>
+  </si>
+  <si>
+    <t>Casey Mize</t>
+  </si>
+  <si>
+    <t>Nate Lowe</t>
+  </si>
+  <si>
+    <t>Anthony Rendon</t>
+  </si>
+  <si>
+    <t>Tim Anderson</t>
+  </si>
+  <si>
+    <t>Brian Anderson</t>
+  </si>
+  <si>
+    <t>Aaron Hicks</t>
+  </si>
+  <si>
+    <t>Austin Riley</t>
+  </si>
+  <si>
+    <t>Matthew Boyd</t>
+  </si>
+  <si>
+    <t>Mike Minor</t>
+  </si>
+  <si>
+    <t>Robbie Ray</t>
+  </si>
+  <si>
+    <t>Ian Anderson</t>
+  </si>
+  <si>
+    <t>Nate Pearson</t>
+  </si>
+  <si>
+    <t>Christian Walker</t>
+  </si>
+  <si>
+    <t>DJ LeMahieu</t>
+  </si>
+  <si>
+    <t>Gio Urshela</t>
+  </si>
+  <si>
+    <t>Cody Bellinger</t>
+  </si>
+  <si>
+    <t>Alex Verdugo</t>
+  </si>
+  <si>
+    <t>Mike Yastrzemski</t>
+  </si>
+  <si>
+    <t>Keibert Ruiz</t>
+  </si>
+  <si>
+    <t>Gavin Lux</t>
+  </si>
+  <si>
+    <t>Walker Buehler</t>
+  </si>
+  <si>
+    <t>Hyun-Jin Ryu</t>
+  </si>
+  <si>
+    <t>Brandon Workman</t>
+  </si>
+  <si>
+    <t>Trevor Story</t>
+  </si>
+  <si>
+    <t>Alex Bregman</t>
+  </si>
+  <si>
+    <t>Aaron Judge</t>
+  </si>
+  <si>
+    <t>Juan Soto</t>
+  </si>
+  <si>
+    <t>Wander Franco</t>
+  </si>
+  <si>
+    <t>Jo Adell</t>
+  </si>
+  <si>
+    <t>Trevor Bauer</t>
+  </si>
+  <si>
+    <t>Jacob deGrom</t>
+  </si>
+  <si>
+    <t>Jack Flaherty</t>
+  </si>
+  <si>
+    <t>Lance McCullers</t>
+  </si>
+  <si>
+    <t>Jose Leclerc</t>
+  </si>
+  <si>
+    <t>Kevin Newman</t>
+  </si>
+  <si>
+    <t>Max Muncy</t>
+  </si>
+  <si>
+    <t>Bo Bichette</t>
+  </si>
+  <si>
+    <t>Brandon Lowe</t>
+  </si>
+  <si>
+    <t>Scott Kingery</t>
+  </si>
+  <si>
+    <t>Ronald Acuna Jr.</t>
+  </si>
+  <si>
+    <t>Jeff McNeil</t>
+  </si>
+  <si>
+    <t>Bryan Reynolds</t>
+  </si>
+  <si>
+    <t>Mike Trout</t>
+  </si>
+  <si>
+    <t>Xavier Edwards</t>
+  </si>
+  <si>
+    <t>Alex Kirilloff</t>
+  </si>
+  <si>
+    <t>Adalberto Mondesi</t>
+  </si>
+  <si>
+    <t>Aristides Aquino</t>
+  </si>
+  <si>
+    <t>Willie Calhoun</t>
+  </si>
+  <si>
+    <t>Oscar Mercado</t>
+  </si>
+  <si>
+    <t>Eddie Rosario</t>
+  </si>
+  <si>
+    <t>Nick Senzel</t>
+  </si>
+  <si>
+    <t>Andrew Vaughn</t>
+  </si>
+  <si>
+    <t>Carter Kieboom</t>
+  </si>
+  <si>
+    <t>Tyler Glasnow</t>
+  </si>
+  <si>
+    <t>Dinelson Lamet</t>
+  </si>
+  <si>
+    <t>James Paxton</t>
   </si>
 </sst>
 </file>
@@ -422,7 +782,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -878,7 +1238,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="78">
+  <cellStyleXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -957,17 +1317,91 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="78">
+  <cellStyles count="152">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1014,6 +1448,43 @@
     <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1037,6 +1508,43 @@
     <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1357,17 +1865,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F622"/>
+  <dimension ref="A1:F729"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="D212" sqref="D212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="26.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="4"/>
     <col min="5" max="5" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1375,10 +1883,10 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -1392,10 +1900,10 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="4">
         <v>19</v>
       </c>
       <c r="D2" t="s">
@@ -1409,10 +1917,10 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="4">
         <v>12</v>
       </c>
       <c r="D3" t="s">
@@ -1426,10 +1934,10 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <v>12</v>
       </c>
       <c r="D4" t="s">
@@ -1443,10 +1951,10 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="4">
         <v>12</v>
       </c>
       <c r="D5" t="s">
@@ -1460,10 +1968,10 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="4">
         <v>11</v>
       </c>
       <c r="D6" t="s">
@@ -1477,10 +1985,10 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="4">
         <v>9</v>
       </c>
       <c r="D7" t="s">
@@ -1494,10 +2002,10 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="4">
         <v>22</v>
       </c>
       <c r="D8" t="s">
@@ -1511,10 +2019,10 @@
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="4">
         <v>8</v>
       </c>
       <c r="D9" t="s">
@@ -1528,10 +2036,10 @@
       <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="4">
         <v>5</v>
       </c>
       <c r="D10" t="s">
@@ -1545,10 +2053,10 @@
       <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="4">
         <v>9</v>
       </c>
       <c r="D11" t="s">
@@ -1562,10 +2070,10 @@
       <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="4">
         <v>0</v>
       </c>
       <c r="D12" t="s">
@@ -1579,10 +2087,10 @@
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="4">
         <v>8</v>
       </c>
       <c r="D13" t="s">
@@ -1596,10 +2104,10 @@
       <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="4">
         <v>8</v>
       </c>
       <c r="D14" t="s">
@@ -1613,10 +2121,10 @@
       <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="4">
         <v>9</v>
       </c>
       <c r="D15" t="s">
@@ -1630,10 +2138,10 @@
       <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="4">
         <v>12</v>
       </c>
       <c r="D16" t="s">
@@ -1647,10 +2155,10 @@
       <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="4">
         <v>16</v>
       </c>
       <c r="D17" t="s">
@@ -1664,10 +2172,10 @@
       <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="4">
         <v>7</v>
       </c>
       <c r="D18" t="s">
@@ -1681,10 +2189,10 @@
       <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="4">
         <v>22</v>
       </c>
       <c r="D19" t="s">
@@ -1698,10 +2206,10 @@
       <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="4">
         <v>0</v>
       </c>
       <c r="D20" t="s">
@@ -1715,10 +2223,10 @@
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="4">
         <v>13</v>
       </c>
       <c r="D21" t="s">
@@ -1732,10 +2240,10 @@
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="4">
         <v>7</v>
       </c>
       <c r="D22" t="s">
@@ -1749,10 +2257,10 @@
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="4">
         <v>12</v>
       </c>
       <c r="D23" t="s">
@@ -1766,10 +2274,10 @@
       <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="4">
         <v>1</v>
       </c>
       <c r="D24" t="s">
@@ -1783,10 +2291,10 @@
       <c r="A25" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="4">
         <v>17</v>
       </c>
       <c r="D25" t="s">
@@ -1800,10 +2308,10 @@
       <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="4">
         <v>5</v>
       </c>
       <c r="D26" t="s">
@@ -1817,10 +2325,10 @@
       <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="4">
         <v>5</v>
       </c>
       <c r="D27" t="s">
@@ -1834,10 +2342,10 @@
       <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="4">
         <v>5</v>
       </c>
       <c r="D28" t="s">
@@ -1851,10 +2359,10 @@
       <c r="A29" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="4">
         <v>22</v>
       </c>
       <c r="D29" t="s">
@@ -1868,10 +2376,10 @@
       <c r="A30" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="4">
         <v>19</v>
       </c>
       <c r="D30" t="s">
@@ -1885,10 +2393,10 @@
       <c r="A31" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="4">
         <v>9</v>
       </c>
       <c r="D31" t="s">
@@ -1902,10 +2410,10 @@
       <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="4">
         <v>0</v>
       </c>
       <c r="D32" t="s">
@@ -1919,10 +2427,10 @@
       <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="4">
         <v>0</v>
       </c>
       <c r="D33" t="s">
@@ -1936,10 +2444,10 @@
       <c r="A34" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="4">
         <v>7</v>
       </c>
       <c r="D34" t="s">
@@ -1953,10 +2461,10 @@
       <c r="A35" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="4">
         <v>23</v>
       </c>
       <c r="D35" t="s">
@@ -1970,10 +2478,10 @@
       <c r="A36" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="4">
         <v>22</v>
       </c>
       <c r="D36" t="s">
@@ -1987,10 +2495,10 @@
       <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="4">
         <v>5</v>
       </c>
       <c r="D37" t="s">
@@ -2004,10 +2512,10 @@
       <c r="A38" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="4">
         <v>5</v>
       </c>
       <c r="D38" t="s">
@@ -2021,10 +2529,10 @@
       <c r="A39" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="4">
         <v>15</v>
       </c>
       <c r="D39" t="s">
@@ -2038,10 +2546,10 @@
       <c r="A40" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="4">
         <v>22</v>
       </c>
       <c r="D40" t="s">
@@ -2055,10 +2563,10 @@
       <c r="A41" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="4">
         <v>5</v>
       </c>
       <c r="D41" t="s">
@@ -2072,10 +2580,10 @@
       <c r="A42" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="4">
         <v>0</v>
       </c>
       <c r="D42" t="s">
@@ -2089,10 +2597,10 @@
       <c r="A43" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="4">
         <v>17</v>
       </c>
       <c r="D43" t="s">
@@ -2106,10 +2614,10 @@
       <c r="A44" t="s">
         <v>36</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="4">
         <v>17</v>
       </c>
       <c r="D44" t="s">
@@ -2123,10 +2631,10 @@
       <c r="A45" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="4">
         <v>9</v>
       </c>
       <c r="D45" t="s">
@@ -2140,10 +2648,10 @@
       <c r="A46" t="s">
         <v>36</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="4">
         <v>10</v>
       </c>
       <c r="D46" t="s">
@@ -2157,10 +2665,10 @@
       <c r="A47" t="s">
         <v>36</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="4">
         <v>5</v>
       </c>
       <c r="D47" t="s">
@@ -2174,10 +2682,10 @@
       <c r="A48" t="s">
         <v>30</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="4">
         <v>8</v>
       </c>
       <c r="D48" t="s">
@@ -2191,10 +2699,10 @@
       <c r="A49" t="s">
         <v>30</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="4">
         <v>23</v>
       </c>
       <c r="D49" t="s">
@@ -2208,10 +2716,10 @@
       <c r="A50" t="s">
         <v>30</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="4">
         <v>13</v>
       </c>
       <c r="D50" t="s">
@@ -2225,10 +2733,10 @@
       <c r="A51" t="s">
         <v>30</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="4">
         <v>9</v>
       </c>
       <c r="D51" t="s">
@@ -2242,10 +2750,10 @@
       <c r="A52" t="s">
         <v>30</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="4">
         <v>8</v>
       </c>
       <c r="D52" t="s">
@@ -2259,10 +2767,10 @@
       <c r="A53" t="s">
         <v>30</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="4">
         <v>5</v>
       </c>
       <c r="D53" t="s">
@@ -2276,10 +2784,10 @@
       <c r="A54" t="s">
         <v>30</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="4">
         <v>0</v>
       </c>
       <c r="D54" t="s">
@@ -2293,10 +2801,10 @@
       <c r="A55" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="4">
         <v>7</v>
       </c>
       <c r="D55" t="s">
@@ -2310,10 +2818,10 @@
       <c r="A56" t="s">
         <v>30</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="4">
         <v>20</v>
       </c>
       <c r="D56" t="s">
@@ -2327,10 +2835,10 @@
       <c r="A57" t="s">
         <v>30</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="4">
         <v>9</v>
       </c>
       <c r="D57" t="s">
@@ -2344,10 +2852,10 @@
       <c r="A58" t="s">
         <v>30</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="4">
         <v>14</v>
       </c>
       <c r="D58" t="s">
@@ -2361,10 +2869,10 @@
       <c r="A59" t="s">
         <v>30</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="4">
         <v>0</v>
       </c>
       <c r="D59" t="s">
@@ -2378,10 +2886,10 @@
       <c r="A60" t="s">
         <v>60</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="4">
         <v>11</v>
       </c>
       <c r="D60" t="s">
@@ -2395,10 +2903,10 @@
       <c r="A61" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="4">
         <v>17</v>
       </c>
       <c r="D61" t="s">
@@ -2412,10 +2920,10 @@
       <c r="A62" t="s">
         <v>60</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="4">
         <v>17</v>
       </c>
       <c r="D62" t="s">
@@ -2429,10 +2937,10 @@
       <c r="A63" t="s">
         <v>60</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="4">
         <v>12</v>
       </c>
       <c r="D63" t="s">
@@ -2446,10 +2954,10 @@
       <c r="A64" t="s">
         <v>60</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="4">
         <v>6</v>
       </c>
       <c r="D64" t="s">
@@ -2463,10 +2971,10 @@
       <c r="A65" t="s">
         <v>60</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65" s="4">
         <v>0</v>
       </c>
       <c r="D65" t="s">
@@ -2480,10 +2988,10 @@
       <c r="A66" t="s">
         <v>60</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66" s="4">
         <v>0</v>
       </c>
       <c r="D66" t="s">
@@ -2497,10 +3005,10 @@
       <c r="A67" t="s">
         <v>60</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67" s="4">
         <v>5</v>
       </c>
       <c r="D67" t="s">
@@ -2514,10 +3022,10 @@
       <c r="A68" t="s">
         <v>60</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68" s="4">
         <v>12</v>
       </c>
       <c r="D68" t="s">
@@ -2531,10 +3039,10 @@
       <c r="A69" t="s">
         <v>60</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69" s="4">
         <v>10</v>
       </c>
       <c r="D69" t="s">
@@ -2548,10 +3056,10 @@
       <c r="A70" t="s">
         <v>60</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70" s="4">
         <v>13</v>
       </c>
       <c r="D70" t="s">
@@ -2565,10 +3073,10 @@
       <c r="A71" t="s">
         <v>60</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71" s="4">
         <v>9</v>
       </c>
       <c r="D71" t="s">
@@ -2582,10 +3090,10 @@
       <c r="A72" t="s">
         <v>21</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72" s="4">
         <v>11</v>
       </c>
       <c r="D72" t="s">
@@ -2599,10 +3107,10 @@
       <c r="A73" t="s">
         <v>21</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C73" s="4">
         <v>7</v>
       </c>
       <c r="D73" t="s">
@@ -2616,10 +3124,10 @@
       <c r="A74" t="s">
         <v>21</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74" s="4">
         <v>16</v>
       </c>
       <c r="D74" t="s">
@@ -2633,10 +3141,10 @@
       <c r="A75" t="s">
         <v>21</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C75" s="2">
+      <c r="C75" s="4">
         <v>12</v>
       </c>
       <c r="D75" t="s">
@@ -2650,10 +3158,10 @@
       <c r="A76" t="s">
         <v>21</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C76" s="4">
         <v>27</v>
       </c>
       <c r="D76" t="s">
@@ -2667,10 +3175,10 @@
       <c r="A77" t="s">
         <v>21</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C77" s="4">
         <v>6</v>
       </c>
       <c r="D77" t="s">
@@ -2684,10 +3192,10 @@
       <c r="A78" t="s">
         <v>21</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C78" s="2">
+      <c r="C78" s="4">
         <v>26</v>
       </c>
       <c r="D78" t="s">
@@ -2701,10 +3209,10 @@
       <c r="A79" t="s">
         <v>21</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C79" s="2">
+      <c r="C79" s="4">
         <v>5</v>
       </c>
       <c r="D79" t="s">
@@ -2718,10 +3226,10 @@
       <c r="A80" t="s">
         <v>21</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C80" s="4">
         <v>6</v>
       </c>
       <c r="D80" t="s">
@@ -2735,10 +3243,10 @@
       <c r="A81" t="s">
         <v>21</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C81" s="2">
+      <c r="C81" s="4">
         <v>23</v>
       </c>
       <c r="D81" t="s">
@@ -2752,10 +3260,10 @@
       <c r="A82" t="s">
         <v>21</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C82" s="2">
+      <c r="C82" s="4">
         <v>0</v>
       </c>
       <c r="D82" t="s">
@@ -2769,10 +3277,10 @@
       <c r="A83" t="s">
         <v>20</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C83" s="2">
+      <c r="C83" s="4">
         <v>5</v>
       </c>
       <c r="D83" t="s">
@@ -2784,16 +3292,16 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>61</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C84" s="2">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C84" s="4">
+        <v>32</v>
       </c>
       <c r="D84" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="E84" s="1">
         <v>43830</v>
@@ -2801,16 +3309,16 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>16</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C85" s="2">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C85" s="4">
+        <v>24</v>
       </c>
       <c r="D85" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="E85" s="1">
         <v>43830</v>
@@ -2818,16 +3326,16 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>14</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C86" s="2">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C86" s="4">
+        <v>19</v>
       </c>
       <c r="D86" t="s">
-        <v>10</v>
+        <v>108</v>
       </c>
       <c r="E86" s="1">
         <v>43830</v>
@@ -2835,16 +3343,16 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>11</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C87" s="2">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C87" s="4">
+        <v>5</v>
       </c>
       <c r="D87" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E87" s="1">
         <v>43830</v>
@@ -2852,16 +3360,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>29</v>
-      </c>
-      <c r="B88" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C88" s="4">
         <v>41</v>
       </c>
-      <c r="C88" s="2">
-        <v>24</v>
-      </c>
       <c r="D88" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="E88" s="1">
         <v>43830</v>
@@ -2869,16 +3377,16 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>62</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C89" s="2">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C89" s="4">
+        <v>12</v>
       </c>
       <c r="D89" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E89" s="1">
         <v>43830</v>
@@ -2886,16 +3394,16 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>9</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C90" s="2">
-        <v>6</v>
+        <v>20</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C90" s="4">
+        <v>10</v>
       </c>
       <c r="D90" t="s">
-        <v>37</v>
+        <v>141</v>
       </c>
       <c r="E90" s="1">
         <v>43830</v>
@@ -2903,16 +3411,16 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>28</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C91" s="2">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C91" s="4">
+        <v>5</v>
       </c>
       <c r="D91" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E91" s="1">
         <v>43830</v>
@@ -2920,16 +3428,16 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>27</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C92" s="2">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C92" s="4">
+        <v>22</v>
       </c>
       <c r="D92" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="E92" s="1">
         <v>43830</v>
@@ -2937,26 +3445,2049 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
+        <v>20</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C93" s="4">
+        <v>0</v>
+      </c>
+      <c r="D93" t="s">
+        <v>75</v>
+      </c>
+      <c r="E93" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>20</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C94" s="4">
+        <v>0</v>
+      </c>
+      <c r="D94" t="s">
+        <v>75</v>
+      </c>
+      <c r="E94" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>61</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C95" s="4">
         <v>5</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="D95" t="s">
+        <v>37</v>
+      </c>
+      <c r="E95" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>61</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C96" s="4">
+        <v>5</v>
+      </c>
+      <c r="D96" t="s">
+        <v>33</v>
+      </c>
+      <c r="E96" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>61</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C97" s="4">
+        <v>7</v>
+      </c>
+      <c r="D97" t="s">
+        <v>23</v>
+      </c>
+      <c r="E97" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>61</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C98" s="4">
+        <v>10</v>
+      </c>
+      <c r="D98" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>61</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C99" s="4">
+        <v>26</v>
+      </c>
+      <c r="D99" t="s">
+        <v>108</v>
+      </c>
+      <c r="E99" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>61</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C100" s="4">
+        <v>18</v>
+      </c>
+      <c r="D100" t="s">
+        <v>13</v>
+      </c>
+      <c r="E100" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>61</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C101" s="4">
+        <v>0</v>
+      </c>
+      <c r="D101" t="s">
+        <v>75</v>
+      </c>
+      <c r="E101" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" t="s">
+        <v>61</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C102" s="4">
+        <v>14</v>
+      </c>
+      <c r="D102" t="s">
+        <v>18</v>
+      </c>
+      <c r="E102" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" t="s">
+        <v>61</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C103" s="4">
+        <v>12</v>
+      </c>
+      <c r="D103" t="s">
+        <v>18</v>
+      </c>
+      <c r="E103" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" t="s">
+        <v>61</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C104" s="4">
+        <v>13</v>
+      </c>
+      <c r="D104" t="s">
+        <v>18</v>
+      </c>
+      <c r="E104" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" t="s">
+        <v>61</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C105" s="4">
+        <v>16</v>
+      </c>
+      <c r="D105" t="s">
+        <v>18</v>
+      </c>
+      <c r="E105" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" t="s">
+        <v>61</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C106" s="4">
+        <v>0</v>
+      </c>
+      <c r="D106" t="s">
+        <v>75</v>
+      </c>
+      <c r="E106" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" t="s">
+        <v>16</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C107" s="4">
+        <v>5</v>
+      </c>
+      <c r="D107" t="s">
+        <v>33</v>
+      </c>
+      <c r="E107" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" t="s">
+        <v>16</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C108" s="4">
+        <v>13</v>
+      </c>
+      <c r="D108" t="s">
+        <v>10</v>
+      </c>
+      <c r="E108" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" t="s">
+        <v>16</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C109" s="4">
+        <v>14</v>
+      </c>
+      <c r="D109" t="s">
+        <v>8</v>
+      </c>
+      <c r="E109" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" t="s">
+        <v>16</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C110" s="4">
+        <v>6</v>
+      </c>
+      <c r="D110" t="s">
+        <v>108</v>
+      </c>
+      <c r="E110" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" t="s">
+        <v>16</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C111" s="4">
+        <v>6</v>
+      </c>
+      <c r="D111" t="s">
+        <v>13</v>
+      </c>
+      <c r="E111" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" t="s">
+        <v>16</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C112" s="4">
+        <v>6</v>
+      </c>
+      <c r="D112" t="s">
+        <v>13</v>
+      </c>
+      <c r="E112" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" t="s">
+        <v>16</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C113" s="4">
+        <v>11</v>
+      </c>
+      <c r="D113" t="s">
+        <v>13</v>
+      </c>
+      <c r="E113" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" t="s">
+        <v>16</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C114" s="4">
+        <v>1</v>
+      </c>
+      <c r="D114" t="s">
+        <v>75</v>
+      </c>
+      <c r="E114" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" t="s">
+        <v>16</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C115" s="4">
+        <v>8</v>
+      </c>
+      <c r="D115" t="s">
+        <v>18</v>
+      </c>
+      <c r="E115" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" t="s">
+        <v>16</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C116" s="4">
+        <v>32</v>
+      </c>
+      <c r="D116" t="s">
+        <v>18</v>
+      </c>
+      <c r="E116" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" t="s">
+        <v>16</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C117" s="4">
+        <v>28</v>
+      </c>
+      <c r="D117" t="s">
+        <v>18</v>
+      </c>
+      <c r="E117" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" t="s">
+        <v>14</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C118" s="4">
+        <v>17</v>
+      </c>
+      <c r="D118" t="s">
+        <v>10</v>
+      </c>
+      <c r="E118" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" t="s">
+        <v>14</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C119" s="4">
+        <v>19</v>
+      </c>
+      <c r="D119" t="s">
+        <v>8</v>
+      </c>
+      <c r="E119" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" t="s">
+        <v>14</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C120" s="4">
+        <v>5</v>
+      </c>
+      <c r="D120" t="s">
+        <v>108</v>
+      </c>
+      <c r="E120" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" t="s">
+        <v>14</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C121" s="4">
+        <v>5</v>
+      </c>
+      <c r="D121" t="s">
+        <v>13</v>
+      </c>
+      <c r="E121" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" t="s">
+        <v>14</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C122" s="4">
+        <v>33</v>
+      </c>
+      <c r="D122" t="s">
+        <v>13</v>
+      </c>
+      <c r="E122" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" t="s">
+        <v>14</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C123" s="4">
+        <v>17</v>
+      </c>
+      <c r="D123" t="s">
+        <v>18</v>
+      </c>
+      <c r="E123" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" t="s">
+        <v>14</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C124" s="4">
+        <v>15</v>
+      </c>
+      <c r="D124" t="s">
+        <v>18</v>
+      </c>
+      <c r="E124" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" t="s">
+        <v>14</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C125" s="4">
+        <v>12</v>
+      </c>
+      <c r="D125" t="s">
+        <v>18</v>
+      </c>
+      <c r="E125" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" t="s">
+        <v>14</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C126" s="4">
+        <v>12</v>
+      </c>
+      <c r="D126" t="s">
+        <v>18</v>
+      </c>
+      <c r="E126" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" t="s">
+        <v>14</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C127" s="4">
+        <v>13</v>
+      </c>
+      <c r="D127" t="s">
+        <v>18</v>
+      </c>
+      <c r="E127" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" t="s">
+        <v>14</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C128" s="4">
+        <v>0</v>
+      </c>
+      <c r="D128" t="s">
+        <v>18</v>
+      </c>
+      <c r="E128" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" t="s">
+        <v>11</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C129" s="4">
+        <v>12</v>
+      </c>
+      <c r="D129" t="s">
+        <v>33</v>
+      </c>
+      <c r="E129" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" t="s">
+        <v>11</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C130" s="4">
+        <v>17</v>
+      </c>
+      <c r="D130" t="s">
+        <v>10</v>
+      </c>
+      <c r="E130" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" t="s">
+        <v>11</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C131" s="4">
+        <v>21</v>
+      </c>
+      <c r="D131" t="s">
+        <v>8</v>
+      </c>
+      <c r="E131" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" t="s">
+        <v>11</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C132" s="4">
+        <v>12</v>
+      </c>
+      <c r="D132" t="s">
+        <v>108</v>
+      </c>
+      <c r="E132" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" t="s">
+        <v>11</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C133" s="4">
+        <v>11</v>
+      </c>
+      <c r="D133" t="s">
+        <v>13</v>
+      </c>
+      <c r="E133" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" t="s">
+        <v>11</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C134" s="4">
+        <v>27</v>
+      </c>
+      <c r="D134" t="s">
+        <v>13</v>
+      </c>
+      <c r="E134" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" t="s">
+        <v>11</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C135" s="4">
+        <v>0</v>
+      </c>
+      <c r="D135" t="s">
+        <v>75</v>
+      </c>
+      <c r="E135" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" t="s">
+        <v>11</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C136" s="4">
+        <v>0</v>
+      </c>
+      <c r="D136" t="s">
+        <v>75</v>
+      </c>
+      <c r="E136" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" t="s">
+        <v>11</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C137" s="4">
+        <v>33</v>
+      </c>
+      <c r="D137" t="s">
+        <v>18</v>
+      </c>
+      <c r="E137" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" t="s">
+        <v>11</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C138" s="4">
+        <v>12</v>
+      </c>
+      <c r="D138" t="s">
+        <v>18</v>
+      </c>
+      <c r="E138" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" t="s">
+        <v>11</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C139" s="4">
+        <v>10</v>
+      </c>
+      <c r="D139" t="s">
+        <v>18</v>
+      </c>
+      <c r="E139" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" t="s">
+        <v>11</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C140" s="4">
+        <v>9</v>
+      </c>
+      <c r="D140" t="s">
+        <v>18</v>
+      </c>
+      <c r="E140" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" t="s">
+        <v>29</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C141" s="4">
+        <v>24</v>
+      </c>
+      <c r="D141" t="s">
+        <v>37</v>
+      </c>
+      <c r="E141" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" t="s">
+        <v>29</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C142" s="4">
+        <v>12</v>
+      </c>
+      <c r="D142" t="s">
+        <v>33</v>
+      </c>
+      <c r="E142" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" t="s">
+        <v>29</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C143" s="4">
+        <v>5</v>
+      </c>
+      <c r="D143" t="s">
+        <v>10</v>
+      </c>
+      <c r="E143" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" t="s">
+        <v>29</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C144" s="4">
+        <v>22</v>
+      </c>
+      <c r="D144" t="s">
+        <v>8</v>
+      </c>
+      <c r="E144" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" t="s">
+        <v>29</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C145" s="4">
+        <v>5</v>
+      </c>
+      <c r="D145" t="s">
+        <v>13</v>
+      </c>
+      <c r="E145" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" t="s">
+        <v>29</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C146" s="4">
+        <v>32</v>
+      </c>
+      <c r="D146" t="s">
+        <v>13</v>
+      </c>
+      <c r="E146" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" t="s">
+        <v>29</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C147" s="4">
+        <v>5</v>
+      </c>
+      <c r="D147" t="s">
+        <v>13</v>
+      </c>
+      <c r="E147" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" t="s">
+        <v>29</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C148" s="4">
+        <v>5</v>
+      </c>
+      <c r="D148" t="s">
+        <v>18</v>
+      </c>
+      <c r="E148" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" t="s">
+        <v>29</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C149" s="4">
+        <v>15</v>
+      </c>
+      <c r="D149" t="s">
+        <v>18</v>
+      </c>
+      <c r="E149" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" t="s">
+        <v>29</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C150" s="4">
+        <v>5</v>
+      </c>
+      <c r="D150" t="s">
+        <v>18</v>
+      </c>
+      <c r="E150" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" t="s">
+        <v>29</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C151" s="4">
+        <v>1</v>
+      </c>
+      <c r="D151" t="s">
+        <v>75</v>
+      </c>
+      <c r="E151" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152" t="s">
+        <v>29</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C152" s="4">
+        <v>0</v>
+      </c>
+      <c r="D152" t="s">
+        <v>75</v>
+      </c>
+      <c r="E152" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" t="s">
+        <v>62</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C153" s="4">
+        <v>5</v>
+      </c>
+      <c r="D153" t="s">
+        <v>26</v>
+      </c>
+      <c r="E153" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" t="s">
+        <v>62</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C154" s="4">
+        <v>5</v>
+      </c>
+      <c r="D154" t="s">
+        <v>33</v>
+      </c>
+      <c r="E154" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155" t="s">
+        <v>62</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C155" s="4">
+        <v>32</v>
+      </c>
+      <c r="D155" t="s">
+        <v>10</v>
+      </c>
+      <c r="E155" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156" t="s">
+        <v>62</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C156" s="4">
+        <v>17</v>
+      </c>
+      <c r="D156" t="s">
+        <v>8</v>
+      </c>
+      <c r="E156" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157" t="s">
+        <v>62</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C157" s="4">
+        <v>9</v>
+      </c>
+      <c r="D157" t="s">
+        <v>13</v>
+      </c>
+      <c r="E157" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" t="s">
+        <v>62</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C158" s="4">
+        <v>12</v>
+      </c>
+      <c r="D158" t="s">
+        <v>13</v>
+      </c>
+      <c r="E158" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="A159" t="s">
+        <v>62</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C159" s="4">
+        <v>5</v>
+      </c>
+      <c r="D159" t="s">
+        <v>13</v>
+      </c>
+      <c r="E159" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="A160" t="s">
+        <v>62</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C160" s="4">
+        <v>9</v>
+      </c>
+      <c r="D160" t="s">
+        <v>18</v>
+      </c>
+      <c r="E160" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" t="s">
+        <v>62</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C161" s="4">
+        <v>5</v>
+      </c>
+      <c r="D161" t="s">
+        <v>18</v>
+      </c>
+      <c r="E161" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162" t="s">
+        <v>62</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C162" s="4">
+        <v>17</v>
+      </c>
+      <c r="D162" t="s">
+        <v>18</v>
+      </c>
+      <c r="E162" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" t="s">
+        <v>62</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C163" s="4">
+        <v>0</v>
+      </c>
+      <c r="D163" t="s">
+        <v>75</v>
+      </c>
+      <c r="E163" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164" t="s">
+        <v>62</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C164" s="4">
+        <v>0</v>
+      </c>
+      <c r="D164" t="s">
+        <v>75</v>
+      </c>
+      <c r="E164" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" t="s">
+        <v>9</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C165" s="4">
+        <v>6</v>
+      </c>
+      <c r="D165" t="s">
+        <v>37</v>
+      </c>
+      <c r="E165" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" t="s">
+        <v>9</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C166" s="4">
+        <v>5</v>
+      </c>
+      <c r="D166" t="s">
+        <v>33</v>
+      </c>
+      <c r="E166" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167" t="s">
+        <v>9</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C167" s="4">
+        <v>14</v>
+      </c>
+      <c r="D167" t="s">
+        <v>23</v>
+      </c>
+      <c r="E167" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" t="s">
+        <v>9</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C168" s="4">
+        <v>6</v>
+      </c>
+      <c r="D168" t="s">
+        <v>10</v>
+      </c>
+      <c r="E168" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169" t="s">
+        <v>9</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C169" s="4">
+        <v>12</v>
+      </c>
+      <c r="D169" t="s">
+        <v>13</v>
+      </c>
+      <c r="E169" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170" t="s">
+        <v>9</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C170" s="4">
+        <v>12</v>
+      </c>
+      <c r="D170" t="s">
+        <v>13</v>
+      </c>
+      <c r="E170" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="A171" t="s">
+        <v>9</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C171" s="4">
+        <v>6</v>
+      </c>
+      <c r="D171" t="s">
+        <v>13</v>
+      </c>
+      <c r="E171" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172" t="s">
+        <v>9</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C172" s="4">
+        <v>0</v>
+      </c>
+      <c r="D172" t="s">
+        <v>75</v>
+      </c>
+      <c r="E172" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173" t="s">
+        <v>9</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C173" s="4">
+        <v>0</v>
+      </c>
+      <c r="D173" t="s">
+        <v>75</v>
+      </c>
+      <c r="E173" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174" t="s">
+        <v>9</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C174" s="4">
+        <v>15</v>
+      </c>
+      <c r="D174" t="s">
+        <v>18</v>
+      </c>
+      <c r="E174" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" t="s">
+        <v>9</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C175" s="4">
+        <v>11</v>
+      </c>
+      <c r="D175" t="s">
+        <v>18</v>
+      </c>
+      <c r="E175" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176" t="s">
+        <v>9</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C176" s="4">
+        <v>5</v>
+      </c>
+      <c r="D176" t="s">
+        <v>18</v>
+      </c>
+      <c r="E176" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" t="s">
+        <v>28</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C177" s="4">
+        <v>12</v>
+      </c>
+      <c r="D177" t="s">
+        <v>10</v>
+      </c>
+      <c r="E177" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" t="s">
+        <v>28</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C178" s="4">
+        <v>17</v>
+      </c>
+      <c r="D178" t="s">
+        <v>8</v>
+      </c>
+      <c r="E178" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" t="s">
+        <v>28</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C179" s="4">
+        <v>17</v>
+      </c>
+      <c r="D179" t="s">
+        <v>108</v>
+      </c>
+      <c r="E179" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" t="s">
+        <v>28</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C180" s="4">
+        <v>12</v>
+      </c>
+      <c r="D180" t="s">
+        <v>13</v>
+      </c>
+      <c r="E180" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" t="s">
+        <v>28</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C181" s="4">
+        <v>9</v>
+      </c>
+      <c r="D181" t="s">
+        <v>13</v>
+      </c>
+      <c r="E181" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" t="s">
+        <v>28</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C182" s="4">
+        <v>8</v>
+      </c>
+      <c r="D182" t="s">
+        <v>75</v>
+      </c>
+      <c r="E182" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" t="s">
+        <v>28</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C183" s="4">
+        <v>5</v>
+      </c>
+      <c r="D183" t="s">
+        <v>75</v>
+      </c>
+      <c r="E183" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" t="s">
+        <v>28</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C184" s="4">
+        <v>12</v>
+      </c>
+      <c r="D184" t="s">
+        <v>18</v>
+      </c>
+      <c r="E184" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" t="s">
+        <v>28</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C185" s="4">
+        <v>27</v>
+      </c>
+      <c r="D185" t="s">
+        <v>18</v>
+      </c>
+      <c r="E185" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" t="s">
+        <v>28</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C186" s="4">
+        <v>11</v>
+      </c>
+      <c r="D186" t="s">
+        <v>18</v>
+      </c>
+      <c r="E186" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
+      <c r="A187" t="s">
+        <v>28</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C187" s="4">
+        <v>5</v>
+      </c>
+      <c r="D187" t="s">
+        <v>18</v>
+      </c>
+      <c r="E187" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="A188" t="s">
+        <v>28</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C188" s="4">
+        <v>9</v>
+      </c>
+      <c r="D188" t="s">
+        <v>18</v>
+      </c>
+      <c r="E188" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189" t="s">
+        <v>27</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C189" s="4">
+        <v>13</v>
+      </c>
+      <c r="D189" t="s">
+        <v>33</v>
+      </c>
+      <c r="E189" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190" t="s">
+        <v>27</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C190" s="4">
+        <v>8</v>
+      </c>
+      <c r="D190" t="s">
+        <v>23</v>
+      </c>
+      <c r="E190" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="A191" t="s">
+        <v>27</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C191" s="4">
+        <v>14</v>
+      </c>
+      <c r="D191" t="s">
+        <v>10</v>
+      </c>
+      <c r="E191" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="A192" t="s">
+        <v>27</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C192" s="4">
+        <v>7</v>
+      </c>
+      <c r="D192" t="s">
+        <v>8</v>
+      </c>
+      <c r="E192" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" t="s">
+        <v>27</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C193" s="4">
+        <v>5</v>
+      </c>
+      <c r="D193" t="s">
+        <v>108</v>
+      </c>
+      <c r="E193" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194" t="s">
+        <v>27</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C194" s="4">
+        <v>6</v>
+      </c>
+      <c r="D194" t="s">
+        <v>13</v>
+      </c>
+      <c r="E194" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195" t="s">
+        <v>27</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C195" s="4">
+        <v>9</v>
+      </c>
+      <c r="D195" t="s">
+        <v>13</v>
+      </c>
+      <c r="E195" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
+      <c r="A196" t="s">
+        <v>27</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C196" s="4">
+        <v>6</v>
+      </c>
+      <c r="D196" t="s">
+        <v>13</v>
+      </c>
+      <c r="E196" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197" t="s">
+        <v>27</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C197" s="4">
+        <v>8</v>
+      </c>
+      <c r="D197" t="s">
+        <v>13</v>
+      </c>
+      <c r="E197" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198" t="s">
+        <v>27</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C198" s="4">
+        <v>52</v>
+      </c>
+      <c r="D198" t="s">
+        <v>13</v>
+      </c>
+      <c r="E198" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
+      <c r="A199" t="s">
+        <v>27</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C199" s="4">
+        <v>0</v>
+      </c>
+      <c r="D199" t="s">
+        <v>75</v>
+      </c>
+      <c r="E199" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5">
+      <c r="A200" t="s">
+        <v>27</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C200" s="4">
+        <v>2</v>
+      </c>
+      <c r="D200" t="s">
+        <v>75</v>
+      </c>
+      <c r="E200" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
+      <c r="A201" t="s">
+        <v>5</v>
+      </c>
+      <c r="B201" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C93" s="2">
+      <c r="C201" s="4">
         <v>12</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D201" t="s">
         <v>23</v>
       </c>
-      <c r="E93" s="1">
-        <v>43830</v>
-      </c>
-    </row>
-    <row r="106" ht="16.5" customHeight="1"/>
-    <row r="148" ht="24" customHeight="1"/>
-    <row r="255" ht="15.75" customHeight="1"/>
-    <row r="622" spans="6:6" ht="15">
-      <c r="F622" s="4"/>
+      <c r="E201" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5">
+      <c r="A202" t="s">
+        <v>5</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C202" s="4">
+        <v>9</v>
+      </c>
+      <c r="D202" t="s">
+        <v>8</v>
+      </c>
+      <c r="E202" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5">
+      <c r="A203" t="s">
+        <v>5</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C203" s="4">
+        <v>5</v>
+      </c>
+      <c r="D203" t="s">
+        <v>13</v>
+      </c>
+      <c r="E203" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
+      <c r="A204" t="s">
+        <v>5</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C204" s="4">
+        <v>9</v>
+      </c>
+      <c r="D204" t="s">
+        <v>13</v>
+      </c>
+      <c r="E204" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
+      <c r="A205" t="s">
+        <v>5</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C205" s="4">
+        <v>5</v>
+      </c>
+      <c r="D205" t="s">
+        <v>13</v>
+      </c>
+      <c r="E205" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5">
+      <c r="A206" t="s">
+        <v>5</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C206" s="4">
+        <v>15</v>
+      </c>
+      <c r="D206" t="s">
+        <v>13</v>
+      </c>
+      <c r="E206" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
+      <c r="A207" t="s">
+        <v>5</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C207" s="4">
+        <v>8</v>
+      </c>
+      <c r="D207" t="s">
+        <v>13</v>
+      </c>
+      <c r="E207" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="A208" t="s">
+        <v>5</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C208" s="4">
+        <v>0</v>
+      </c>
+      <c r="D208" t="s">
+        <v>75</v>
+      </c>
+      <c r="E208" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5">
+      <c r="A209" t="s">
+        <v>5</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C209" s="4">
+        <v>0</v>
+      </c>
+      <c r="D209" t="s">
+        <v>75</v>
+      </c>
+      <c r="E209" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5">
+      <c r="A210" t="s">
+        <v>5</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C210" s="4">
+        <v>12</v>
+      </c>
+      <c r="D210" t="s">
+        <v>18</v>
+      </c>
+      <c r="E210" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
+      <c r="A211" t="s">
+        <v>5</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C211" s="4">
+        <v>5</v>
+      </c>
+      <c r="D211" t="s">
+        <v>18</v>
+      </c>
+      <c r="E211" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
+      <c r="A212" t="s">
+        <v>5</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C212" s="4">
+        <v>19</v>
+      </c>
+      <c r="D212" t="s">
+        <v>18</v>
+      </c>
+      <c r="E212" s="1">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" ht="16.5" customHeight="1"/>
+    <row r="255" ht="24" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="729" spans="6:6" ht="15">
+      <c r="F729" s="3"/>
     </row>
   </sheetData>
   <sortState ref="A261:E276">

</xml_diff>

<commit_message>
fixed some errors, start of draft
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="290">
   <si>
     <t>team</t>
   </si>
@@ -216,9 +216,6 @@
     <t>perpetual</t>
   </si>
   <si>
-    <t>Pete Alonso</t>
-  </si>
-  <si>
     <t>Salvador Perez</t>
   </si>
   <si>
@@ -705,9 +702,6 @@
     <t>Jack Flaherty</t>
   </si>
   <si>
-    <t>Lance McCullers</t>
-  </si>
-  <si>
     <t>Jose Leclerc</t>
   </si>
   <si>
@@ -775,6 +769,132 @@
   </si>
   <si>
     <t>James Paxton</t>
+  </si>
+  <si>
+    <t>Manny Machado</t>
+  </si>
+  <si>
+    <t>Alex Reyes</t>
+  </si>
+  <si>
+    <t>Max Scherzer</t>
+  </si>
+  <si>
+    <t>Aaron Nola</t>
+  </si>
+  <si>
+    <t>Jesse Winker</t>
+  </si>
+  <si>
+    <t>Michael Brantley</t>
+  </si>
+  <si>
+    <t>Jose Altuve</t>
+  </si>
+  <si>
+    <t>Yasmani Grandal</t>
+  </si>
+  <si>
+    <t>Kris Bryant</t>
+  </si>
+  <si>
+    <t>Garrett Hampson</t>
+  </si>
+  <si>
+    <t>Willson Contreras</t>
+  </si>
+  <si>
+    <t>Zack Greinke</t>
+  </si>
+  <si>
+    <t>Clayton Kershaw</t>
+  </si>
+  <si>
+    <t>Buster Posey</t>
+  </si>
+  <si>
+    <t>Chris Sale</t>
+  </si>
+  <si>
+    <t>Zach Davies</t>
+  </si>
+  <si>
+    <t>Starling Marte</t>
+  </si>
+  <si>
+    <t>Paul Goldschmidt</t>
+  </si>
+  <si>
+    <t>Bryce Harper</t>
+  </si>
+  <si>
+    <t>Nomar Mazara</t>
+  </si>
+  <si>
+    <t>Starlin Castro</t>
+  </si>
+  <si>
+    <t>Yu Darvish</t>
+  </si>
+  <si>
+    <t>Dakota Hudson</t>
+  </si>
+  <si>
+    <t>Giancarlo Stanton</t>
+  </si>
+  <si>
+    <t>Anthony Rizzo</t>
+  </si>
+  <si>
+    <t>Yadier Molina</t>
+  </si>
+  <si>
+    <t>Kenley Jansen</t>
+  </si>
+  <si>
+    <t>Josh Donaldson</t>
+  </si>
+  <si>
+    <t>Wilson Ramos</t>
+  </si>
+  <si>
+    <t>Aroldis Chapman</t>
+  </si>
+  <si>
+    <t>Zack Wheeler</t>
+  </si>
+  <si>
+    <t>Jorge Polanco</t>
+  </si>
+  <si>
+    <t>Andrew Heaney</t>
+  </si>
+  <si>
+    <t>Jason Heyward</t>
+  </si>
+  <si>
+    <t>Corey Kluber</t>
+  </si>
+  <si>
+    <t>Raisel Iglesias</t>
+  </si>
+  <si>
+    <t>Travis Shaw</t>
+  </si>
+  <si>
+    <t>Luis Arraez</t>
+  </si>
+  <si>
+    <t>Carlos Santana</t>
+  </si>
+  <si>
+    <t>Lance McCullers Jr.</t>
+  </si>
+  <si>
+    <t>Peter Alonso</t>
+  </si>
+  <si>
+    <t>Freddie Freeman</t>
   </si>
 </sst>
 </file>
@@ -1238,7 +1358,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="152">
+  <cellStyleXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1391,6 +1511,28 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1401,7 +1543,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="152">
+  <cellStyles count="174">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1485,6 +1627,17 @@
     <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1545,6 +1698,17 @@
     <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1867,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F729"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="D212" sqref="D212"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="B215" sqref="B215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2105,7 +2269,7 @@
         <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="4">
         <v>8</v>
@@ -2122,7 +2286,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="4">
         <v>9</v>
@@ -2139,7 +2303,7 @@
         <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="4">
         <v>12</v>
@@ -2156,7 +2320,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" s="4">
         <v>16</v>
@@ -2173,7 +2337,7 @@
         <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="4">
         <v>7</v>
@@ -2190,7 +2354,7 @@
         <v>22</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="4">
         <v>22</v>
@@ -2207,13 +2371,13 @@
         <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" s="4">
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E20" s="1">
         <v>43830</v>
@@ -2224,7 +2388,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="4">
         <v>13</v>
@@ -2241,7 +2405,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C22" s="4">
         <v>7</v>
@@ -2258,7 +2422,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23" s="4">
         <v>12</v>
@@ -2275,7 +2439,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C24" s="4">
         <v>1</v>
@@ -2309,7 +2473,7 @@
         <v>32</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C26" s="4">
         <v>5</v>
@@ -2326,7 +2490,7 @@
         <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" s="4">
         <v>5</v>
@@ -2343,7 +2507,7 @@
         <v>32</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C28" s="4">
         <v>5</v>
@@ -2360,7 +2524,7 @@
         <v>32</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29" s="4">
         <v>22</v>
@@ -2377,7 +2541,7 @@
         <v>32</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C30" s="4">
         <v>19</v>
@@ -2394,7 +2558,7 @@
         <v>32</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C31" s="4">
         <v>9</v>
@@ -2411,13 +2575,13 @@
         <v>32</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C32" s="4">
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E32" s="1">
         <v>43830</v>
@@ -2428,13 +2592,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C33" s="4">
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E33" s="1">
         <v>43830</v>
@@ -2445,7 +2609,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C34" s="4">
         <v>7</v>
@@ -2462,7 +2626,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C35" s="4">
         <v>23</v>
@@ -2479,7 +2643,7 @@
         <v>32</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C36" s="4">
         <v>22</v>
@@ -2513,7 +2677,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C38" s="4">
         <v>5</v>
@@ -2530,7 +2694,7 @@
         <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C39" s="4">
         <v>15</v>
@@ -2547,7 +2711,7 @@
         <v>36</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C40" s="4">
         <v>22</v>
@@ -2564,7 +2728,7 @@
         <v>36</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C41" s="4">
         <v>5</v>
@@ -2581,13 +2745,13 @@
         <v>36</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C42" s="4">
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E42" s="1">
         <v>43830</v>
@@ -2598,7 +2762,7 @@
         <v>36</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C43" s="4">
         <v>17</v>
@@ -2615,7 +2779,7 @@
         <v>36</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C44" s="4">
         <v>17</v>
@@ -2632,7 +2796,7 @@
         <v>36</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C45" s="4">
         <v>9</v>
@@ -2649,7 +2813,7 @@
         <v>36</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C46" s="4">
         <v>10</v>
@@ -2666,7 +2830,7 @@
         <v>36</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C47" s="4">
         <v>5</v>
@@ -2700,7 +2864,7 @@
         <v>30</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C49" s="4">
         <v>23</v>
@@ -2717,7 +2881,7 @@
         <v>30</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C50" s="4">
         <v>13</v>
@@ -2734,7 +2898,7 @@
         <v>30</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C51" s="4">
         <v>9</v>
@@ -2751,13 +2915,13 @@
         <v>30</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C52" s="4">
         <v>8</v>
       </c>
       <c r="D52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E52" s="1">
         <v>43830</v>
@@ -2768,7 +2932,7 @@
         <v>30</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C53" s="4">
         <v>5</v>
@@ -2785,13 +2949,13 @@
         <v>30</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C54" s="4">
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E54" s="1">
         <v>43830</v>
@@ -2802,7 +2966,7 @@
         <v>30</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C55" s="4">
         <v>7</v>
@@ -2819,7 +2983,7 @@
         <v>30</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C56" s="4">
         <v>20</v>
@@ -2836,7 +3000,7 @@
         <v>30</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C57" s="4">
         <v>9</v>
@@ -2853,7 +3017,7 @@
         <v>30</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C58" s="4">
         <v>14</v>
@@ -2870,13 +3034,13 @@
         <v>30</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C59" s="4">
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E59" s="1">
         <v>43830</v>
@@ -2904,7 +3068,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C61" s="4">
         <v>17</v>
@@ -2921,7 +3085,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C62" s="4">
         <v>17</v>
@@ -2938,7 +3102,7 @@
         <v>60</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C63" s="4">
         <v>12</v>
@@ -2955,7 +3119,7 @@
         <v>60</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C64" s="4">
         <v>6</v>
@@ -2972,13 +3136,13 @@
         <v>60</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C65" s="4">
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E65" s="1">
         <v>43830</v>
@@ -2989,13 +3153,13 @@
         <v>60</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C66" s="4">
         <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E66" s="1">
         <v>43830</v>
@@ -3006,7 +3170,7 @@
         <v>60</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C67" s="4">
         <v>5</v>
@@ -3023,7 +3187,7 @@
         <v>60</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C68" s="4">
         <v>12</v>
@@ -3040,7 +3204,7 @@
         <v>60</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C69" s="4">
         <v>10</v>
@@ -3057,7 +3221,7 @@
         <v>60</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C70" s="4">
         <v>13</v>
@@ -3074,7 +3238,7 @@
         <v>60</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C71" s="4">
         <v>9</v>
@@ -3108,7 +3272,7 @@
         <v>21</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C73" s="4">
         <v>7</v>
@@ -3125,7 +3289,7 @@
         <v>21</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C74" s="4">
         <v>16</v>
@@ -3142,7 +3306,7 @@
         <v>21</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C75" s="4">
         <v>12</v>
@@ -3159,7 +3323,7 @@
         <v>21</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C76" s="4">
         <v>27</v>
@@ -3176,7 +3340,7 @@
         <v>21</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C77" s="4">
         <v>6</v>
@@ -3193,7 +3357,7 @@
         <v>21</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C78" s="4">
         <v>26</v>
@@ -3210,7 +3374,7 @@
         <v>21</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C79" s="4">
         <v>5</v>
@@ -3227,7 +3391,7 @@
         <v>21</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C80" s="4">
         <v>6</v>
@@ -3244,7 +3408,7 @@
         <v>21</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C81" s="4">
         <v>23</v>
@@ -3261,13 +3425,13 @@
         <v>21</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C82" s="4">
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E82" s="1">
         <v>43830</v>
@@ -3295,7 +3459,7 @@
         <v>20</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C84" s="4">
         <v>32</v>
@@ -3312,7 +3476,7 @@
         <v>20</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C85" s="4">
         <v>24</v>
@@ -3329,13 +3493,13 @@
         <v>20</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C86" s="4">
         <v>19</v>
       </c>
       <c r="D86" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E86" s="1">
         <v>43830</v>
@@ -3346,7 +3510,7 @@
         <v>20</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C87" s="4">
         <v>5</v>
@@ -3363,7 +3527,7 @@
         <v>20</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C88" s="4">
         <v>41</v>
@@ -3380,7 +3544,7 @@
         <v>20</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C89" s="4">
         <v>12</v>
@@ -3397,13 +3561,13 @@
         <v>20</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C90" s="4">
         <v>10</v>
       </c>
       <c r="D90" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E90" s="1">
         <v>43830</v>
@@ -3414,7 +3578,7 @@
         <v>20</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C91" s="4">
         <v>5</v>
@@ -3431,7 +3595,7 @@
         <v>20</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C92" s="4">
         <v>22</v>
@@ -3448,13 +3612,13 @@
         <v>20</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C93" s="4">
         <v>0</v>
       </c>
       <c r="D93" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E93" s="1">
         <v>43830</v>
@@ -3465,13 +3629,13 @@
         <v>20</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C94" s="4">
         <v>0</v>
       </c>
       <c r="D94" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E94" s="1">
         <v>43830</v>
@@ -3499,7 +3663,7 @@
         <v>61</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C96" s="4">
         <v>5</v>
@@ -3516,7 +3680,7 @@
         <v>61</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C97" s="4">
         <v>7</v>
@@ -3533,7 +3697,7 @@
         <v>61</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C98" s="4">
         <v>10</v>
@@ -3550,13 +3714,13 @@
         <v>61</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C99" s="4">
         <v>26</v>
       </c>
       <c r="D99" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E99" s="1">
         <v>43830</v>
@@ -3567,7 +3731,7 @@
         <v>61</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C100" s="4">
         <v>18</v>
@@ -3584,13 +3748,13 @@
         <v>61</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C101" s="4">
         <v>0</v>
       </c>
       <c r="D101" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E101" s="1">
         <v>43830</v>
@@ -3601,7 +3765,7 @@
         <v>61</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C102" s="4">
         <v>14</v>
@@ -3618,7 +3782,7 @@
         <v>61</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C103" s="4">
         <v>12</v>
@@ -3635,7 +3799,7 @@
         <v>61</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C104" s="4">
         <v>13</v>
@@ -3652,7 +3816,7 @@
         <v>61</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C105" s="4">
         <v>16</v>
@@ -3669,13 +3833,13 @@
         <v>61</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C106" s="4">
         <v>0</v>
       </c>
       <c r="D106" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E106" s="1">
         <v>43830</v>
@@ -3703,7 +3867,7 @@
         <v>16</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C108" s="4">
         <v>13</v>
@@ -3720,7 +3884,7 @@
         <v>16</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C109" s="4">
         <v>14</v>
@@ -3737,13 +3901,13 @@
         <v>16</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C110" s="4">
         <v>6</v>
       </c>
       <c r="D110" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E110" s="1">
         <v>43830</v>
@@ -3754,7 +3918,7 @@
         <v>16</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C111" s="4">
         <v>6</v>
@@ -3771,7 +3935,7 @@
         <v>16</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C112" s="4">
         <v>6</v>
@@ -3788,7 +3952,7 @@
         <v>16</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C113" s="4">
         <v>11</v>
@@ -3805,13 +3969,13 @@
         <v>16</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C114" s="4">
         <v>1</v>
       </c>
       <c r="D114" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E114" s="1">
         <v>43830</v>
@@ -3822,7 +3986,7 @@
         <v>16</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C115" s="4">
         <v>8</v>
@@ -3839,7 +4003,7 @@
         <v>16</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C116" s="4">
         <v>32</v>
@@ -3856,7 +4020,7 @@
         <v>16</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C117" s="4">
         <v>28</v>
@@ -3890,7 +4054,7 @@
         <v>14</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C119" s="4">
         <v>19</v>
@@ -3907,13 +4071,13 @@
         <v>14</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C120" s="4">
         <v>5</v>
       </c>
       <c r="D120" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E120" s="1">
         <v>43830</v>
@@ -3924,7 +4088,7 @@
         <v>14</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C121" s="4">
         <v>5</v>
@@ -3941,7 +4105,7 @@
         <v>14</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C122" s="4">
         <v>33</v>
@@ -3958,7 +4122,7 @@
         <v>14</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C123" s="4">
         <v>17</v>
@@ -3975,7 +4139,7 @@
         <v>14</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C124" s="4">
         <v>15</v>
@@ -3992,7 +4156,7 @@
         <v>14</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C125" s="4">
         <v>12</v>
@@ -4009,7 +4173,7 @@
         <v>14</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C126" s="4">
         <v>12</v>
@@ -4026,7 +4190,7 @@
         <v>14</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C127" s="4">
         <v>13</v>
@@ -4043,7 +4207,7 @@
         <v>14</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C128" s="4">
         <v>0</v>
@@ -4077,7 +4241,7 @@
         <v>11</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C130" s="4">
         <v>17</v>
@@ -4094,7 +4258,7 @@
         <v>11</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C131" s="4">
         <v>21</v>
@@ -4111,13 +4275,13 @@
         <v>11</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C132" s="4">
         <v>12</v>
       </c>
       <c r="D132" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E132" s="1">
         <v>43830</v>
@@ -4128,7 +4292,7 @@
         <v>11</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C133" s="4">
         <v>11</v>
@@ -4145,7 +4309,7 @@
         <v>11</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C134" s="4">
         <v>27</v>
@@ -4162,13 +4326,13 @@
         <v>11</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C135" s="4">
         <v>0</v>
       </c>
       <c r="D135" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E135" s="1">
         <v>43830</v>
@@ -4179,13 +4343,13 @@
         <v>11</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C136" s="4">
         <v>0</v>
       </c>
       <c r="D136" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E136" s="1">
         <v>43830</v>
@@ -4196,7 +4360,7 @@
         <v>11</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C137" s="4">
         <v>33</v>
@@ -4213,7 +4377,7 @@
         <v>11</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C138" s="4">
         <v>12</v>
@@ -4230,7 +4394,7 @@
         <v>11</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C139" s="4">
         <v>10</v>
@@ -4247,7 +4411,7 @@
         <v>11</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C140" s="4">
         <v>9</v>
@@ -4281,7 +4445,7 @@
         <v>29</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C142" s="4">
         <v>12</v>
@@ -4298,7 +4462,7 @@
         <v>29</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C143" s="4">
         <v>5</v>
@@ -4315,7 +4479,7 @@
         <v>29</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C144" s="4">
         <v>22</v>
@@ -4332,7 +4496,7 @@
         <v>29</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C145" s="4">
         <v>5</v>
@@ -4349,7 +4513,7 @@
         <v>29</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C146" s="4">
         <v>32</v>
@@ -4366,7 +4530,7 @@
         <v>29</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C147" s="4">
         <v>5</v>
@@ -4383,7 +4547,7 @@
         <v>29</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C148" s="4">
         <v>5</v>
@@ -4400,7 +4564,7 @@
         <v>29</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C149" s="4">
         <v>15</v>
@@ -4417,7 +4581,7 @@
         <v>29</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C150" s="4">
         <v>5</v>
@@ -4434,13 +4598,13 @@
         <v>29</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C151" s="4">
         <v>1</v>
       </c>
       <c r="D151" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E151" s="1">
         <v>43830</v>
@@ -4451,13 +4615,13 @@
         <v>29</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C152" s="4">
         <v>0</v>
       </c>
       <c r="D152" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E152" s="1">
         <v>43830</v>
@@ -4485,7 +4649,7 @@
         <v>62</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C154" s="4">
         <v>5</v>
@@ -4502,7 +4666,7 @@
         <v>62</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C155" s="4">
         <v>32</v>
@@ -4519,7 +4683,7 @@
         <v>62</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C156" s="4">
         <v>17</v>
@@ -4536,7 +4700,7 @@
         <v>62</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C157" s="4">
         <v>9</v>
@@ -4553,7 +4717,7 @@
         <v>62</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C158" s="4">
         <v>12</v>
@@ -4570,7 +4734,7 @@
         <v>62</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C159" s="4">
         <v>5</v>
@@ -4587,7 +4751,7 @@
         <v>62</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C160" s="4">
         <v>9</v>
@@ -4604,7 +4768,7 @@
         <v>62</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C161" s="4">
         <v>5</v>
@@ -4621,7 +4785,7 @@
         <v>62</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C162" s="4">
         <v>17</v>
@@ -4638,13 +4802,13 @@
         <v>62</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C163" s="4">
         <v>0</v>
       </c>
       <c r="D163" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E163" s="1">
         <v>43830</v>
@@ -4655,13 +4819,13 @@
         <v>62</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C164" s="4">
         <v>0</v>
       </c>
       <c r="D164" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E164" s="1">
         <v>43830</v>
@@ -4689,7 +4853,7 @@
         <v>9</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C166" s="4">
         <v>5</v>
@@ -4706,7 +4870,7 @@
         <v>9</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C167" s="4">
         <v>14</v>
@@ -4723,7 +4887,7 @@
         <v>9</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C168" s="4">
         <v>6</v>
@@ -4740,7 +4904,7 @@
         <v>9</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C169" s="4">
         <v>12</v>
@@ -4757,7 +4921,7 @@
         <v>9</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C170" s="4">
         <v>12</v>
@@ -4774,7 +4938,7 @@
         <v>9</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C171" s="4">
         <v>6</v>
@@ -4791,13 +4955,13 @@
         <v>9</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C172" s="4">
         <v>0</v>
       </c>
       <c r="D172" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E172" s="1">
         <v>43830</v>
@@ -4808,13 +4972,13 @@
         <v>9</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C173" s="4">
         <v>0</v>
       </c>
       <c r="D173" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E173" s="1">
         <v>43830</v>
@@ -4825,7 +4989,7 @@
         <v>9</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C174" s="4">
         <v>15</v>
@@ -4842,7 +5006,7 @@
         <v>9</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C175" s="4">
         <v>11</v>
@@ -4859,7 +5023,7 @@
         <v>9</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C176" s="4">
         <v>5</v>
@@ -4893,7 +5057,7 @@
         <v>28</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C178" s="4">
         <v>17</v>
@@ -4910,13 +5074,13 @@
         <v>28</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C179" s="4">
         <v>17</v>
       </c>
       <c r="D179" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E179" s="1">
         <v>43830</v>
@@ -4927,7 +5091,7 @@
         <v>28</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C180" s="4">
         <v>12</v>
@@ -4944,7 +5108,7 @@
         <v>28</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C181" s="4">
         <v>9</v>
@@ -4961,13 +5125,13 @@
         <v>28</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C182" s="4">
         <v>8</v>
       </c>
       <c r="D182" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E182" s="1">
         <v>43830</v>
@@ -4978,13 +5142,13 @@
         <v>28</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C183" s="4">
         <v>5</v>
       </c>
       <c r="D183" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E183" s="1">
         <v>43830</v>
@@ -4995,7 +5159,7 @@
         <v>28</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C184" s="4">
         <v>12</v>
@@ -5012,7 +5176,7 @@
         <v>28</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C185" s="4">
         <v>27</v>
@@ -5029,7 +5193,7 @@
         <v>28</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C186" s="4">
         <v>11</v>
@@ -5046,7 +5210,7 @@
         <v>28</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>226</v>
+        <v>287</v>
       </c>
       <c r="C187" s="4">
         <v>5</v>
@@ -5063,7 +5227,7 @@
         <v>28</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C188" s="4">
         <v>9</v>
@@ -5080,7 +5244,7 @@
         <v>27</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>63</v>
+        <v>288</v>
       </c>
       <c r="C189" s="4">
         <v>13</v>
@@ -5097,7 +5261,7 @@
         <v>27</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C190" s="4">
         <v>8</v>
@@ -5114,7 +5278,7 @@
         <v>27</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C191" s="4">
         <v>14</v>
@@ -5131,7 +5295,7 @@
         <v>27</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C192" s="4">
         <v>7</v>
@@ -5148,13 +5312,13 @@
         <v>27</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C193" s="4">
         <v>5</v>
       </c>
       <c r="D193" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E193" s="1">
         <v>43830</v>
@@ -5165,7 +5329,7 @@
         <v>27</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C194" s="4">
         <v>6</v>
@@ -5182,7 +5346,7 @@
         <v>27</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C195" s="4">
         <v>9</v>
@@ -5199,7 +5363,7 @@
         <v>27</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C196" s="4">
         <v>6</v>
@@ -5216,7 +5380,7 @@
         <v>27</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C197" s="4">
         <v>8</v>
@@ -5233,7 +5397,7 @@
         <v>27</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C198" s="4">
         <v>52</v>
@@ -5250,13 +5414,13 @@
         <v>27</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C199" s="4">
         <v>0</v>
       </c>
       <c r="D199" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E199" s="1">
         <v>43830</v>
@@ -5267,13 +5431,13 @@
         <v>27</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C200" s="4">
         <v>2</v>
       </c>
       <c r="D200" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E200" s="1">
         <v>43830</v>
@@ -5301,7 +5465,7 @@
         <v>5</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C202" s="4">
         <v>9</v>
@@ -5318,7 +5482,7 @@
         <v>5</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C203" s="4">
         <v>5</v>
@@ -5335,7 +5499,7 @@
         <v>5</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C204" s="4">
         <v>9</v>
@@ -5352,7 +5516,7 @@
         <v>5</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C205" s="4">
         <v>5</v>
@@ -5369,7 +5533,7 @@
         <v>5</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C206" s="4">
         <v>15</v>
@@ -5386,7 +5550,7 @@
         <v>5</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C207" s="4">
         <v>8</v>
@@ -5403,13 +5567,13 @@
         <v>5</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C208" s="4">
         <v>0</v>
       </c>
       <c r="D208" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E208" s="1">
         <v>43830</v>
@@ -5420,13 +5584,13 @@
         <v>5</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C209" s="4">
         <v>0</v>
       </c>
       <c r="D209" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E209" s="1">
         <v>43830</v>
@@ -5437,7 +5601,7 @@
         <v>5</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C210" s="4">
         <v>12</v>
@@ -5454,7 +5618,7 @@
         <v>5</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C211" s="4">
         <v>5</v>
@@ -5471,7 +5635,7 @@
         <v>5</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C212" s="4">
         <v>19</v>
@@ -5483,8 +5647,687 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="16.5" customHeight="1"/>
-    <row r="255" ht="24" customHeight="1"/>
+    <row r="213" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A213" t="s">
+        <v>32</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C213" s="4">
+        <v>29</v>
+      </c>
+      <c r="D213" t="s">
+        <v>8</v>
+      </c>
+      <c r="E213" s="1">
+        <v>43836</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5">
+      <c r="A214" t="s">
+        <v>22</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C214" s="4">
+        <v>4</v>
+      </c>
+      <c r="D214" t="s">
+        <v>18</v>
+      </c>
+      <c r="E214" s="1">
+        <v>43836</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5">
+      <c r="A215" t="s">
+        <v>14</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C215" s="4">
+        <v>34</v>
+      </c>
+      <c r="D215" t="s">
+        <v>33</v>
+      </c>
+      <c r="E215" s="1">
+        <v>43836</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5">
+      <c r="A216" t="s">
+        <v>60</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C216" s="4">
+        <v>39</v>
+      </c>
+      <c r="D216" t="s">
+        <v>18</v>
+      </c>
+      <c r="E216" s="1">
+        <v>43836</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5">
+      <c r="A217" t="s">
+        <v>21</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C217" s="4">
+        <v>30</v>
+      </c>
+      <c r="D217" t="s">
+        <v>18</v>
+      </c>
+      <c r="E217" s="1">
+        <v>43836</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5">
+      <c r="A218" t="s">
+        <v>9</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C218" s="4">
+        <v>6</v>
+      </c>
+      <c r="D218" t="s">
+        <v>13</v>
+      </c>
+      <c r="E218" s="1">
+        <v>43836</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5">
+      <c r="A219" t="s">
+        <v>22</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C219" s="4">
+        <v>19</v>
+      </c>
+      <c r="D219" t="s">
+        <v>13</v>
+      </c>
+      <c r="E219" s="1">
+        <v>43836</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5">
+      <c r="A220" t="s">
+        <v>29</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C220" s="4">
+        <v>25</v>
+      </c>
+      <c r="D220" t="s">
+        <v>23</v>
+      </c>
+      <c r="E220" s="1">
+        <v>43836</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5">
+      <c r="A221" t="s">
+        <v>30</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C221" s="4">
+        <v>23</v>
+      </c>
+      <c r="D221" t="s">
+        <v>37</v>
+      </c>
+      <c r="E221" s="1">
+        <v>43837</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5">
+      <c r="A222" t="s">
+        <v>61</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C222" s="4">
+        <v>29</v>
+      </c>
+      <c r="D222" t="s">
+        <v>13</v>
+      </c>
+      <c r="E222" s="1">
+        <v>43837</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5">
+      <c r="A223" t="s">
+        <v>28</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C223" s="4">
+        <v>10</v>
+      </c>
+      <c r="D223" t="s">
+        <v>23</v>
+      </c>
+      <c r="E223" s="1">
+        <v>43837</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5">
+      <c r="A224" t="s">
+        <v>28</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C224" s="4">
+        <v>18</v>
+      </c>
+      <c r="D224" t="s">
+        <v>37</v>
+      </c>
+      <c r="E224" s="1">
+        <v>43837</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5">
+      <c r="A225" t="s">
+        <v>22</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C225" s="4">
+        <v>23</v>
+      </c>
+      <c r="D225" t="s">
+        <v>18</v>
+      </c>
+      <c r="E225" s="1">
+        <v>43837</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5">
+      <c r="A226" t="s">
+        <v>22</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C226" s="4">
+        <v>28</v>
+      </c>
+      <c r="D226" t="s">
+        <v>18</v>
+      </c>
+      <c r="E226" s="1">
+        <v>43837</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5">
+      <c r="A227" t="s">
+        <v>20</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C227" s="4">
+        <v>8</v>
+      </c>
+      <c r="D227" t="s">
+        <v>37</v>
+      </c>
+      <c r="E227" s="1">
+        <v>43837</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5">
+      <c r="A228" t="s">
+        <v>16</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C228" s="4">
+        <v>33</v>
+      </c>
+      <c r="D228" t="s">
+        <v>18</v>
+      </c>
+      <c r="E228" s="1">
+        <v>43837</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5">
+      <c r="A229" t="s">
+        <v>30</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C229" s="4">
+        <v>1</v>
+      </c>
+      <c r="D229" t="s">
+        <v>18</v>
+      </c>
+      <c r="E229" s="1">
+        <v>43838</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5">
+      <c r="A230" t="s">
+        <v>36</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C230" s="4">
+        <v>31</v>
+      </c>
+      <c r="D230" t="s">
+        <v>13</v>
+      </c>
+      <c r="E230" s="1">
+        <v>43838</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5">
+      <c r="A231" t="s">
+        <v>32</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C231" s="4">
+        <v>24</v>
+      </c>
+      <c r="D231" t="s">
+        <v>33</v>
+      </c>
+      <c r="E231" s="1">
+        <v>43838</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5">
+      <c r="A232" t="s">
+        <v>60</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C232" s="4">
+        <v>34</v>
+      </c>
+      <c r="D232" t="s">
+        <v>13</v>
+      </c>
+      <c r="E232" s="1">
+        <v>43838</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5">
+      <c r="A233" t="s">
+        <v>36</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C233" s="4">
+        <v>16</v>
+      </c>
+      <c r="D233" t="s">
+        <v>13</v>
+      </c>
+      <c r="E233" s="1">
+        <v>43838</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5">
+      <c r="A234" t="s">
+        <v>22</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C234" s="4">
+        <v>8</v>
+      </c>
+      <c r="D234" t="s">
+        <v>107</v>
+      </c>
+      <c r="E234" s="1">
+        <v>43838</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5">
+      <c r="A235" t="s">
+        <v>27</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C235" s="4">
+        <v>24</v>
+      </c>
+      <c r="D235" t="s">
+        <v>18</v>
+      </c>
+      <c r="E235" s="1">
+        <v>43838</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5">
+      <c r="A236" t="s">
+        <v>22</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C236" s="4">
+        <v>8</v>
+      </c>
+      <c r="D236" t="s">
+        <v>18</v>
+      </c>
+      <c r="E236" s="1">
+        <v>43838</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5">
+      <c r="A237" t="s">
+        <v>5</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C237" s="4">
+        <v>34</v>
+      </c>
+      <c r="D237" t="s">
+        <v>13</v>
+      </c>
+      <c r="E237" s="1">
+        <v>43839</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5">
+      <c r="A238" t="s">
+        <v>20</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C238" s="4">
+        <v>29</v>
+      </c>
+      <c r="D238" t="s">
+        <v>33</v>
+      </c>
+      <c r="E238" s="1">
+        <v>43839</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5">
+      <c r="A239" t="s">
+        <v>5</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C239" s="4">
+        <v>8</v>
+      </c>
+      <c r="D239" t="s">
+        <v>37</v>
+      </c>
+      <c r="E239" s="1">
+        <v>43839</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5">
+      <c r="A240" t="s">
+        <v>9</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C240" s="4">
+        <v>20</v>
+      </c>
+      <c r="D240" t="s">
+        <v>18</v>
+      </c>
+      <c r="E240" s="1">
+        <v>43839</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5">
+      <c r="A241" t="s">
+        <v>16</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C241" s="4">
+        <v>24</v>
+      </c>
+      <c r="D241" t="s">
+        <v>26</v>
+      </c>
+      <c r="E241" s="1">
+        <v>43839</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5">
+      <c r="A242" t="s">
+        <v>20</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C242" s="4">
+        <v>13</v>
+      </c>
+      <c r="D242" t="s">
+        <v>37</v>
+      </c>
+      <c r="E242" s="1">
+        <v>43839</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5">
+      <c r="A243" t="s">
+        <v>27</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C243" s="4">
+        <v>26</v>
+      </c>
+      <c r="D243" t="s">
+        <v>18</v>
+      </c>
+      <c r="E243" s="1">
+        <v>43839</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5">
+      <c r="A244" t="s">
+        <v>6</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C244" s="4">
+        <v>20</v>
+      </c>
+      <c r="D244" t="s">
+        <v>18</v>
+      </c>
+      <c r="E244" s="1">
+        <v>43839</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5">
+      <c r="A245" t="s">
+        <v>9</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C245" s="4">
+        <v>15</v>
+      </c>
+      <c r="D245" t="s">
+        <v>8</v>
+      </c>
+      <c r="E245" s="1">
+        <v>43840</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5">
+      <c r="A246" t="s">
+        <v>29</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C246" s="4">
+        <v>16</v>
+      </c>
+      <c r="D246" t="s">
+        <v>18</v>
+      </c>
+      <c r="E246" s="1">
+        <v>43840</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5">
+      <c r="A247" t="s">
+        <v>36</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C247" s="4">
+        <v>7</v>
+      </c>
+      <c r="D247" t="s">
+        <v>13</v>
+      </c>
+      <c r="E247" s="1">
+        <v>43840</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5">
+      <c r="A248" t="s">
+        <v>16</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C248" s="4">
+        <v>21</v>
+      </c>
+      <c r="D248" t="s">
+        <v>18</v>
+      </c>
+      <c r="E248" s="1">
+        <v>43840</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5">
+      <c r="A249" t="s">
+        <v>27</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C249" s="4">
+        <v>22</v>
+      </c>
+      <c r="D249" t="s">
+        <v>18</v>
+      </c>
+      <c r="E249" s="1">
+        <v>43840</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5">
+      <c r="A250" t="s">
+        <v>5</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C250" s="4">
+        <v>6</v>
+      </c>
+      <c r="D250" t="s">
+        <v>10</v>
+      </c>
+      <c r="E250" s="1">
+        <v>43840</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5">
+      <c r="A251" t="s">
+        <v>32</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C251" s="4">
+        <v>9</v>
+      </c>
+      <c r="D251" t="s">
+        <v>107</v>
+      </c>
+      <c r="E251" s="1">
+        <v>43840</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5">
+      <c r="A252" t="s">
+        <v>5</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C252" s="4">
+        <v>19</v>
+      </c>
+      <c r="D252" t="s">
+        <v>33</v>
+      </c>
+      <c r="E252" s="1">
+        <v>43840</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" ht="24" customHeight="1"/>
     <row r="362" ht="15.75" customHeight="1"/>
     <row r="729" spans="6:6" ht="15">
       <c r="F729" s="3"/>

</xml_diff>

<commit_message>
added picks to RMD doc
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -2031,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F729"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="B215" sqref="B215"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4329,7 +4329,7 @@
         <v>177</v>
       </c>
       <c r="C135" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D135" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
fixed draft bugs and more picks
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HRDUser\Desktop\fantasy2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28C22D4-DE95-4216-8DEB-950BFF66F95E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="17925" yWindow="1845" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="draftpicks" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="344">
   <si>
     <t>team</t>
   </si>
@@ -366,9 +367,6 @@
     <t>Miguel Andujar</t>
   </si>
   <si>
-    <t>UT</t>
-  </si>
-  <si>
     <t>Frankie Montas</t>
   </si>
   <si>
@@ -1036,22 +1034,51 @@
   </si>
   <si>
     <t>Chris Archer</t>
+  </si>
+  <si>
+    <t>Mike Ford</t>
+  </si>
+  <si>
+    <t>Joe Musgrove</t>
+  </si>
+  <si>
+    <t>Robinson Chirinos</t>
+  </si>
+  <si>
+    <t>Ian Kennedy</t>
+  </si>
+  <si>
+    <t>Harrison Bader</t>
+  </si>
+  <si>
+    <t>Scott Oberg</t>
+  </si>
+  <si>
+    <t>Kyle Seager</t>
+  </si>
+  <si>
+    <t>Lewis Brinson</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\$#,##0;[Red]\$#,##0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Material Icons"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1074,13 +1101,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1360,14 +1393,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E362"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A284" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E302" sqref="E302:E308"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125"/>
     <col min="2" max="2" width="26.7109375" style="1" customWidth="1"/>
@@ -1377,7 +1410,7 @@
     <col min="6" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1394,7 +1427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1411,7 +1444,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1428,7 +1461,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1445,7 +1478,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1462,7 +1495,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1479,7 +1512,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1496,7 +1529,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1513,7 +1546,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1530,7 +1563,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1547,7 +1580,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1564,7 +1597,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1581,7 +1614,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1598,7 +1631,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1615,7 +1648,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1632,7 +1665,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1649,7 +1682,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1666,7 +1699,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1683,7 +1716,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1700,7 +1733,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1717,7 +1750,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1734,7 +1767,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1751,7 +1784,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1768,7 +1801,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1785,7 +1818,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1802,7 +1835,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1819,7 +1852,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1836,7 +1869,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1853,7 +1886,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1870,7 +1903,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -1887,7 +1920,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1904,7 +1937,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -1921,7 +1954,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1938,7 +1971,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1955,7 +1988,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1972,7 +2005,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1989,7 +2022,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -2006,7 +2039,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -2023,7 +2056,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -2040,7 +2073,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -2057,7 +2090,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -2074,7 +2107,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -2091,7 +2124,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -2108,7 +2141,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -2125,7 +2158,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -2142,7 +2175,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -2159,7 +2192,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -2176,7 +2209,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>64</v>
       </c>
@@ -2193,7 +2226,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>64</v>
       </c>
@@ -2210,7 +2243,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -2227,7 +2260,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -2244,7 +2277,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>64</v>
       </c>
@@ -2261,7 +2294,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -2278,7 +2311,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -2295,7 +2328,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -2312,7 +2345,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -2329,7 +2362,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -2346,7 +2379,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -2363,7 +2396,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>64</v>
       </c>
@@ -2380,7 +2413,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>78</v>
       </c>
@@ -2397,7 +2430,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>78</v>
       </c>
@@ -2414,7 +2447,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>78</v>
       </c>
@@ -2431,7 +2464,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -2448,7 +2481,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>78</v>
       </c>
@@ -2465,7 +2498,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>78</v>
       </c>
@@ -2482,7 +2515,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>78</v>
       </c>
@@ -2499,7 +2532,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>78</v>
       </c>
@@ -2516,7 +2549,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>78</v>
       </c>
@@ -2533,7 +2566,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>78</v>
       </c>
@@ -2550,7 +2583,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>78</v>
       </c>
@@ -2567,7 +2600,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>78</v>
       </c>
@@ -2584,7 +2617,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>91</v>
       </c>
@@ -2601,7 +2634,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>91</v>
       </c>
@@ -2618,7 +2651,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>91</v>
       </c>
@@ -2635,7 +2668,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>91</v>
       </c>
@@ -2652,7 +2685,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>91</v>
       </c>
@@ -2669,7 +2702,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>91</v>
       </c>
@@ -2686,7 +2719,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>91</v>
       </c>
@@ -2703,7 +2736,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>91</v>
       </c>
@@ -2720,7 +2753,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>91</v>
       </c>
@@ -2737,7 +2770,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>91</v>
       </c>
@@ -2754,7 +2787,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>91</v>
       </c>
@@ -2771,7 +2804,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>104</v>
       </c>
@@ -2788,7 +2821,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
         <v>104</v>
       </c>
@@ -2805,7 +2838,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
         <v>104</v>
       </c>
@@ -2822,7 +2855,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>104</v>
       </c>
@@ -2839,7 +2872,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
         <v>104</v>
       </c>
@@ -2856,7 +2889,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>104</v>
       </c>
@@ -2873,7 +2906,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>104</v>
       </c>
@@ -2890,7 +2923,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>104</v>
       </c>
@@ -2901,18 +2934,18 @@
         <v>10</v>
       </c>
       <c r="D90" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="E90" s="3">
         <v>43830</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>104</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C91" s="2">
         <v>5</v>
@@ -2924,12 +2957,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>104</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C92" s="2">
         <v>22</v>
@@ -2941,12 +2974,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>104</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C93" s="2">
         <v>0</v>
@@ -2958,12 +2991,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>104</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C94" s="2">
         <v>0</v>
@@ -2975,12 +3008,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
+        <v>117</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="C95" s="2">
         <v>5</v>
@@ -2992,12 +3025,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C96" s="2">
         <v>5</v>
@@ -3009,12 +3042,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C97" s="2">
         <v>7</v>
@@ -3026,12 +3059,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C98" s="2">
         <v>10</v>
@@ -3043,12 +3076,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C99" s="2">
         <v>26</v>
@@ -3060,12 +3093,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C100" s="2">
         <v>18</v>
@@ -3077,12 +3110,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C101" s="2">
         <v>0</v>
@@ -3094,12 +3127,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C102" s="2">
         <v>14</v>
@@ -3111,12 +3144,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C103" s="2">
         <v>12</v>
@@ -3128,29 +3161,29 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C104" s="2">
+        <v>13</v>
+      </c>
+      <c r="D104" t="s">
+        <v>19</v>
+      </c>
+      <c r="E104" s="3">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" t="s">
+        <v>117</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="C104" s="2">
-        <v>13</v>
-      </c>
-      <c r="D104" t="s">
-        <v>19</v>
-      </c>
-      <c r="E104" s="3">
-        <v>43830</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>118</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="C105" s="2">
         <v>16</v>
@@ -3162,12 +3195,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C106" s="2">
         <v>0</v>
@@ -3179,12 +3212,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5">
       <c r="A107" t="s">
+        <v>130</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="C107" s="2">
         <v>5</v>
@@ -3196,12 +3229,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C108" s="2">
         <v>13</v>
@@ -3213,12 +3246,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C109" s="2">
         <v>14</v>
@@ -3230,12 +3263,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C110" s="2">
         <v>6</v>
@@ -3247,12 +3280,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C111" s="2">
         <v>6</v>
@@ -3264,12 +3297,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C112" s="2">
         <v>6</v>
@@ -3281,12 +3314,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5">
       <c r="A113" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C113" s="2">
         <v>11</v>
@@ -3298,12 +3331,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5">
       <c r="A114" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C114" s="2">
         <v>1</v>
@@ -3315,12 +3348,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C115" s="2">
         <v>8</v>
@@ -3332,12 +3365,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5">
       <c r="A116" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C116" s="2">
         <v>32</v>
@@ -3349,12 +3382,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5">
       <c r="A117" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C117" s="2">
         <v>28</v>
@@ -3366,12 +3399,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5">
       <c r="A118" t="s">
+        <v>142</v>
+      </c>
+      <c r="B118" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="C118" s="2">
         <v>17</v>
@@ -3383,12 +3416,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5">
       <c r="A119" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C119" s="2">
         <v>19</v>
@@ -3400,12 +3433,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5">
       <c r="A120" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C120" s="2">
         <v>5</v>
@@ -3417,12 +3450,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5">
       <c r="A121" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C121" s="2">
         <v>5</v>
@@ -3434,12 +3467,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5">
       <c r="A122" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C122" s="2">
         <v>33</v>
@@ -3451,12 +3484,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5">
       <c r="A123" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C123" s="2">
         <v>17</v>
@@ -3468,12 +3501,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5">
       <c r="A124" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C124" s="2">
         <v>15</v>
@@ -3485,12 +3518,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5">
       <c r="A125" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C125" s="2">
         <v>12</v>
@@ -3502,12 +3535,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5">
       <c r="A126" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C126" s="2">
         <v>12</v>
@@ -3519,46 +3552,46 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5">
       <c r="A127" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B127" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C127" s="2">
+        <v>13</v>
+      </c>
+      <c r="D127" t="s">
+        <v>19</v>
+      </c>
+      <c r="E127" s="3">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" t="s">
+        <v>142</v>
+      </c>
+      <c r="B128" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="C127" s="2">
-        <v>13</v>
-      </c>
-      <c r="D127" t="s">
-        <v>19</v>
-      </c>
-      <c r="E127" s="3">
-        <v>43830</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>143</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="C128" s="2">
         <v>0</v>
       </c>
       <c r="D128" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="E128" s="3">
         <v>43830</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5">
       <c r="A129" t="s">
+        <v>154</v>
+      </c>
+      <c r="B129" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="C129" s="2">
         <v>12</v>
@@ -3570,12 +3603,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5">
       <c r="A130" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C130" s="2">
         <v>17</v>
@@ -3587,12 +3620,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5">
       <c r="A131" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C131" s="2">
         <v>21</v>
@@ -3604,12 +3637,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5">
       <c r="A132" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C132" s="2">
         <v>12</v>
@@ -3621,12 +3654,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5">
       <c r="A133" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C133" s="2">
         <v>11</v>
@@ -3638,12 +3671,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5">
       <c r="A134" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C134" s="2">
         <v>27</v>
@@ -3655,12 +3688,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5">
       <c r="A135" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C135" s="2">
         <v>1</v>
@@ -3672,12 +3705,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5">
       <c r="A136" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C136" s="2">
         <v>0</v>
@@ -3689,12 +3722,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5">
       <c r="A137" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C137" s="2">
         <v>33</v>
@@ -3706,12 +3739,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5">
       <c r="A138" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C138" s="2">
         <v>12</v>
@@ -3723,12 +3756,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5">
       <c r="A139" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C139" s="2">
         <v>10</v>
@@ -3740,12 +3773,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5">
       <c r="A140" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C140" s="2">
         <v>9</v>
@@ -3757,12 +3790,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5">
       <c r="A141" t="s">
+        <v>167</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="C141" s="2">
         <v>24</v>
@@ -3774,12 +3807,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5">
       <c r="A142" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C142" s="2">
         <v>12</v>
@@ -3791,12 +3824,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5">
       <c r="A143" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C143" s="2">
         <v>5</v>
@@ -3808,12 +3841,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5">
       <c r="A144" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C144" s="2">
         <v>22</v>
@@ -3825,12 +3858,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5">
       <c r="A145" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C145" s="2">
         <v>5</v>
@@ -3842,12 +3875,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5">
       <c r="A146" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C146" s="2">
         <v>32</v>
@@ -3859,12 +3892,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5">
       <c r="A147" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C147" s="2">
         <v>5</v>
@@ -3876,12 +3909,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5">
       <c r="A148" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C148" s="2">
         <v>5</v>
@@ -3893,12 +3926,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5">
       <c r="A149" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C149" s="2">
         <v>15</v>
@@ -3910,12 +3943,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5">
       <c r="A150" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C150" s="2">
         <v>5</v>
@@ -3927,12 +3960,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5">
       <c r="A151" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C151" s="2">
         <v>1</v>
@@ -3944,12 +3977,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5">
       <c r="A152" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C152" s="2">
         <v>0</v>
@@ -3961,12 +3994,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5">
       <c r="A153" t="s">
+        <v>180</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="C153" s="2">
         <v>5</v>
@@ -3978,12 +4011,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5">
       <c r="A154" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C154" s="2">
         <v>5</v>
@@ -3995,12 +4028,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5">
       <c r="A155" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C155" s="2">
         <v>32</v>
@@ -4012,12 +4045,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5">
       <c r="A156" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C156" s="2">
         <v>17</v>
@@ -4029,12 +4062,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5">
       <c r="A157" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C157" s="2">
         <v>9</v>
@@ -4046,12 +4079,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5">
       <c r="A158" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C158" s="2">
         <v>12</v>
@@ -4063,12 +4096,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5">
       <c r="A159" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C159" s="2">
         <v>5</v>
@@ -4080,12 +4113,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5">
       <c r="A160" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C160" s="2">
         <v>9</v>
@@ -4097,12 +4130,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5">
       <c r="A161" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C161" s="2">
         <v>5</v>
@@ -4114,12 +4147,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5">
       <c r="A162" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C162" s="2">
         <v>17</v>
@@ -4131,12 +4164,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5">
       <c r="A163" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C163" s="2">
         <v>0</v>
@@ -4148,12 +4181,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5">
       <c r="A164" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C164" s="2">
         <v>0</v>
@@ -4165,12 +4198,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5">
       <c r="A165" t="s">
+        <v>193</v>
+      </c>
+      <c r="B165" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="C165" s="2">
         <v>6</v>
@@ -4182,12 +4215,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5">
       <c r="A166" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C166" s="2">
         <v>5</v>
@@ -4199,12 +4232,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5">
       <c r="A167" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C167" s="2">
         <v>14</v>
@@ -4216,12 +4249,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5">
       <c r="A168" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C168" s="2">
         <v>6</v>
@@ -4233,12 +4266,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5">
       <c r="A169" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C169" s="2">
         <v>12</v>
@@ -4250,12 +4283,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5">
       <c r="A170" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C170" s="2">
         <v>12</v>
@@ -4267,12 +4300,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5">
       <c r="A171" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C171" s="2">
         <v>6</v>
@@ -4284,12 +4317,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5">
       <c r="A172" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C172" s="2">
         <v>0</v>
@@ -4301,12 +4334,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5">
       <c r="A173" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C173" s="2">
         <v>0</v>
@@ -4318,12 +4351,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5">
       <c r="A174" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C174" s="2">
         <v>15</v>
@@ -4335,12 +4368,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5">
       <c r="A175" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C175" s="2">
         <v>11</v>
@@ -4352,12 +4385,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5">
       <c r="A176" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C176" s="2">
         <v>5</v>
@@ -4369,12 +4402,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5">
       <c r="A177" t="s">
+        <v>206</v>
+      </c>
+      <c r="B177" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="C177" s="2">
         <v>12</v>
@@ -4386,12 +4419,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5">
       <c r="A178" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C178" s="2">
         <v>17</v>
@@ -4403,12 +4436,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5">
       <c r="A179" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C179" s="2">
         <v>17</v>
@@ -4420,12 +4453,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5">
       <c r="A180" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C180" s="2">
         <v>12</v>
@@ -4437,12 +4470,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5">
       <c r="A181" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C181" s="2">
         <v>9</v>
@@ -4454,12 +4487,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5">
       <c r="A182" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C182" s="2">
         <v>8</v>
@@ -4471,12 +4504,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5">
       <c r="A183" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C183" s="2">
         <v>5</v>
@@ -4488,12 +4521,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5">
       <c r="A184" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C184" s="2">
         <v>12</v>
@@ -4505,12 +4538,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5">
       <c r="A185" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C185" s="2">
         <v>27</v>
@@ -4522,12 +4555,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5">
       <c r="A186" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C186" s="2">
         <v>11</v>
@@ -4539,12 +4572,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5">
       <c r="A187" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C187" s="2">
         <v>5</v>
@@ -4556,12 +4589,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5">
       <c r="A188" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C188" s="2">
         <v>9</v>
@@ -4573,12 +4606,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5">
       <c r="A189" t="s">
+        <v>219</v>
+      </c>
+      <c r="B189" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="B189" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="C189" s="2">
         <v>13</v>
@@ -4590,12 +4623,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5">
       <c r="A190" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C190" s="2">
         <v>8</v>
@@ -4607,12 +4640,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5">
       <c r="A191" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C191" s="2">
         <v>14</v>
@@ -4624,12 +4657,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5">
       <c r="A192" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C192" s="2">
         <v>7</v>
@@ -4641,12 +4674,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5">
       <c r="A193" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C193" s="2">
         <v>5</v>
@@ -4658,12 +4691,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5">
       <c r="A194" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C194" s="2">
         <v>6</v>
@@ -4675,12 +4708,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5">
       <c r="A195" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C195" s="2">
         <v>9</v>
@@ -4692,12 +4725,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5">
       <c r="A196" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C196" s="2">
         <v>6</v>
@@ -4709,12 +4742,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5">
       <c r="A197" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C197" s="2">
         <v>8</v>
@@ -4726,12 +4759,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5">
       <c r="A198" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C198" s="2">
         <v>52</v>
@@ -4743,12 +4776,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5">
       <c r="A199" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C199" s="2">
         <v>0</v>
@@ -4760,12 +4793,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5">
       <c r="A200" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C200" s="2">
         <v>2</v>
@@ -4777,12 +4810,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5">
       <c r="A201" t="s">
+        <v>232</v>
+      </c>
+      <c r="B201" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="C201" s="2">
         <v>12</v>
@@ -4794,12 +4827,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5">
       <c r="A202" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C202" s="2">
         <v>9</v>
@@ -4811,12 +4844,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5">
       <c r="A203" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C203" s="2">
         <v>5</v>
@@ -4828,12 +4861,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5">
       <c r="A204" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C204" s="2">
         <v>9</v>
@@ -4845,12 +4878,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5">
       <c r="A205" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C205" s="2">
         <v>5</v>
@@ -4862,12 +4895,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5">
       <c r="A206" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C206" s="2">
         <v>15</v>
@@ -4879,12 +4912,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5">
       <c r="A207" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C207" s="2">
         <v>8</v>
@@ -4896,12 +4929,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5">
       <c r="A208" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C208" s="2">
         <v>0</v>
@@ -4913,12 +4946,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5">
       <c r="A209" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C209" s="2">
         <v>0</v>
@@ -4930,12 +4963,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5">
       <c r="A210" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C210" s="2">
         <v>12</v>
@@ -4947,12 +4980,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5">
       <c r="A211" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C211" s="2">
         <v>5</v>
@@ -4964,12 +4997,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5">
       <c r="A212" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C212" s="2">
         <v>19</v>
@@ -4981,12 +5014,12 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" ht="16.5" customHeight="1">
       <c r="A213" t="s">
         <v>39</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C213" s="2">
         <v>29</v>
@@ -4998,12 +5031,12 @@
         <v>43836</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5">
       <c r="A214" t="s">
         <v>23</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C214" s="2">
         <v>4</v>
@@ -5015,12 +5048,12 @@
         <v>43836</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5">
       <c r="A215" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C215" s="2">
         <v>34</v>
@@ -5032,12 +5065,12 @@
         <v>43836</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5">
       <c r="A216" t="s">
         <v>78</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C216" s="2">
         <v>39</v>
@@ -5049,12 +5082,12 @@
         <v>43836</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5">
       <c r="A217" t="s">
         <v>91</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C217" s="2">
         <v>30</v>
@@ -5066,12 +5099,12 @@
         <v>43836</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5">
       <c r="A218" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C218" s="2">
         <v>6</v>
@@ -5083,12 +5116,12 @@
         <v>43836</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5">
       <c r="A219" t="s">
         <v>23</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C219" s="2">
         <v>19</v>
@@ -5100,12 +5133,12 @@
         <v>43836</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5">
       <c r="A220" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C220" s="2">
         <v>25</v>
@@ -5117,12 +5150,12 @@
         <v>43836</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5">
       <c r="A221" t="s">
         <v>64</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C221" s="2">
         <v>23</v>
@@ -5134,12 +5167,12 @@
         <v>43837</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5">
       <c r="A222" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C222" s="2">
         <v>29</v>
@@ -5151,12 +5184,12 @@
         <v>43837</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5">
       <c r="A223" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C223" s="2">
         <v>10</v>
@@ -5168,12 +5201,12 @@
         <v>43837</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5">
       <c r="A224" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C224" s="2">
         <v>18</v>
@@ -5185,12 +5218,12 @@
         <v>43837</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5">
       <c r="A225" t="s">
         <v>23</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C225" s="2">
         <v>23</v>
@@ -5202,12 +5235,12 @@
         <v>43837</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5">
       <c r="A226" t="s">
         <v>23</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C226" s="2">
         <v>28</v>
@@ -5219,12 +5252,12 @@
         <v>43837</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5">
       <c r="A227" t="s">
         <v>104</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C227" s="2">
         <v>8</v>
@@ -5236,12 +5269,12 @@
         <v>43837</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5">
       <c r="A228" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C228" s="2">
         <v>33</v>
@@ -5253,12 +5286,12 @@
         <v>43837</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5">
       <c r="A229" t="s">
         <v>64</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C229" s="2">
         <v>1</v>
@@ -5270,12 +5303,12 @@
         <v>43838</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5">
       <c r="A230" t="s">
         <v>52</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C230" s="2">
         <v>31</v>
@@ -5287,12 +5320,12 @@
         <v>43838</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5">
       <c r="A231" t="s">
         <v>39</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C231" s="2">
         <v>24</v>
@@ -5304,12 +5337,12 @@
         <v>43838</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5">
       <c r="A232" t="s">
         <v>78</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C232" s="2">
         <v>34</v>
@@ -5321,12 +5354,12 @@
         <v>43838</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5">
       <c r="A233" t="s">
         <v>52</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C233" s="2">
         <v>16</v>
@@ -5338,12 +5371,12 @@
         <v>43838</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5">
       <c r="A234" t="s">
         <v>23</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C234" s="2">
         <v>8</v>
@@ -5355,12 +5388,12 @@
         <v>43838</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5">
       <c r="A235" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C235" s="2">
         <v>24</v>
@@ -5372,12 +5405,12 @@
         <v>43838</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5">
       <c r="A236" t="s">
         <v>23</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C236" s="2">
         <v>8</v>
@@ -5389,12 +5422,12 @@
         <v>43838</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5">
       <c r="A237" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C237" s="2">
         <v>34</v>
@@ -5406,12 +5439,12 @@
         <v>43839</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5">
       <c r="A238" t="s">
         <v>104</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C238" s="2">
         <v>29</v>
@@ -5423,12 +5456,12 @@
         <v>43839</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5">
       <c r="A239" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C239" s="2">
         <v>8</v>
@@ -5440,12 +5473,12 @@
         <v>43839</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5">
       <c r="A240" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C240" s="2">
         <v>20</v>
@@ -5457,12 +5490,12 @@
         <v>43839</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5">
       <c r="A241" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C241" s="2">
         <v>24</v>
@@ -5474,12 +5507,12 @@
         <v>43839</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5">
       <c r="A242" t="s">
         <v>104</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C242" s="2">
         <v>13</v>
@@ -5491,12 +5524,12 @@
         <v>43839</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5">
       <c r="A243" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C243" s="2">
         <v>26</v>
@@ -5508,12 +5541,12 @@
         <v>43839</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5">
       <c r="A244" t="s">
         <v>5</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C244" s="2">
         <v>20</v>
@@ -5525,12 +5558,12 @@
         <v>43839</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5">
       <c r="A245" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C245" s="2">
         <v>15</v>
@@ -5542,12 +5575,12 @@
         <v>43840</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5">
       <c r="A246" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C246" s="2">
         <v>16</v>
@@ -5559,12 +5592,12 @@
         <v>43840</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5">
       <c r="A247" t="s">
         <v>52</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C247" s="2">
         <v>7</v>
@@ -5576,12 +5609,12 @@
         <v>43840</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5">
       <c r="A248" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C248" s="2">
         <v>21</v>
@@ -5593,12 +5626,12 @@
         <v>43840</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5">
       <c r="A249" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C249" s="2">
         <v>22</v>
@@ -5610,12 +5643,12 @@
         <v>43840</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5">
       <c r="A250" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C250" s="2">
         <v>6</v>
@@ -5627,12 +5660,12 @@
         <v>43840</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5">
       <c r="A251" t="s">
         <v>39</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C251" s="2">
         <v>9</v>
@@ -5644,12 +5677,12 @@
         <v>43840</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5">
       <c r="A252" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C252" s="2">
         <v>19</v>
@@ -5661,12 +5694,12 @@
         <v>43840</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5">
       <c r="A253" t="s">
         <v>5</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C253" s="2">
         <v>17</v>
@@ -5678,12 +5711,12 @@
         <v>43843</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5">
       <c r="A254" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C254" s="2">
         <v>8</v>
@@ -5695,12 +5728,12 @@
         <v>43843</v>
       </c>
     </row>
-    <row r="255" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" ht="24" customHeight="1">
       <c r="A255" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C255" s="2">
         <v>17</v>
@@ -5712,12 +5745,12 @@
         <v>43843</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5">
       <c r="A256" t="s">
         <v>52</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C256" s="2">
         <v>13</v>
@@ -5729,12 +5762,12 @@
         <v>43843</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5">
       <c r="A257" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C257" s="2">
         <v>20</v>
@@ -5746,12 +5779,12 @@
         <v>43843</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5">
       <c r="A258" t="s">
         <v>52</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C258" s="2">
         <v>16</v>
@@ -5763,12 +5796,12 @@
         <v>43843</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5">
       <c r="A259" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C259" s="2">
         <v>20</v>
@@ -5780,12 +5813,12 @@
         <v>43843</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5">
       <c r="A260" t="s">
-        <v>131</v>
+        <v>193</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C260" s="2">
         <v>15</v>
@@ -5797,12 +5830,12 @@
         <v>43843</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5">
       <c r="A261" t="s">
         <v>91</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C261" s="2">
         <v>24</v>
@@ -5814,12 +5847,12 @@
         <v>43844</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5">
       <c r="A262" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C262" s="2">
         <v>26</v>
@@ -5831,12 +5864,12 @@
         <v>43844</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5">
       <c r="A263" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C263" s="2">
         <v>35</v>
@@ -5848,12 +5881,12 @@
         <v>43844</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5">
       <c r="A264" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C264" s="2">
         <v>17</v>
@@ -5865,12 +5898,12 @@
         <v>43844</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5">
       <c r="A265" t="s">
         <v>23</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C265" s="2">
         <v>7</v>
@@ -5882,12 +5915,12 @@
         <v>43844</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5">
       <c r="A266" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C266" s="2">
         <v>10</v>
@@ -5899,12 +5932,12 @@
         <v>43844</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5">
       <c r="A267" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C267" s="2">
         <v>27</v>
@@ -5916,12 +5949,12 @@
         <v>43844</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5">
       <c r="A268" t="s">
         <v>104</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C268" s="2">
         <v>16</v>
@@ -5933,12 +5966,12 @@
         <v>43844</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5">
       <c r="A269" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C269" s="2">
         <v>16</v>
@@ -5950,12 +5983,12 @@
         <v>43845</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5">
       <c r="A270" t="s">
         <v>5</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C270" s="2">
         <v>24</v>
@@ -5967,29 +6000,29 @@
         <v>43845</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5">
       <c r="A271" t="s">
         <v>23</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C271" s="2">
         <v>2</v>
       </c>
       <c r="D271" t="s">
-        <v>93</v>
+        <v>11</v>
       </c>
       <c r="E271" s="3">
         <v>43845</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5">
       <c r="A272" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C272" s="2">
         <v>13</v>
@@ -6001,12 +6034,12 @@
         <v>43845</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5">
       <c r="A273" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C273" s="2">
         <v>20</v>
@@ -6018,12 +6051,12 @@
         <v>43845</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5">
       <c r="A274" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C274" s="2">
         <v>9</v>
@@ -6035,12 +6068,12 @@
         <v>43845</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5">
       <c r="A275" t="s">
         <v>91</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C275" s="2">
         <v>7</v>
@@ -6052,12 +6085,12 @@
         <v>43845</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5">
       <c r="A276" t="s">
         <v>104</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C276" s="2">
         <v>5</v>
@@ -6069,12 +6102,12 @@
         <v>43845</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5">
       <c r="A277" t="s">
         <v>91</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C277" s="2">
         <v>15</v>
@@ -6086,12 +6119,12 @@
         <v>43846</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5">
       <c r="A278" t="s">
         <v>52</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C278" s="2">
         <v>2</v>
@@ -6103,12 +6136,12 @@
         <v>43846</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5">
       <c r="A279" t="s">
         <v>91</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C279" s="2">
         <v>16</v>
@@ -6120,12 +6153,12 @@
         <v>43846</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5">
       <c r="A280" t="s">
         <v>39</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C280" s="2">
         <v>19</v>
@@ -6137,12 +6170,12 @@
         <v>43846</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5">
       <c r="A281" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C281" s="2">
         <v>14</v>
@@ -6154,12 +6187,12 @@
         <v>43846</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5">
       <c r="A282" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C282" s="2">
         <v>5</v>
@@ -6171,12 +6204,12 @@
         <v>43846</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5">
       <c r="A283" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C283" s="2">
         <v>17</v>
@@ -6188,12 +6221,12 @@
         <v>43846</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5">
       <c r="A284" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C284" s="2">
         <v>17</v>
@@ -6205,12 +6238,12 @@
         <v>43846</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5">
       <c r="A285" t="s">
         <v>23</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C285" s="2">
         <v>24</v>
@@ -6222,12 +6255,12 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5">
       <c r="A286" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C286" s="2">
         <v>20</v>
@@ -6239,12 +6272,12 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5">
       <c r="A287" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C287" s="2">
         <v>11</v>
@@ -6256,12 +6289,12 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5">
       <c r="A288" t="s">
         <v>78</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C288" s="2">
         <v>11</v>
@@ -6273,12 +6306,12 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5">
       <c r="A289" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C289" s="2">
         <v>13</v>
@@ -6290,12 +6323,12 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5">
       <c r="A290" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C290" s="2">
         <v>8</v>
@@ -6307,12 +6340,12 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5">
       <c r="A291" t="s">
         <v>52</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C291" s="2">
         <v>26</v>
@@ -6324,12 +6357,12 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5">
       <c r="A292" t="s">
         <v>39</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C292" s="2">
         <v>14</v>
@@ -6341,12 +6374,12 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5">
       <c r="A293" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C293" s="2">
         <v>5</v>
@@ -6358,12 +6391,12 @@
         <v>43851</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5">
       <c r="A294" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C294" s="2">
         <v>10</v>
@@ -6375,12 +6408,12 @@
         <v>43851</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5">
       <c r="A295" t="s">
         <v>64</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C295" s="2">
         <v>19</v>
@@ -6392,12 +6425,12 @@
         <v>43851</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5">
       <c r="A296" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C296" s="2">
         <v>4</v>
@@ -6409,12 +6442,12 @@
         <v>43851</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5">
       <c r="A297" t="s">
         <v>64</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C297" s="2">
         <v>26</v>
@@ -6426,12 +6459,12 @@
         <v>43851</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5">
       <c r="A298" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C298" s="2">
         <v>23</v>
@@ -6443,12 +6476,12 @@
         <v>43851</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5">
       <c r="A299" t="s">
         <v>5</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C299" s="2">
         <v>11</v>
@@ -6460,12 +6493,12 @@
         <v>43851</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5">
       <c r="A300" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C300" s="2">
         <v>12</v>
@@ -6477,7 +6510,149 @@
         <v>43851</v>
       </c>
     </row>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" spans="1:5">
+      <c r="A301" t="s">
+        <v>64</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C301" s="2">
+        <v>3</v>
+      </c>
+      <c r="D301" t="s">
+        <v>13</v>
+      </c>
+      <c r="E301" s="3">
+        <v>43852</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5">
+      <c r="A302" t="s">
+        <v>78</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C302" s="2">
+        <v>9</v>
+      </c>
+      <c r="D302" t="s">
+        <v>7</v>
+      </c>
+      <c r="E302" s="3">
+        <v>43852</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5">
+      <c r="A303" t="s">
+        <v>23</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C303" s="2">
+        <v>9</v>
+      </c>
+      <c r="D303" t="s">
+        <v>19</v>
+      </c>
+      <c r="E303" s="3">
+        <v>43852</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5">
+      <c r="A304" t="s">
+        <v>130</v>
+      </c>
+      <c r="B304" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C304" s="2">
+        <v>5</v>
+      </c>
+      <c r="D304" t="s">
+        <v>13</v>
+      </c>
+      <c r="E304" s="3">
+        <v>43852</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5">
+      <c r="A305" t="s">
+        <v>193</v>
+      </c>
+      <c r="B305" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C305" s="2">
+        <v>10</v>
+      </c>
+      <c r="D305" t="s">
+        <v>19</v>
+      </c>
+      <c r="E305" s="3">
+        <v>43852</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5">
+      <c r="A306" t="s">
+        <v>154</v>
+      </c>
+      <c r="B306" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C306" s="2">
+        <v>7</v>
+      </c>
+      <c r="D306" t="s">
+        <v>25</v>
+      </c>
+      <c r="E306" s="3">
+        <v>43852</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5">
+      <c r="A307" t="s">
+        <v>5</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C307" s="2">
+        <v>12</v>
+      </c>
+      <c r="D307" t="s">
+        <v>19</v>
+      </c>
+      <c r="E307" s="3">
+        <v>43852</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5">
+      <c r="A308" t="s">
+        <v>193</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C308" s="2">
+        <v>4</v>
+      </c>
+      <c r="D308" t="s">
+        <v>17</v>
+      </c>
+      <c r="E308" s="3">
+        <v>43852</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5">
+      <c r="B309" s="4"/>
+    </row>
+    <row r="310" spans="1:5">
+      <c r="B310" s="5"/>
+    </row>
+    <row r="362" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6485,102 +6660,102 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
added pecota and more picks
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44656ED-69E8-4FBF-8CBC-306A9DDBE46A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638FA773-3A01-4C21-8611-0DE17F67B0C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6300" yWindow="4764" windowWidth="14172" windowHeight="12204" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="draftpicks" sheetId="1" r:id="rId1"/>
     <sheet name="teams" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="440">
   <si>
     <t>team</t>
   </si>
@@ -1323,6 +1322,30 @@
   </si>
   <si>
     <t>Trent Grisham</t>
+  </si>
+  <si>
+    <t>Kevin Gausman</t>
+  </si>
+  <si>
+    <t>Kevin Pillar</t>
+  </si>
+  <si>
+    <t>Josh Lindblom</t>
+  </si>
+  <si>
+    <t>Austin Hedges</t>
+  </si>
+  <si>
+    <t>Garrett Richards</t>
+  </si>
+  <si>
+    <t>Mike Tauchman</t>
+  </si>
+  <si>
+    <t>Shogo Akiyama</t>
+  </si>
+  <si>
+    <t>Stephen Piscotty</t>
   </si>
 </sst>
 </file>
@@ -1648,10 +1671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E396"/>
+  <dimension ref="A1:E404"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A355" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L384" sqref="L384"/>
+    <sheetView tabSelected="1" topLeftCell="A367" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D404" sqref="D404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8394,6 +8417,142 @@
       </c>
       <c r="E396" s="3">
         <v>43866</v>
+      </c>
+    </row>
+    <row r="397" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A397" t="s">
+        <v>39</v>
+      </c>
+      <c r="B397" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C397" s="2">
+        <v>1</v>
+      </c>
+      <c r="D397" t="s">
+        <v>13</v>
+      </c>
+      <c r="E397" s="3">
+        <v>43867</v>
+      </c>
+    </row>
+    <row r="398" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A398" t="s">
+        <v>217</v>
+      </c>
+      <c r="B398" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C398" s="2">
+        <v>4</v>
+      </c>
+      <c r="D398" t="s">
+        <v>19</v>
+      </c>
+      <c r="E398" s="3">
+        <v>43867</v>
+      </c>
+    </row>
+    <row r="399" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A399" t="s">
+        <v>5</v>
+      </c>
+      <c r="B399" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C399" s="2">
+        <v>1</v>
+      </c>
+      <c r="D399" t="s">
+        <v>25</v>
+      </c>
+      <c r="E399" s="3">
+        <v>43867</v>
+      </c>
+    </row>
+    <row r="400" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A400" t="s">
+        <v>52</v>
+      </c>
+      <c r="B400" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C400" s="2">
+        <v>6</v>
+      </c>
+      <c r="D400" t="s">
+        <v>19</v>
+      </c>
+      <c r="E400" s="3">
+        <v>43867</v>
+      </c>
+    </row>
+    <row r="401" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A401" t="s">
+        <v>91</v>
+      </c>
+      <c r="B401" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C401" s="2">
+        <v>1</v>
+      </c>
+      <c r="D401" t="s">
+        <v>13</v>
+      </c>
+      <c r="E401" s="3">
+        <v>43867</v>
+      </c>
+    </row>
+    <row r="402" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A402" t="s">
+        <v>78</v>
+      </c>
+      <c r="B402" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C402" s="2">
+        <v>5</v>
+      </c>
+      <c r="D402" t="s">
+        <v>13</v>
+      </c>
+      <c r="E402" s="3">
+        <v>43867</v>
+      </c>
+    </row>
+    <row r="403" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A403" t="s">
+        <v>117</v>
+      </c>
+      <c r="B403" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C403" s="2">
+        <v>3</v>
+      </c>
+      <c r="D403" t="s">
+        <v>13</v>
+      </c>
+      <c r="E403" s="3">
+        <v>43867</v>
+      </c>
+    </row>
+    <row r="404" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A404" t="s">
+        <v>52</v>
+      </c>
+      <c r="B404" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C404" s="2">
+        <v>3</v>
+      </c>
+      <c r="D404" t="s">
+        <v>19</v>
+      </c>
+      <c r="E404" s="3">
+        <v>43867</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more picks, updated depth charts
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="456">
   <si>
     <t>team</t>
   </si>
@@ -1369,6 +1369,30 @@
   </si>
   <si>
     <t>Ryne Stanek</t>
+  </si>
+  <si>
+    <t>Seth Lugo</t>
+  </si>
+  <si>
+    <t>Wilmer Flores</t>
+  </si>
+  <si>
+    <t>Clint Frazier</t>
+  </si>
+  <si>
+    <t>Adrian Houser</t>
+  </si>
+  <si>
+    <t>Shed Long</t>
+  </si>
+  <si>
+    <t>Brandon Belt</t>
+  </si>
+  <si>
+    <t>Jasson Dominguez</t>
+  </si>
+  <si>
+    <t>Nick Anderson</t>
   </si>
 </sst>
 </file>
@@ -1694,10 +1718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E412"/>
+  <dimension ref="A1:E420"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A405" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D407" sqref="D407"/>
+    <sheetView tabSelected="1" topLeftCell="A408" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B422" sqref="B422"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1806,7 +1830,7 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E6" s="3">
         <v>43830</v>
@@ -8712,6 +8736,142 @@
       </c>
       <c r="E412" s="3">
         <v>43868</v>
+      </c>
+    </row>
+    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A413" t="s">
+        <v>230</v>
+      </c>
+      <c r="B413" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C413" s="2">
+        <v>1</v>
+      </c>
+      <c r="D413" t="s">
+        <v>70</v>
+      </c>
+      <c r="E413" s="3">
+        <v>43871</v>
+      </c>
+    </row>
+    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A414" t="s">
+        <v>5</v>
+      </c>
+      <c r="B414" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="C414" s="2">
+        <v>3</v>
+      </c>
+      <c r="D414" t="s">
+        <v>13</v>
+      </c>
+      <c r="E414" s="3">
+        <v>43871</v>
+      </c>
+    </row>
+    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A415" t="s">
+        <v>217</v>
+      </c>
+      <c r="B415" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C415" s="2">
+        <v>5</v>
+      </c>
+      <c r="D415" t="s">
+        <v>19</v>
+      </c>
+      <c r="E415" s="3">
+        <v>43871</v>
+      </c>
+    </row>
+    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>117</v>
+      </c>
+      <c r="B416" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C416" s="2">
+        <v>2</v>
+      </c>
+      <c r="D416" t="s">
+        <v>13</v>
+      </c>
+      <c r="E416" s="3">
+        <v>43871</v>
+      </c>
+    </row>
+    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A417" t="s">
+        <v>117</v>
+      </c>
+      <c r="B417" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C417" s="2">
+        <v>2</v>
+      </c>
+      <c r="D417" t="s">
+        <v>11</v>
+      </c>
+      <c r="E417" s="3">
+        <v>43871</v>
+      </c>
+    </row>
+    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
+        <v>217</v>
+      </c>
+      <c r="B418" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C418" s="2">
+        <v>1</v>
+      </c>
+      <c r="D418" t="s">
+        <v>17</v>
+      </c>
+      <c r="E418" s="3">
+        <v>43871</v>
+      </c>
+    </row>
+    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>230</v>
+      </c>
+      <c r="B419" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C419" s="2">
+        <v>13</v>
+      </c>
+      <c r="D419" t="s">
+        <v>19</v>
+      </c>
+      <c r="E419" s="3">
+        <v>43871</v>
+      </c>
+    </row>
+    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A420" t="s">
+        <v>39</v>
+      </c>
+      <c r="B420" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C420" s="2">
+        <v>3</v>
+      </c>
+      <c r="D420" t="s">
+        <v>19</v>
+      </c>
+      <c r="E420" s="3">
+        <v>43871</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more picks, refreshed projections
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F44987-AD0E-4FB4-93D4-368552BF91C4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6817AF-4B7B-4EFD-801D-74B6BDB7053F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6840" yWindow="4464" windowWidth="14172" windowHeight="12204" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4464" windowWidth="14172" windowHeight="12204" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="draftpicks" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="497">
   <si>
     <t>team</t>
   </si>
@@ -1466,6 +1466,57 @@
   </si>
   <si>
     <t>Jordan Hicks</t>
+  </si>
+  <si>
+    <t>Albert Pujols</t>
+  </si>
+  <si>
+    <t>Wade Davis</t>
+  </si>
+  <si>
+    <t>Austin Romine</t>
+  </si>
+  <si>
+    <t>Jake Bauers</t>
+  </si>
+  <si>
+    <t>Dexter Fowler</t>
+  </si>
+  <si>
+    <t>Mike Fiers</t>
+  </si>
+  <si>
+    <t>Daniel Hudson</t>
+  </si>
+  <si>
+    <t>Rich Hill</t>
+  </si>
+  <si>
+    <t>Chad Green</t>
+  </si>
+  <si>
+    <t>Seranthony Dominguez</t>
+  </si>
+  <si>
+    <t>Andres Munoz</t>
+  </si>
+  <si>
+    <t>Stephen Vogt</t>
+  </si>
+  <si>
+    <t>Luis Urias</t>
+  </si>
+  <si>
+    <t>Jordan Montgomery</t>
+  </si>
+  <si>
+    <t>Ryan Mountcastle</t>
+  </si>
+  <si>
+    <t>Rowan Wick</t>
+  </si>
+  <si>
+    <t>Todd Frazier</t>
   </si>
 </sst>
 </file>
@@ -1791,10 +1842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E444"/>
+  <dimension ref="A1:E463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A408" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B445" sqref="B445"/>
+    <sheetView tabSelected="1" topLeftCell="A440" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A461" sqref="A461"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9354,6 +9405,298 @@
       <c r="E444" s="3">
         <v>43874</v>
       </c>
+    </row>
+    <row r="445" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A445" t="s">
+        <v>78</v>
+      </c>
+      <c r="B445" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="C445" s="2">
+        <v>1</v>
+      </c>
+      <c r="D445" t="s">
+        <v>93</v>
+      </c>
+      <c r="E445" s="3">
+        <v>43875</v>
+      </c>
+    </row>
+    <row r="446" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A446" t="s">
+        <v>230</v>
+      </c>
+      <c r="B446" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="C446" s="2">
+        <v>7</v>
+      </c>
+      <c r="D446" t="s">
+        <v>19</v>
+      </c>
+      <c r="E446" s="3">
+        <v>43875</v>
+      </c>
+    </row>
+    <row r="447" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A447" t="s">
+        <v>91</v>
+      </c>
+      <c r="B447" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C447" s="2">
+        <v>5</v>
+      </c>
+      <c r="D447" t="s">
+        <v>25</v>
+      </c>
+      <c r="E447" s="3">
+        <v>43875</v>
+      </c>
+    </row>
+    <row r="448" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A448" t="s">
+        <v>154</v>
+      </c>
+      <c r="B448" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="C448" s="2">
+        <v>1</v>
+      </c>
+      <c r="D448" t="s">
+        <v>11</v>
+      </c>
+      <c r="E448" s="3">
+        <v>43875</v>
+      </c>
+    </row>
+    <row r="449" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A449" t="s">
+        <v>117</v>
+      </c>
+      <c r="B449" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="C449" s="2">
+        <v>2</v>
+      </c>
+      <c r="D449" t="s">
+        <v>17</v>
+      </c>
+      <c r="E449" s="3">
+        <v>43875</v>
+      </c>
+    </row>
+    <row r="450" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A450" t="s">
+        <v>204</v>
+      </c>
+      <c r="B450" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="C450" s="2">
+        <v>1</v>
+      </c>
+      <c r="D450" t="s">
+        <v>19</v>
+      </c>
+      <c r="E450" s="3">
+        <v>43875</v>
+      </c>
+    </row>
+    <row r="451" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A451" t="s">
+        <v>142</v>
+      </c>
+      <c r="B451" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="C451" s="2">
+        <v>1</v>
+      </c>
+      <c r="D451" t="s">
+        <v>19</v>
+      </c>
+      <c r="E451" s="3">
+        <v>43875</v>
+      </c>
+    </row>
+    <row r="452" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A452" t="s">
+        <v>104</v>
+      </c>
+      <c r="B452" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="C452" s="2">
+        <v>1</v>
+      </c>
+      <c r="D452" t="s">
+        <v>19</v>
+      </c>
+      <c r="E452" s="3">
+        <v>43875</v>
+      </c>
+    </row>
+    <row r="453" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A453" t="s">
+        <v>117</v>
+      </c>
+      <c r="B453" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C453" s="2">
+        <v>2</v>
+      </c>
+      <c r="D453" t="s">
+        <v>19</v>
+      </c>
+      <c r="E453" s="3">
+        <v>43876</v>
+      </c>
+    </row>
+    <row r="454" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A454" t="s">
+        <v>117</v>
+      </c>
+      <c r="B454" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="C454" s="2">
+        <v>1</v>
+      </c>
+      <c r="D454" t="s">
+        <v>19</v>
+      </c>
+      <c r="E454" s="3">
+        <v>43876</v>
+      </c>
+    </row>
+    <row r="455" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A455" t="s">
+        <v>39</v>
+      </c>
+      <c r="B455" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C455" s="2">
+        <v>1</v>
+      </c>
+      <c r="D455" t="s">
+        <v>19</v>
+      </c>
+      <c r="E455" s="3">
+        <v>43876</v>
+      </c>
+    </row>
+    <row r="456" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A456" t="s">
+        <v>230</v>
+      </c>
+      <c r="B456" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="C456" s="2">
+        <v>1</v>
+      </c>
+      <c r="D456" t="s">
+        <v>25</v>
+      </c>
+      <c r="E456" s="3">
+        <v>43876</v>
+      </c>
+    </row>
+    <row r="457" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A457" t="s">
+        <v>167</v>
+      </c>
+      <c r="B457" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C457" s="2">
+        <v>1</v>
+      </c>
+      <c r="D457" t="s">
+        <v>19</v>
+      </c>
+      <c r="E457" s="3">
+        <v>43876</v>
+      </c>
+    </row>
+    <row r="458" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A458" t="s">
+        <v>91</v>
+      </c>
+      <c r="B458" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C458" s="2">
+        <v>1</v>
+      </c>
+      <c r="D458" t="s">
+        <v>19</v>
+      </c>
+      <c r="E458" s="3">
+        <v>43876</v>
+      </c>
+    </row>
+    <row r="459" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A459" t="s">
+        <v>78</v>
+      </c>
+      <c r="B459" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="C459" s="2">
+        <v>3</v>
+      </c>
+      <c r="D459" t="s">
+        <v>11</v>
+      </c>
+      <c r="E459" s="3">
+        <v>43876</v>
+      </c>
+    </row>
+    <row r="460" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A460" t="s">
+        <v>217</v>
+      </c>
+      <c r="B460" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="C460" s="2">
+        <v>1</v>
+      </c>
+      <c r="D460" t="s">
+        <v>19</v>
+      </c>
+      <c r="E460" s="3">
+        <v>43876</v>
+      </c>
+    </row>
+    <row r="461" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A461" t="s">
+        <v>230</v>
+      </c>
+      <c r="B461" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="C461" s="2">
+        <v>2</v>
+      </c>
+      <c r="D461" t="s">
+        <v>93</v>
+      </c>
+      <c r="E461" s="3">
+        <v>43877</v>
+      </c>
+    </row>
+    <row r="463" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A463" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
more projection systems. start of bench draft
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AE3AA2-D81B-436B-8B9A-AFE86076CC52}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4288E5C6-08B2-4A96-A563-1A08FEAD14EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4464" windowWidth="14172" windowHeight="12204" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6768" yWindow="1152" windowWidth="14172" windowHeight="11052" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="draftpicks" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="558">
   <si>
     <t>team</t>
   </si>
@@ -1417,9 +1417,6 @@
     <t>Justin Smoak</t>
   </si>
   <si>
-    <t>Josh James</t>
-  </si>
-  <si>
     <t xml:space="preserve">Freddy Peralta </t>
   </si>
   <si>
@@ -1580,6 +1577,129 @@
   </si>
   <si>
     <t>Raimel Tapia</t>
+  </si>
+  <si>
+    <t>Joshua James</t>
+  </si>
+  <si>
+    <t>Christian Pache</t>
+  </si>
+  <si>
+    <t>Oneil Cruz</t>
+  </si>
+  <si>
+    <t>CJ Abrams</t>
+  </si>
+  <si>
+    <t>Jurickson Profar</t>
+  </si>
+  <si>
+    <t>Miguel Cabrera</t>
+  </si>
+  <si>
+    <t>Rowdy Tellez</t>
+  </si>
+  <si>
+    <t>Drew Waters</t>
+  </si>
+  <si>
+    <t>Adam Haseley</t>
+  </si>
+  <si>
+    <t>Nicky Lopez</t>
+  </si>
+  <si>
+    <t>Emmanuel Clase</t>
+  </si>
+  <si>
+    <t>Bobby Witt Jr.</t>
+  </si>
+  <si>
+    <t>Franklin Barreto</t>
+  </si>
+  <si>
+    <t>Brendan Rodgers</t>
+  </si>
+  <si>
+    <t>Zach Plesac</t>
+  </si>
+  <si>
+    <t>Kyle Wright</t>
+  </si>
+  <si>
+    <t>Blake Treinen</t>
+  </si>
+  <si>
+    <t>JJ Bleday</t>
+  </si>
+  <si>
+    <t>Sheldon Neuse</t>
+  </si>
+  <si>
+    <t>Alex Gordon</t>
+  </si>
+  <si>
+    <t>Nico Hoerner</t>
+  </si>
+  <si>
+    <t>Adbert Alzolay</t>
+  </si>
+  <si>
+    <t>PLACEHOLDER</t>
+  </si>
+  <si>
+    <t>Jose Alvarado</t>
+  </si>
+  <si>
+    <t>Lewis Thorpe</t>
+  </si>
+  <si>
+    <t>Jeter Downs</t>
+  </si>
+  <si>
+    <t>Spencer Turnbull</t>
+  </si>
+  <si>
+    <t>Asdrubal Cabrera</t>
+  </si>
+  <si>
+    <t>Nolan Jones</t>
+  </si>
+  <si>
+    <t>Austin Voth</t>
+  </si>
+  <si>
+    <t>Brian Goodwin</t>
+  </si>
+  <si>
+    <t>Mitch Moreland</t>
+  </si>
+  <si>
+    <t>Isan Diaz</t>
+  </si>
+  <si>
+    <t>Leury Garcia</t>
+  </si>
+  <si>
+    <t>Nick Markakis</t>
+  </si>
+  <si>
+    <t>Shaun Anderson</t>
+  </si>
+  <si>
+    <t>Lane Thomas</t>
+  </si>
+  <si>
+    <t>Josiah Gray</t>
+  </si>
+  <si>
+    <t>Corbin Burnes</t>
+  </si>
+  <si>
+    <t>Garrett Cooper</t>
+  </si>
+  <si>
+    <t>Collin McHugh</t>
   </si>
 </sst>
 </file>
@@ -1905,10 +2025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E482"/>
+  <dimension ref="A1:E523"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A318" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D330" sqref="D330"/>
+    <sheetView tabSelected="1" topLeftCell="A487" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G498" sqref="G498"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9168,7 +9288,7 @@
         <v>167</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>463</v>
+        <v>517</v>
       </c>
       <c r="C427" s="2">
         <v>5</v>
@@ -9202,7 +9322,7 @@
         <v>167</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C429" s="2">
         <v>1</v>
@@ -9219,7 +9339,7 @@
         <v>91</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C430" s="2">
         <v>1</v>
@@ -9236,7 +9356,7 @@
         <v>167</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C431" s="2">
         <v>5</v>
@@ -9253,7 +9373,7 @@
         <v>217</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C432" s="2">
         <v>1</v>
@@ -9270,7 +9390,7 @@
         <v>52</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C433" s="2">
         <v>1</v>
@@ -9287,7 +9407,7 @@
         <v>91</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C434" s="2">
         <v>2</v>
@@ -9304,7 +9424,7 @@
         <v>154</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C435" s="2">
         <v>3</v>
@@ -9321,7 +9441,7 @@
         <v>23</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C436" s="2">
         <v>1</v>
@@ -9338,7 +9458,7 @@
         <v>204</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C437" s="2">
         <v>1</v>
@@ -9355,7 +9475,7 @@
         <v>142</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C438" s="2">
         <v>2</v>
@@ -9372,7 +9492,7 @@
         <v>142</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C439" s="2">
         <v>2</v>
@@ -9389,7 +9509,7 @@
         <v>117</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C440" s="2">
         <v>1</v>
@@ -9406,7 +9526,7 @@
         <v>39</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C441" s="2">
         <v>1</v>
@@ -9423,7 +9543,7 @@
         <v>167</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C442" s="2">
         <v>3</v>
@@ -9440,7 +9560,7 @@
         <v>167</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C443" s="2">
         <v>3</v>
@@ -9457,7 +9577,7 @@
         <v>91</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C444" s="2">
         <v>1</v>
@@ -9474,7 +9594,7 @@
         <v>78</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C445" s="2">
         <v>1</v>
@@ -9491,7 +9611,7 @@
         <v>230</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C446" s="2">
         <v>7</v>
@@ -9508,7 +9628,7 @@
         <v>91</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C447" s="2">
         <v>5</v>
@@ -9525,7 +9645,7 @@
         <v>154</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C448" s="2">
         <v>1</v>
@@ -9542,7 +9662,7 @@
         <v>117</v>
       </c>
       <c r="B449" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C449" s="2">
         <v>2</v>
@@ -9559,7 +9679,7 @@
         <v>204</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C450" s="2">
         <v>1</v>
@@ -9576,7 +9696,7 @@
         <v>142</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C451" s="2">
         <v>1</v>
@@ -9593,7 +9713,7 @@
         <v>104</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C452" s="2">
         <v>1</v>
@@ -9610,7 +9730,7 @@
         <v>117</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C453" s="2">
         <v>2</v>
@@ -9627,7 +9747,7 @@
         <v>117</v>
       </c>
       <c r="B454" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C454" s="2">
         <v>1</v>
@@ -9644,7 +9764,7 @@
         <v>39</v>
       </c>
       <c r="B455" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C455" s="2">
         <v>1</v>
@@ -9661,7 +9781,7 @@
         <v>230</v>
       </c>
       <c r="B456" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C456" s="2">
         <v>1</v>
@@ -9678,7 +9798,7 @@
         <v>167</v>
       </c>
       <c r="B457" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C457" s="2">
         <v>1</v>
@@ -9695,7 +9815,7 @@
         <v>91</v>
       </c>
       <c r="B458" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C458" s="2">
         <v>1</v>
@@ -9712,7 +9832,7 @@
         <v>78</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C459" s="2">
         <v>3</v>
@@ -9729,7 +9849,7 @@
         <v>217</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C460" s="2">
         <v>1</v>
@@ -9746,7 +9866,7 @@
         <v>230</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C461" s="2">
         <v>2</v>
@@ -9763,7 +9883,7 @@
         <v>130</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C462" s="2">
         <v>1</v>
@@ -9780,7 +9900,7 @@
         <v>154</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C463" s="2">
         <v>2</v>
@@ -9797,7 +9917,7 @@
         <v>23</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C464" s="2">
         <v>1</v>
@@ -9814,7 +9934,7 @@
         <v>142</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C465" s="2">
         <v>1</v>
@@ -9831,7 +9951,7 @@
         <v>117</v>
       </c>
       <c r="B466" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C466" s="2">
         <v>1</v>
@@ -9848,7 +9968,7 @@
         <v>39</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C467" s="2">
         <v>1</v>
@@ -9865,7 +9985,7 @@
         <v>91</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C468" s="2">
         <v>3</v>
@@ -9882,7 +10002,7 @@
         <v>78</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C469" s="2">
         <v>1</v>
@@ -9899,7 +10019,7 @@
         <v>217</v>
       </c>
       <c r="B470" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C470" s="2">
         <v>1</v>
@@ -9916,7 +10036,7 @@
         <v>104</v>
       </c>
       <c r="B471" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C471" s="2">
         <v>1</v>
@@ -9933,7 +10053,7 @@
         <v>130</v>
       </c>
       <c r="B472" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C472" s="2">
         <v>1</v>
@@ -9950,7 +10070,7 @@
         <v>39</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C473" s="2">
         <v>1</v>
@@ -9967,7 +10087,7 @@
         <v>104</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C474" s="2">
         <v>1</v>
@@ -9984,7 +10104,7 @@
         <v>78</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C475" s="2">
         <v>1</v>
@@ -10001,7 +10121,7 @@
         <v>130</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C476" s="2">
         <v>1</v>
@@ -10018,7 +10138,7 @@
         <v>130</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C477" s="2">
         <v>1</v>
@@ -10035,7 +10155,7 @@
         <v>104</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C478" s="2">
         <v>1</v>
@@ -10052,7 +10172,7 @@
         <v>104</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C479" s="2">
         <v>1</v>
@@ -10069,7 +10189,7 @@
         <v>104</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C480" s="2">
         <v>1</v>
@@ -10086,7 +10206,7 @@
         <v>104</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C481" s="2">
         <v>1</v>
@@ -10103,7 +10223,7 @@
         <v>104</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C482" s="2">
         <v>1</v>
@@ -10113,6 +10233,703 @@
       </c>
       <c r="E482" s="3">
         <v>43877</v>
+      </c>
+    </row>
+    <row r="483" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A483" t="s">
+        <v>91</v>
+      </c>
+      <c r="B483" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="C483" s="2">
+        <v>0</v>
+      </c>
+      <c r="D483" t="s">
+        <v>34</v>
+      </c>
+      <c r="E483" s="3">
+        <v>43878</v>
+      </c>
+    </row>
+    <row r="484" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A484" t="s">
+        <v>52</v>
+      </c>
+      <c r="B484" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="C484" s="2">
+        <v>0</v>
+      </c>
+      <c r="D484" t="s">
+        <v>34</v>
+      </c>
+      <c r="E484" s="3">
+        <v>43878</v>
+      </c>
+    </row>
+    <row r="485" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A485" t="s">
+        <v>5</v>
+      </c>
+      <c r="B485" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C485" s="2">
+        <v>0</v>
+      </c>
+      <c r="D485" t="s">
+        <v>34</v>
+      </c>
+      <c r="E485" s="3">
+        <v>43878</v>
+      </c>
+    </row>
+    <row r="486" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A486" t="s">
+        <v>78</v>
+      </c>
+      <c r="B486" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C486" s="2">
+        <v>0</v>
+      </c>
+      <c r="D486" t="s">
+        <v>34</v>
+      </c>
+      <c r="E486" s="3">
+        <v>43878</v>
+      </c>
+    </row>
+    <row r="487" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A487" t="s">
+        <v>130</v>
+      </c>
+      <c r="B487" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="C487" s="2">
+        <v>0</v>
+      </c>
+      <c r="D487" t="s">
+        <v>34</v>
+      </c>
+      <c r="E487" s="3">
+        <v>43878</v>
+      </c>
+    </row>
+    <row r="488" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A488" t="s">
+        <v>64</v>
+      </c>
+      <c r="B488" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="C488" s="2">
+        <v>0</v>
+      </c>
+      <c r="D488" t="s">
+        <v>34</v>
+      </c>
+      <c r="E488" s="3">
+        <v>43878</v>
+      </c>
+    </row>
+    <row r="489" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A489" t="s">
+        <v>230</v>
+      </c>
+      <c r="B489" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="C489" s="2">
+        <v>0</v>
+      </c>
+      <c r="D489" t="s">
+        <v>34</v>
+      </c>
+      <c r="E489" s="3">
+        <v>43878</v>
+      </c>
+    </row>
+    <row r="490" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A490" t="s">
+        <v>217</v>
+      </c>
+      <c r="B490" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="C490" s="2">
+        <v>0</v>
+      </c>
+      <c r="D490" t="s">
+        <v>34</v>
+      </c>
+      <c r="E490" s="3">
+        <v>43878</v>
+      </c>
+    </row>
+    <row r="491" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A491" t="s">
+        <v>204</v>
+      </c>
+      <c r="B491" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="C491" s="2">
+        <v>0</v>
+      </c>
+      <c r="D491" t="s">
+        <v>34</v>
+      </c>
+      <c r="E491" s="3">
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="492" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A492" t="s">
+        <v>217</v>
+      </c>
+      <c r="B492" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="C492" s="2">
+        <v>0</v>
+      </c>
+      <c r="D492" t="s">
+        <v>34</v>
+      </c>
+      <c r="E492" s="3">
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="493" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A493" t="s">
+        <v>204</v>
+      </c>
+      <c r="B493" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C493" s="2">
+        <v>0</v>
+      </c>
+      <c r="D493" t="s">
+        <v>34</v>
+      </c>
+      <c r="E493" s="3">
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="494" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A494" t="s">
+        <v>78</v>
+      </c>
+      <c r="B494" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="C494" s="2">
+        <v>0</v>
+      </c>
+      <c r="D494" t="s">
+        <v>34</v>
+      </c>
+      <c r="E494" s="3">
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="495" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A495" t="s">
+        <v>104</v>
+      </c>
+      <c r="B495" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C495" s="2">
+        <v>0</v>
+      </c>
+      <c r="D495" t="s">
+        <v>34</v>
+      </c>
+      <c r="E495" s="3">
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="496" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A496" t="s">
+        <v>39</v>
+      </c>
+      <c r="B496" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="C496" s="2">
+        <v>0</v>
+      </c>
+      <c r="D496" t="s">
+        <v>34</v>
+      </c>
+      <c r="E496" s="3">
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="497" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A497" t="s">
+        <v>154</v>
+      </c>
+      <c r="B497" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="C497" s="2">
+        <v>0</v>
+      </c>
+      <c r="D497" t="s">
+        <v>34</v>
+      </c>
+      <c r="E497" s="3">
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="498" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A498" t="s">
+        <v>167</v>
+      </c>
+      <c r="B498" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="C498" s="2">
+        <v>0</v>
+      </c>
+      <c r="D498" t="s">
+        <v>34</v>
+      </c>
+      <c r="E498" s="3">
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="499" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A499" t="s">
+        <v>117</v>
+      </c>
+      <c r="B499" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="C499" s="2">
+        <v>0</v>
+      </c>
+      <c r="D499" t="s">
+        <v>34</v>
+      </c>
+      <c r="E499" s="3">
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="500" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A500" t="s">
+        <v>5</v>
+      </c>
+      <c r="B500" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="C500" s="2">
+        <v>0</v>
+      </c>
+      <c r="D500" t="s">
+        <v>34</v>
+      </c>
+      <c r="E500" s="3">
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="501" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A501" t="s">
+        <v>204</v>
+      </c>
+      <c r="B501" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="C501" s="2">
+        <v>0</v>
+      </c>
+      <c r="D501" t="s">
+        <v>34</v>
+      </c>
+      <c r="E501" s="3">
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="502" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A502" t="s">
+        <v>204</v>
+      </c>
+      <c r="B502" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C502" s="2">
+        <v>0</v>
+      </c>
+      <c r="D502" t="s">
+        <v>34</v>
+      </c>
+      <c r="E502" s="3">
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="503" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A503" t="s">
+        <v>117</v>
+      </c>
+      <c r="B503" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="C503" s="2">
+        <v>0</v>
+      </c>
+      <c r="D503" t="s">
+        <v>34</v>
+      </c>
+      <c r="E503" s="3">
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="504" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A504" t="s">
+        <v>52</v>
+      </c>
+      <c r="B504" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C504" s="2">
+        <v>0</v>
+      </c>
+      <c r="D504" t="s">
+        <v>34</v>
+      </c>
+      <c r="E504" s="3">
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="505" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A505" t="s">
+        <v>91</v>
+      </c>
+      <c r="B505" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="C505" s="2">
+        <v>0</v>
+      </c>
+      <c r="D505" t="s">
+        <v>34</v>
+      </c>
+      <c r="E505" s="3">
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="506" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A506" t="s">
+        <v>91</v>
+      </c>
+      <c r="B506" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="C506" s="2">
+        <v>0</v>
+      </c>
+      <c r="D506" t="s">
+        <v>34</v>
+      </c>
+      <c r="E506" s="3">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="507" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A507" t="s">
+        <v>52</v>
+      </c>
+      <c r="B507" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="C507" s="2">
+        <v>0</v>
+      </c>
+      <c r="D507" t="s">
+        <v>34</v>
+      </c>
+      <c r="E507" s="3">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="508" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A508" t="s">
+        <v>78</v>
+      </c>
+      <c r="B508" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="C508" s="2">
+        <v>0</v>
+      </c>
+      <c r="D508" t="s">
+        <v>34</v>
+      </c>
+      <c r="E508" s="3">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="509" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A509" t="s">
+        <v>230</v>
+      </c>
+      <c r="B509" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="C509" s="2">
+        <v>0</v>
+      </c>
+      <c r="D509" t="s">
+        <v>34</v>
+      </c>
+      <c r="E509" s="3">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="510" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A510" t="s">
+        <v>204</v>
+      </c>
+      <c r="B510" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="C510" s="2">
+        <v>0</v>
+      </c>
+      <c r="D510" t="s">
+        <v>34</v>
+      </c>
+      <c r="E510" s="3">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="511" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A511" t="s">
+        <v>5</v>
+      </c>
+      <c r="B511" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="C511" s="2">
+        <v>0</v>
+      </c>
+      <c r="D511" t="s">
+        <v>34</v>
+      </c>
+      <c r="E511" s="3">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="512" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A512" t="s">
+        <v>117</v>
+      </c>
+      <c r="B512" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="C512" s="2">
+        <v>0</v>
+      </c>
+      <c r="D512" t="s">
+        <v>34</v>
+      </c>
+      <c r="E512" s="3">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="513" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A513" t="s">
+        <v>204</v>
+      </c>
+      <c r="B513" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="C513" s="2">
+        <v>0</v>
+      </c>
+      <c r="D513" t="s">
+        <v>34</v>
+      </c>
+      <c r="E513" s="3">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="514" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A514" t="s">
+        <v>154</v>
+      </c>
+      <c r="B514" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C514" s="2">
+        <v>0</v>
+      </c>
+      <c r="D514" t="s">
+        <v>34</v>
+      </c>
+      <c r="E514" s="3">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="515" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A515" t="s">
+        <v>39</v>
+      </c>
+      <c r="B515" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C515" s="2">
+        <v>0</v>
+      </c>
+      <c r="D515" t="s">
+        <v>34</v>
+      </c>
+      <c r="E515" s="3">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="516" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A516" t="s">
+        <v>23</v>
+      </c>
+      <c r="B516" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="C516" s="2">
+        <v>0</v>
+      </c>
+      <c r="D516" t="s">
+        <v>34</v>
+      </c>
+      <c r="E516" s="3">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="517" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A517" t="s">
+        <v>104</v>
+      </c>
+      <c r="B517" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="C517" s="2">
+        <v>0</v>
+      </c>
+      <c r="D517" t="s">
+        <v>34</v>
+      </c>
+      <c r="E517" s="3">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="518" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A518" t="s">
+        <v>204</v>
+      </c>
+      <c r="B518" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="C518" s="2">
+        <v>0</v>
+      </c>
+      <c r="D518" t="s">
+        <v>34</v>
+      </c>
+      <c r="E518" s="3">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="519" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A519" t="s">
+        <v>117</v>
+      </c>
+      <c r="B519" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="C519" s="2">
+        <v>0</v>
+      </c>
+      <c r="D519" t="s">
+        <v>34</v>
+      </c>
+      <c r="E519" s="3">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="520" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A520" t="s">
+        <v>192</v>
+      </c>
+      <c r="B520" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="C520" s="2">
+        <v>0</v>
+      </c>
+      <c r="D520" t="s">
+        <v>34</v>
+      </c>
+      <c r="E520" s="3">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="521" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A521" t="s">
+        <v>230</v>
+      </c>
+      <c r="B521" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="C521" s="2">
+        <v>0</v>
+      </c>
+      <c r="D521" t="s">
+        <v>34</v>
+      </c>
+      <c r="E521" s="3">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="522" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A522" t="s">
+        <v>167</v>
+      </c>
+      <c r="B522" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="C522" s="2">
+        <v>0</v>
+      </c>
+      <c r="D522" t="s">
+        <v>34</v>
+      </c>
+      <c r="E522" s="3">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="523" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A523" t="s">
+        <v>64</v>
+      </c>
+      <c r="B523" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="C523" s="2">
+        <v>0</v>
+      </c>
+      <c r="D523" t="s">
+        <v>34</v>
+      </c>
+      <c r="E523" s="3">
+        <v>43880</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a few more picks and corrections
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seana\Documents\rprojects\fantasy2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5071A33B-6743-4055-99D7-B38166D4D637}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05E4D2B-C70B-40E6-8672-A418F6D2CDB5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6768" yWindow="1152" windowWidth="14172" windowHeight="11052" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="627">
   <si>
     <t>team</t>
   </si>
@@ -985,9 +985,6 @@
     <t>Kyle Hendricks</t>
   </si>
   <si>
-    <t>Kwang-Hyun Kim</t>
-  </si>
-  <si>
     <t>Nelson Cruz</t>
   </si>
   <si>
@@ -1519,9 +1516,6 @@
     <t>Adam Ottavino</t>
   </si>
   <si>
-    <t>Brad Keller </t>
-  </si>
-  <si>
     <t>Christin Stewart</t>
   </si>
   <si>
@@ -1765,9 +1759,6 @@
     <t>Logan Gilbert</t>
   </si>
   <si>
-    <t>Jake Junis</t>
-  </si>
-  <si>
     <t>Trevor May</t>
   </si>
   <si>
@@ -1898,6 +1889,24 @@
   </si>
   <si>
     <t>Patrick Sandoval</t>
+  </si>
+  <si>
+    <t>Brad Keller</t>
+  </si>
+  <si>
+    <t>Jakob Junis</t>
+  </si>
+  <si>
+    <t>Kwang-hyun Kim</t>
+  </si>
+  <si>
+    <t>Pedro Baez</t>
+  </si>
+  <si>
+    <t>Luis Campusano</t>
+  </si>
+  <si>
+    <t>Andy Young</t>
   </si>
 </sst>
 </file>
@@ -2225,8 +2234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E595"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A525" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F536" sqref="F536"/>
+    <sheetView tabSelected="1" topLeftCell="A576" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B592" sqref="B592"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4845,7 +4854,7 @@
         <v>180</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C154" s="2">
         <v>5</v>
@@ -5083,7 +5092,7 @@
         <v>192</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C168" s="2">
         <v>6</v>
@@ -7157,7 +7166,7 @@
         <v>192</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>319</v>
+        <v>623</v>
       </c>
       <c r="C290" s="2">
         <v>8</v>
@@ -7174,7 +7183,7 @@
         <v>52</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C291" s="2">
         <v>26</v>
@@ -7191,7 +7200,7 @@
         <v>39</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C292" s="2">
         <v>14</v>
@@ -7208,7 +7217,7 @@
         <v>130</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C293" s="2">
         <v>5</v>
@@ -7225,7 +7234,7 @@
         <v>167</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C294" s="2">
         <v>10</v>
@@ -7242,7 +7251,7 @@
         <v>64</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C295" s="2">
         <v>19</v>
@@ -7259,7 +7268,7 @@
         <v>154</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C296" s="2">
         <v>4</v>
@@ -7276,7 +7285,7 @@
         <v>64</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C297" s="2">
         <v>26</v>
@@ -7293,7 +7302,7 @@
         <v>117</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C298" s="2">
         <v>23</v>
@@ -7310,7 +7319,7 @@
         <v>5</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C299" s="2">
         <v>11</v>
@@ -7327,7 +7336,7 @@
         <v>230</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C300" s="2">
         <v>12</v>
@@ -7344,7 +7353,7 @@
         <v>64</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C301" s="2">
         <v>3</v>
@@ -7361,7 +7370,7 @@
         <v>78</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C302" s="2">
         <v>9</v>
@@ -7378,7 +7387,7 @@
         <v>23</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C303" s="2">
         <v>9</v>
@@ -7395,7 +7404,7 @@
         <v>130</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C304" s="2">
         <v>5</v>
@@ -7412,7 +7421,7 @@
         <v>192</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C305" s="2">
         <v>10</v>
@@ -7429,7 +7438,7 @@
         <v>154</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C306" s="2">
         <v>7</v>
@@ -7446,7 +7455,7 @@
         <v>5</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C307" s="2">
         <v>12</v>
@@ -7463,7 +7472,7 @@
         <v>192</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C308" s="2">
         <v>4</v>
@@ -7480,7 +7489,7 @@
         <v>230</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C309" s="2">
         <v>16</v>
@@ -7497,7 +7506,7 @@
         <v>204</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C310" s="2">
         <v>8</v>
@@ -7514,7 +7523,7 @@
         <v>192</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C311" s="2">
         <v>3</v>
@@ -7531,7 +7540,7 @@
         <v>5</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C312" s="2">
         <v>3</v>
@@ -7548,7 +7557,7 @@
         <v>230</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C313" s="2">
         <v>8</v>
@@ -7565,7 +7574,7 @@
         <v>180</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C314" s="2">
         <v>8</v>
@@ -7582,7 +7591,7 @@
         <v>154</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C315" s="2">
         <v>14</v>
@@ -7599,7 +7608,7 @@
         <v>180</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C316" s="2">
         <v>9</v>
@@ -7616,7 +7625,7 @@
         <v>204</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C317" s="2">
         <v>9</v>
@@ -7633,7 +7642,7 @@
         <v>142</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C318" s="2">
         <v>12</v>
@@ -7650,7 +7659,7 @@
         <v>64</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C319" s="2">
         <v>5</v>
@@ -7667,7 +7676,7 @@
         <v>204</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C320" s="2">
         <v>17</v>
@@ -7684,7 +7693,7 @@
         <v>204</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C321" s="2">
         <v>10</v>
@@ -7701,7 +7710,7 @@
         <v>64</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C322" s="2">
         <v>11</v>
@@ -7718,7 +7727,7 @@
         <v>52</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C323" s="2">
         <v>8</v>
@@ -7735,7 +7744,7 @@
         <v>78</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C324" s="2">
         <v>13</v>
@@ -7752,7 +7761,7 @@
         <v>192</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C325" s="2">
         <v>7</v>
@@ -7769,7 +7778,7 @@
         <v>91</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C326" s="2">
         <v>8</v>
@@ -7786,7 +7795,7 @@
         <v>64</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C327" s="2">
         <v>8</v>
@@ -7803,7 +7812,7 @@
         <v>78</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C328" s="2">
         <v>5</v>
@@ -7820,7 +7829,7 @@
         <v>192</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C329" s="2">
         <v>4</v>
@@ -7837,7 +7846,7 @@
         <v>130</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C330" s="2">
         <v>6</v>
@@ -7854,7 +7863,7 @@
         <v>154</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C331" s="2">
         <v>5</v>
@@ -7871,7 +7880,7 @@
         <v>180</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C332" s="2">
         <v>3</v>
@@ -7888,7 +7897,7 @@
         <v>91</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C333" s="2">
         <v>4</v>
@@ -7905,7 +7914,7 @@
         <v>217</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C334" s="2">
         <v>11</v>
@@ -7922,7 +7931,7 @@
         <v>142</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C335" s="2">
         <v>8</v>
@@ -7939,7 +7948,7 @@
         <v>142</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C336" s="2">
         <v>8</v>
@@ -7956,7 +7965,7 @@
         <v>64</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C337" s="2">
         <v>8</v>
@@ -7973,7 +7982,7 @@
         <v>192</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C338" s="2">
         <v>10</v>
@@ -7990,7 +7999,7 @@
         <v>154</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C339" s="2">
         <v>7</v>
@@ -8007,7 +8016,7 @@
         <v>23</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C340" s="2">
         <v>3</v>
@@ -8024,7 +8033,7 @@
         <v>204</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C341" s="2">
         <v>12</v>
@@ -8041,7 +8050,7 @@
         <v>39</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C342" s="2">
         <v>11</v>
@@ -8058,7 +8067,7 @@
         <v>180</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C343" s="2">
         <v>4</v>
@@ -8075,7 +8084,7 @@
         <v>154</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C344" s="2">
         <v>10</v>
@@ -8092,7 +8101,7 @@
         <v>180</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C345" s="2">
         <v>8</v>
@@ -8109,7 +8118,7 @@
         <v>78</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C346" s="2">
         <v>10</v>
@@ -8126,7 +8135,7 @@
         <v>217</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C347" s="2">
         <v>5</v>
@@ -8143,7 +8152,7 @@
         <v>5</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C348" s="2">
         <v>5</v>
@@ -8160,7 +8169,7 @@
         <v>5</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C349" s="2">
         <v>13</v>
@@ -8177,7 +8186,7 @@
         <v>180</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C350" s="2">
         <v>5</v>
@@ -8194,7 +8203,7 @@
         <v>180</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C351" s="2">
         <v>5</v>
@@ -8211,7 +8220,7 @@
         <v>154</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C352" s="2">
         <v>10</v>
@@ -8228,7 +8237,7 @@
         <v>180</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C353" s="2">
         <v>8</v>
@@ -8245,7 +8254,7 @@
         <v>64</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C354" s="2">
         <v>7</v>
@@ -8262,7 +8271,7 @@
         <v>180</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C355" s="2">
         <v>10</v>
@@ -8279,7 +8288,7 @@
         <v>52</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C356" s="2">
         <v>3</v>
@@ -8296,7 +8305,7 @@
         <v>142</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C357" s="2">
         <v>6</v>
@@ -8313,7 +8322,7 @@
         <v>104</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C358" s="2">
         <v>4</v>
@@ -8330,7 +8339,7 @@
         <v>180</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C359" s="2">
         <v>3</v>
@@ -8347,7 +8356,7 @@
         <v>217</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C360" s="2">
         <v>4</v>
@@ -8364,7 +8373,7 @@
         <v>39</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C361" s="2">
         <v>4</v>
@@ -8381,7 +8390,7 @@
         <v>52</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C362" s="2">
         <v>4</v>
@@ -8398,7 +8407,7 @@
         <v>78</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C363" s="2">
         <v>8</v>
@@ -8415,7 +8424,7 @@
         <v>180</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C364" s="2">
         <v>8</v>
@@ -8432,7 +8441,7 @@
         <v>64</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C365" s="2">
         <v>2</v>
@@ -8449,7 +8458,7 @@
         <v>142</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C366" s="2">
         <v>6</v>
@@ -8466,7 +8475,7 @@
         <v>180</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C367" s="2">
         <v>8</v>
@@ -8483,7 +8492,7 @@
         <v>204</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C368" s="2">
         <v>3</v>
@@ -8500,7 +8509,7 @@
         <v>5</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C369" s="2">
         <v>3</v>
@@ -8517,7 +8526,7 @@
         <v>78</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C370" s="2">
         <v>5</v>
@@ -8534,7 +8543,7 @@
         <v>142</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C371" s="2">
         <v>2</v>
@@ -8551,7 +8560,7 @@
         <v>64</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C372" s="2">
         <v>3</v>
@@ -8568,7 +8577,7 @@
         <v>142</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C373" s="2">
         <v>3</v>
@@ -8585,7 +8594,7 @@
         <v>204</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C374" s="2">
         <v>4</v>
@@ -8602,7 +8611,7 @@
         <v>204</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C375" s="2">
         <v>3</v>
@@ -8619,7 +8628,7 @@
         <v>167</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C376" s="2">
         <v>6</v>
@@ -8636,7 +8645,7 @@
         <v>5</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C377" s="2">
         <v>5</v>
@@ -8653,7 +8662,7 @@
         <v>130</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C378" s="2">
         <v>5</v>
@@ -8670,7 +8679,7 @@
         <v>154</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C379" s="2">
         <v>5</v>
@@ -8687,7 +8696,7 @@
         <v>23</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C380" s="2">
         <v>6</v>
@@ -8704,7 +8713,7 @@
         <v>217</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C381" s="2">
         <v>4</v>
@@ -8721,7 +8730,7 @@
         <v>5</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C382" s="2">
         <v>1</v>
@@ -8738,7 +8747,7 @@
         <v>64</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C383" s="2">
         <v>7</v>
@@ -8755,7 +8764,7 @@
         <v>64</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C384" s="2">
         <v>2</v>
@@ -8772,7 +8781,7 @@
         <v>91</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C385" s="2">
         <v>1</v>
@@ -8789,7 +8798,7 @@
         <v>204</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C386" s="2">
         <v>6</v>
@@ -8806,7 +8815,7 @@
         <v>217</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C387" s="2">
         <v>7</v>
@@ -8823,7 +8832,7 @@
         <v>52</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C388" s="2">
         <v>1</v>
@@ -8840,7 +8849,7 @@
         <v>78</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C389" s="2">
         <v>2</v>
@@ -8857,7 +8866,7 @@
         <v>130</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C390" s="2">
         <v>1</v>
@@ -8874,7 +8883,7 @@
         <v>64</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C391" s="2">
         <v>4</v>
@@ -8891,7 +8900,7 @@
         <v>104</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C392" s="2">
         <v>2</v>
@@ -8908,7 +8917,7 @@
         <v>217</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C393" s="2">
         <v>5</v>
@@ -8925,7 +8934,7 @@
         <v>5</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C394" s="2">
         <v>7</v>
@@ -8942,7 +8951,7 @@
         <v>180</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C395" s="2">
         <v>2</v>
@@ -8959,7 +8968,7 @@
         <v>167</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C396" s="2">
         <v>3</v>
@@ -8976,7 +8985,7 @@
         <v>39</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C397" s="2">
         <v>1</v>
@@ -8993,7 +9002,7 @@
         <v>217</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C398" s="2">
         <v>4</v>
@@ -9010,7 +9019,7 @@
         <v>5</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C399" s="2">
         <v>1</v>
@@ -9027,7 +9036,7 @@
         <v>52</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C400" s="2">
         <v>6</v>
@@ -9044,7 +9053,7 @@
         <v>91</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C401" s="2">
         <v>1</v>
@@ -9061,7 +9070,7 @@
         <v>78</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C402" s="2">
         <v>5</v>
@@ -9078,7 +9087,7 @@
         <v>117</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C403" s="2">
         <v>3</v>
@@ -9095,7 +9104,7 @@
         <v>52</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C404" s="2">
         <v>3</v>
@@ -9112,7 +9121,7 @@
         <v>130</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C405" s="2">
         <v>1</v>
@@ -9129,7 +9138,7 @@
         <v>154</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C406" s="2">
         <v>4</v>
@@ -9146,7 +9155,7 @@
         <v>23</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C407" s="2">
         <v>2</v>
@@ -9163,7 +9172,7 @@
         <v>39</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C408" s="2">
         <v>2</v>
@@ -9180,7 +9189,7 @@
         <v>142</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C409" s="2">
         <v>3</v>
@@ -9197,7 +9206,7 @@
         <v>154</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C410" s="2">
         <v>2</v>
@@ -9214,7 +9223,7 @@
         <v>117</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C411" s="2">
         <v>1</v>
@@ -9231,7 +9240,7 @@
         <v>167</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C412" s="2">
         <v>5</v>
@@ -9248,7 +9257,7 @@
         <v>230</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C413" s="2">
         <v>1</v>
@@ -9265,7 +9274,7 @@
         <v>5</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C414" s="2">
         <v>3</v>
@@ -9282,7 +9291,7 @@
         <v>217</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C415" s="2">
         <v>5</v>
@@ -9299,7 +9308,7 @@
         <v>117</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C416" s="2">
         <v>2</v>
@@ -9316,7 +9325,7 @@
         <v>117</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C417" s="2">
         <v>2</v>
@@ -9333,7 +9342,7 @@
         <v>217</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C418" s="2">
         <v>1</v>
@@ -9350,7 +9359,7 @@
         <v>230</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C419" s="2">
         <v>13</v>
@@ -9367,7 +9376,7 @@
         <v>39</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C420" s="2">
         <v>3</v>
@@ -9384,7 +9393,7 @@
         <v>39</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C421" s="2">
         <v>4</v>
@@ -9401,7 +9410,7 @@
         <v>167</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C422" s="2">
         <v>4</v>
@@ -9418,7 +9427,7 @@
         <v>204</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C423" s="2">
         <v>1</v>
@@ -9435,7 +9444,7 @@
         <v>142</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C424" s="2">
         <v>4</v>
@@ -9452,7 +9461,7 @@
         <v>52</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C425" s="2">
         <v>3</v>
@@ -9469,7 +9478,7 @@
         <v>5</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C426" s="2">
         <v>3</v>
@@ -9486,7 +9495,7 @@
         <v>167</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C427" s="2">
         <v>5</v>
@@ -9503,7 +9512,7 @@
         <v>230</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C428" s="2">
         <v>1</v>
@@ -9520,7 +9529,7 @@
         <v>167</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C429" s="2">
         <v>1</v>
@@ -9537,7 +9546,7 @@
         <v>91</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C430" s="2">
         <v>1</v>
@@ -9554,7 +9563,7 @@
         <v>167</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C431" s="2">
         <v>5</v>
@@ -9571,7 +9580,7 @@
         <v>217</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C432" s="2">
         <v>1</v>
@@ -9588,7 +9597,7 @@
         <v>52</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C433" s="2">
         <v>1</v>
@@ -9605,7 +9614,7 @@
         <v>91</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C434" s="2">
         <v>2</v>
@@ -9622,7 +9631,7 @@
         <v>154</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C435" s="2">
         <v>3</v>
@@ -9639,7 +9648,7 @@
         <v>23</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C436" s="2">
         <v>1</v>
@@ -9656,7 +9665,7 @@
         <v>204</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C437" s="2">
         <v>1</v>
@@ -9673,7 +9682,7 @@
         <v>142</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C438" s="2">
         <v>2</v>
@@ -9690,7 +9699,7 @@
         <v>142</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C439" s="2">
         <v>2</v>
@@ -9707,7 +9716,7 @@
         <v>117</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C440" s="2">
         <v>1</v>
@@ -9724,7 +9733,7 @@
         <v>39</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C441" s="2">
         <v>1</v>
@@ -9741,7 +9750,7 @@
         <v>167</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C442" s="2">
         <v>3</v>
@@ -9758,7 +9767,7 @@
         <v>167</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C443" s="2">
         <v>3</v>
@@ -9775,7 +9784,7 @@
         <v>91</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C444" s="2">
         <v>1</v>
@@ -9792,7 +9801,7 @@
         <v>78</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C445" s="2">
         <v>1</v>
@@ -9809,7 +9818,7 @@
         <v>230</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C446" s="2">
         <v>7</v>
@@ -9826,7 +9835,7 @@
         <v>91</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C447" s="2">
         <v>5</v>
@@ -9843,7 +9852,7 @@
         <v>154</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C448" s="2">
         <v>1</v>
@@ -9860,7 +9869,7 @@
         <v>117</v>
       </c>
       <c r="B449" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C449" s="2">
         <v>2</v>
@@ -9877,7 +9886,7 @@
         <v>204</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C450" s="2">
         <v>1</v>
@@ -9894,7 +9903,7 @@
         <v>142</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C451" s="2">
         <v>1</v>
@@ -9911,7 +9920,7 @@
         <v>104</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C452" s="2">
         <v>1</v>
@@ -9928,7 +9937,7 @@
         <v>117</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C453" s="2">
         <v>2</v>
@@ -9945,7 +9954,7 @@
         <v>117</v>
       </c>
       <c r="B454" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C454" s="2">
         <v>1</v>
@@ -9962,7 +9971,7 @@
         <v>39</v>
       </c>
       <c r="B455" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C455" s="2">
         <v>1</v>
@@ -9979,7 +9988,7 @@
         <v>230</v>
       </c>
       <c r="B456" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C456" s="2">
         <v>1</v>
@@ -9996,7 +10005,7 @@
         <v>167</v>
       </c>
       <c r="B457" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C457" s="2">
         <v>1</v>
@@ -10013,7 +10022,7 @@
         <v>91</v>
       </c>
       <c r="B458" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C458" s="2">
         <v>1</v>
@@ -10030,7 +10039,7 @@
         <v>78</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C459" s="2">
         <v>3</v>
@@ -10047,7 +10056,7 @@
         <v>217</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C460" s="2">
         <v>1</v>
@@ -10064,7 +10073,7 @@
         <v>230</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C461" s="2">
         <v>2</v>
@@ -10081,7 +10090,7 @@
         <v>130</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C462" s="2">
         <v>1</v>
@@ -10098,7 +10107,7 @@
         <v>154</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>497</v>
+        <v>621</v>
       </c>
       <c r="C463" s="2">
         <v>2</v>
@@ -10115,7 +10124,7 @@
         <v>23</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C464" s="2">
         <v>1</v>
@@ -10132,7 +10141,7 @@
         <v>142</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C465" s="2">
         <v>1</v>
@@ -10149,7 +10158,7 @@
         <v>117</v>
       </c>
       <c r="B466" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C466" s="2">
         <v>1</v>
@@ -10166,7 +10175,7 @@
         <v>39</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C467" s="2">
         <v>1</v>
@@ -10183,7 +10192,7 @@
         <v>91</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C468" s="2">
         <v>3</v>
@@ -10200,7 +10209,7 @@
         <v>78</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C469" s="2">
         <v>1</v>
@@ -10217,7 +10226,7 @@
         <v>217</v>
       </c>
       <c r="B470" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C470" s="2">
         <v>1</v>
@@ -10234,7 +10243,7 @@
         <v>104</v>
       </c>
       <c r="B471" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C471" s="2">
         <v>1</v>
@@ -10251,7 +10260,7 @@
         <v>130</v>
       </c>
       <c r="B472" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C472" s="2">
         <v>1</v>
@@ -10268,7 +10277,7 @@
         <v>39</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C473" s="2">
         <v>1</v>
@@ -10285,7 +10294,7 @@
         <v>104</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C474" s="2">
         <v>1</v>
@@ -10302,7 +10311,7 @@
         <v>78</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C475" s="2">
         <v>1</v>
@@ -10319,7 +10328,7 @@
         <v>130</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C476" s="2">
         <v>1</v>
@@ -10336,7 +10345,7 @@
         <v>130</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C477" s="2">
         <v>1</v>
@@ -10353,7 +10362,7 @@
         <v>104</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C478" s="2">
         <v>1</v>
@@ -10370,7 +10379,7 @@
         <v>104</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C479" s="2">
         <v>1</v>
@@ -10387,7 +10396,7 @@
         <v>104</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C480" s="2">
         <v>1</v>
@@ -10404,7 +10413,7 @@
         <v>104</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C481" s="2">
         <v>1</v>
@@ -10421,7 +10430,7 @@
         <v>104</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C482" s="2">
         <v>1</v>
@@ -10438,7 +10447,7 @@
         <v>91</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C483" s="2">
         <v>0</v>
@@ -10455,7 +10464,7 @@
         <v>52</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C484" s="2">
         <v>0</v>
@@ -10472,7 +10481,7 @@
         <v>5</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C485" s="2">
         <v>0</v>
@@ -10489,7 +10498,7 @@
         <v>78</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C486" s="2">
         <v>0</v>
@@ -10506,7 +10515,7 @@
         <v>130</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C487" s="2">
         <v>0</v>
@@ -10523,7 +10532,7 @@
         <v>64</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C488" s="2">
         <v>0</v>
@@ -10540,7 +10549,7 @@
         <v>230</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C489" s="2">
         <v>0</v>
@@ -10557,7 +10566,7 @@
         <v>217</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C490" s="2">
         <v>0</v>
@@ -10574,7 +10583,7 @@
         <v>204</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C491" s="2">
         <v>0</v>
@@ -10591,7 +10600,7 @@
         <v>217</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C492" s="2">
         <v>0</v>
@@ -10608,7 +10617,7 @@
         <v>204</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C493" s="2">
         <v>0</v>
@@ -10625,7 +10634,7 @@
         <v>78</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C494" s="2">
         <v>0</v>
@@ -10642,7 +10651,7 @@
         <v>104</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C495" s="2">
         <v>0</v>
@@ -10659,7 +10668,7 @@
         <v>39</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C496" s="2">
         <v>0</v>
@@ -10676,7 +10685,7 @@
         <v>154</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C497" s="2">
         <v>0</v>
@@ -10693,7 +10702,7 @@
         <v>167</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C498" s="2">
         <v>0</v>
@@ -10710,7 +10719,7 @@
         <v>117</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C499" s="2">
         <v>0</v>
@@ -10727,7 +10736,7 @@
         <v>5</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C500" s="2">
         <v>0</v>
@@ -10744,7 +10753,7 @@
         <v>204</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C501" s="2">
         <v>0</v>
@@ -10761,7 +10770,7 @@
         <v>204</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C502" s="2">
         <v>0</v>
@@ -10778,7 +10787,7 @@
         <v>117</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C503" s="2">
         <v>0</v>
@@ -10795,7 +10804,7 @@
         <v>52</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C504" s="2">
         <v>0</v>
@@ -10812,7 +10821,7 @@
         <v>91</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C505" s="2">
         <v>0</v>
@@ -10829,7 +10838,7 @@
         <v>91</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C506" s="2">
         <v>0</v>
@@ -10846,7 +10855,7 @@
         <v>52</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C507" s="2">
         <v>0</v>
@@ -10863,7 +10872,7 @@
         <v>78</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C508" s="2">
         <v>0</v>
@@ -10880,7 +10889,7 @@
         <v>230</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C509" s="2">
         <v>0</v>
@@ -10897,7 +10906,7 @@
         <v>204</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C510" s="2">
         <v>0</v>
@@ -10914,7 +10923,7 @@
         <v>5</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C511" s="2">
         <v>0</v>
@@ -10931,7 +10940,7 @@
         <v>117</v>
       </c>
       <c r="B512" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C512" s="2">
         <v>0</v>
@@ -10948,7 +10957,7 @@
         <v>204</v>
       </c>
       <c r="B513" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C513" s="2">
         <v>0</v>
@@ -10965,7 +10974,7 @@
         <v>154</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C514" s="2">
         <v>0</v>
@@ -10982,7 +10991,7 @@
         <v>39</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C515" s="2">
         <v>0</v>
@@ -10999,7 +11008,7 @@
         <v>23</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C516" s="2">
         <v>0</v>
@@ -11016,7 +11025,7 @@
         <v>104</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C517" s="2">
         <v>0</v>
@@ -11033,7 +11042,7 @@
         <v>204</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C518" s="2">
         <v>0</v>
@@ -11050,7 +11059,7 @@
         <v>117</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C519" s="2">
         <v>0</v>
@@ -11067,7 +11076,7 @@
         <v>192</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C520" s="2">
         <v>0</v>
@@ -11084,7 +11093,7 @@
         <v>230</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C521" s="2">
         <v>0</v>
@@ -11101,7 +11110,7 @@
         <v>167</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C522" s="2">
         <v>0</v>
@@ -11118,7 +11127,7 @@
         <v>64</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C523" s="2">
         <v>0</v>
@@ -11135,7 +11144,7 @@
         <v>64</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C524" s="2">
         <v>0</v>
@@ -11152,7 +11161,7 @@
         <v>230</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C525" s="2">
         <v>0</v>
@@ -11169,7 +11178,7 @@
         <v>154</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C526" s="2">
         <v>0</v>
@@ -11186,7 +11195,7 @@
         <v>192</v>
       </c>
       <c r="B527" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C527" s="2">
         <v>0</v>
@@ -11203,7 +11212,7 @@
         <v>142</v>
       </c>
       <c r="B528" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C528" s="2">
         <v>0</v>
@@ -11220,7 +11229,7 @@
         <v>130</v>
       </c>
       <c r="B529" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C529" s="2">
         <v>0</v>
@@ -11237,7 +11246,7 @@
         <v>104</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C530" s="2">
         <v>0</v>
@@ -11254,7 +11263,7 @@
         <v>192</v>
       </c>
       <c r="B531" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C531" s="2">
         <v>0</v>
@@ -11271,7 +11280,7 @@
         <v>39</v>
       </c>
       <c r="B532" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C532" s="2">
         <v>0</v>
@@ -11288,7 +11297,7 @@
         <v>154</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C533" s="2">
         <v>0</v>
@@ -11305,7 +11314,7 @@
         <v>204</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C534" s="2">
         <v>0</v>
@@ -11322,7 +11331,7 @@
         <v>117</v>
       </c>
       <c r="B535" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C535" s="2">
         <v>0</v>
@@ -11339,7 +11348,7 @@
         <v>5</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C536" s="2">
         <v>0</v>
@@ -11356,7 +11365,7 @@
         <v>130</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C537" s="2">
         <v>0</v>
@@ -11373,7 +11382,7 @@
         <v>167</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C538" s="2">
         <v>0</v>
@@ -11390,7 +11399,7 @@
         <v>104</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C539" s="2">
         <v>0</v>
@@ -11407,7 +11416,7 @@
         <v>52</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C540" s="2">
         <v>0</v>
@@ -11424,7 +11433,7 @@
         <v>91</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="C541" s="2">
         <v>0</v>
@@ -11441,7 +11450,7 @@
         <v>91</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C542" s="2">
         <v>0</v>
@@ -11458,7 +11467,7 @@
         <v>52</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C543" s="2">
         <v>0</v>
@@ -11475,7 +11484,7 @@
         <v>104</v>
       </c>
       <c r="B544" s="1" t="s">
-        <v>579</v>
+        <v>622</v>
       </c>
       <c r="C544" s="2">
         <v>0</v>
@@ -11492,7 +11501,7 @@
         <v>130</v>
       </c>
       <c r="B545" s="1" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="C545" s="2">
         <v>0</v>
@@ -11509,7 +11518,7 @@
         <v>192</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="C546" s="2">
         <v>0</v>
@@ -11526,7 +11535,7 @@
         <v>5</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="C547" s="2">
         <v>0</v>
@@ -11543,7 +11552,7 @@
         <v>117</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C548" s="2">
         <v>0</v>
@@ -11560,7 +11569,7 @@
         <v>192</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="C549" s="2">
         <v>0</v>
@@ -11577,7 +11586,7 @@
         <v>154</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C550" s="2">
         <v>0</v>
@@ -11594,7 +11603,7 @@
         <v>39</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="C551" s="2">
         <v>0</v>
@@ -11611,7 +11620,7 @@
         <v>23</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="C552" s="2">
         <v>0</v>
@@ -11628,7 +11637,7 @@
         <v>142</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="C553" s="2">
         <v>0</v>
@@ -11645,7 +11654,7 @@
         <v>130</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="C554" s="2">
         <v>0</v>
@@ -11662,7 +11671,7 @@
         <v>104</v>
       </c>
       <c r="B555" s="1" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C555" s="2">
         <v>0</v>
@@ -11679,7 +11688,7 @@
         <v>192</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="C556" s="2">
         <v>0</v>
@@ -11696,7 +11705,7 @@
         <v>180</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="C557" s="2">
         <v>0</v>
@@ -11713,7 +11722,7 @@
         <v>167</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="C558" s="2">
         <v>0</v>
@@ -11730,7 +11739,7 @@
         <v>64</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C559" s="2">
         <v>0</v>
@@ -11747,7 +11756,7 @@
         <v>64</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C560" s="2">
         <v>0</v>
@@ -11764,7 +11773,7 @@
         <v>180</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C561" s="2">
         <v>0</v>
@@ -11781,7 +11790,7 @@
         <v>217</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="C562" s="2">
         <v>0</v>
@@ -11798,7 +11807,7 @@
         <v>192</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="C563" s="2">
         <v>0</v>
@@ -11815,7 +11824,7 @@
         <v>142</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="C564" s="2">
         <v>0</v>
@@ -11832,7 +11841,7 @@
         <v>130</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="C565" s="2">
         <v>0</v>
@@ -11849,7 +11858,7 @@
         <v>142</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C566" s="2">
         <v>0</v>
@@ -11866,7 +11875,7 @@
         <v>23</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C567" s="2">
         <v>0</v>
@@ -11883,7 +11892,7 @@
         <v>39</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C568" s="2">
         <v>0</v>
@@ -11900,7 +11909,7 @@
         <v>154</v>
       </c>
       <c r="B569" s="1" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C569" s="2">
         <v>0</v>
@@ -11917,7 +11926,7 @@
         <v>167</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="C570" s="2">
         <v>0</v>
@@ -11934,7 +11943,7 @@
         <v>117</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C571" s="2">
         <v>0</v>
@@ -11951,7 +11960,7 @@
         <v>5</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C572" s="2">
         <v>0</v>
@@ -11968,7 +11977,7 @@
         <v>78</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="C573" s="2">
         <v>0</v>
@@ -11985,7 +11994,7 @@
         <v>217</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="C574" s="2">
         <v>0</v>
@@ -12002,7 +12011,7 @@
         <v>104</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="C575" s="2">
         <v>0</v>
@@ -12019,7 +12028,7 @@
         <v>52</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="C576" s="2">
         <v>0</v>
@@ -12036,7 +12045,7 @@
         <v>91</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="C577" s="2">
         <v>0</v>
@@ -12053,7 +12062,7 @@
         <v>91</v>
       </c>
       <c r="B578" s="1" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="C578" s="2">
         <v>0</v>
@@ -12070,7 +12079,7 @@
         <v>52</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="C579" s="2">
         <v>0</v>
@@ -12087,7 +12096,7 @@
         <v>142</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="C580" s="2">
         <v>0</v>
@@ -12104,7 +12113,7 @@
         <v>217</v>
       </c>
       <c r="B581" s="1" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="C581" s="2">
         <v>0</v>
@@ -12121,7 +12130,7 @@
         <v>217</v>
       </c>
       <c r="B582" s="1" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C582" s="2">
         <v>0</v>
@@ -12138,7 +12147,7 @@
         <v>5</v>
       </c>
       <c r="B583" s="1" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="C583" s="2">
         <v>0</v>
@@ -12155,7 +12164,7 @@
         <v>78</v>
       </c>
       <c r="B584" s="1" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C584" s="2">
         <v>0</v>
@@ -12172,7 +12181,7 @@
         <v>167</v>
       </c>
       <c r="B585" s="1" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="C585" s="2">
         <v>0</v>
@@ -12189,7 +12198,7 @@
         <v>154</v>
       </c>
       <c r="B586" s="1" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C586" s="2">
         <v>0</v>
@@ -12206,7 +12215,7 @@
         <v>39</v>
       </c>
       <c r="B587" s="1" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="C587" s="2">
         <v>0</v>
@@ -12223,7 +12232,7 @@
         <v>23</v>
       </c>
       <c r="B588" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C588" s="2">
         <v>0</v>
@@ -12240,7 +12249,7 @@
         <v>142</v>
       </c>
       <c r="B589" s="1" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="C589" s="2">
         <v>0</v>
@@ -12257,7 +12266,7 @@
         <v>130</v>
       </c>
       <c r="B590" s="1" t="s">
-        <v>539</v>
+        <v>624</v>
       </c>
       <c r="C590" s="2">
         <v>0</v>
@@ -12274,7 +12283,7 @@
         <v>78</v>
       </c>
       <c r="B591" s="1" t="s">
-        <v>539</v>
+        <v>625</v>
       </c>
       <c r="C591" s="2">
         <v>0</v>
@@ -12291,7 +12300,7 @@
         <v>192</v>
       </c>
       <c r="B592" s="1" t="s">
-        <v>539</v>
+        <v>626</v>
       </c>
       <c r="C592" s="2">
         <v>0</v>
@@ -12308,7 +12317,7 @@
         <v>180</v>
       </c>
       <c r="B593" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C593" s="2">
         <v>0</v>
@@ -12325,7 +12334,7 @@
         <v>230</v>
       </c>
       <c r="B594" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C594" s="2">
         <v>0</v>
@@ -12342,7 +12351,7 @@
         <v>64</v>
       </c>
       <c r="B595" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C595" s="2">
         <v>0</v>
@@ -12393,7 +12402,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
@@ -12403,7 +12412,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
@@ -12423,7 +12432,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
@@ -12453,7 +12462,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>